<commit_message>
Update 23-Apr-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$63</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -102,9 +102,6 @@
     <t>1420-770-21</t>
   </si>
   <si>
-    <t>OPEN</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -115,6 +112,69 @@
   </si>
   <si>
     <t>Cost outlay: 500</t>
+  </si>
+  <si>
+    <t>1439-37154</t>
+  </si>
+  <si>
+    <t>1439-47244</t>
+  </si>
+  <si>
+    <t>1439-53964</t>
+  </si>
+  <si>
+    <t>HERO</t>
+  </si>
+  <si>
+    <t>1442-91351</t>
+  </si>
+  <si>
+    <t>1443-01972</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>1444-95611</t>
+  </si>
+  <si>
+    <t>1444-97499</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>1447-49473</t>
+  </si>
+  <si>
+    <t>1447-50168</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>1447-97608</t>
+  </si>
+  <si>
+    <t>KBYW</t>
+  </si>
+  <si>
+    <t>1450-02969</t>
+  </si>
+  <si>
+    <t>1450-21377</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>1451-08474</t>
+  </si>
+  <si>
+    <t>AMZN</t>
   </si>
 </sst>
 </file>
@@ -123,10 +183,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00;[Red]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -167,12 +227,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -469,11 +529,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,11 +543,11 @@
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -526,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" hidden="1">
       <c r="A2" s="1">
         <v>44301</v>
       </c>
@@ -558,11 +618,8 @@
         <f t="shared" ref="K2:K3" si="0">D2*I2</f>
         <v>557</v>
       </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:15" hidden="1">
       <c r="A3" s="1">
         <v>44301</v>
       </c>
@@ -594,15 +651,12 @@
         <f t="shared" si="0"/>
         <v>-462</v>
       </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
       <c r="M3" s="5">
         <f>SUM(K2:K3)</f>
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" hidden="1">
       <c r="A4" s="1">
         <v>44301</v>
       </c>
@@ -635,7 +689,7 @@
         <v>-105</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" hidden="1">
       <c r="A5" s="1">
         <v>44301</v>
       </c>
@@ -672,7 +726,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" hidden="1">
       <c r="A6" s="1">
         <v>44301</v>
       </c>
@@ -705,7 +759,7 @@
         <v>-160</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" hidden="1">
       <c r="A7" s="1">
         <v>44301</v>
       </c>
@@ -742,7 +796,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" hidden="1">
       <c r="A8" s="1">
         <v>44300</v>
       </c>
@@ -775,7 +829,7 @@
         <v>-685</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" hidden="1">
       <c r="A9" s="1">
         <v>44300</v>
       </c>
@@ -846,7 +900,7 @@
         <v>87</v>
       </c>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:15" hidden="1">
@@ -886,7 +940,7 @@
         <v>25</v>
       </c>
       <c r="O11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:15" hidden="1">
@@ -955,14 +1009,14 @@
         <v>-500</v>
       </c>
       <c r="L13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M13" s="5">
         <f>SUM(K12:K13)</f>
         <v>110</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:15" hidden="1">
@@ -1027,7 +1081,7 @@
         <v>4.28</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" ref="K15:K27" si="2">D15*I15</f>
+        <f t="shared" ref="K15:K63" si="2">D15*I15</f>
         <v>-428</v>
       </c>
       <c r="M15" s="5">
@@ -1448,18 +1502,1222 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="M30" s="5">
-        <f>SUM(M1:M29)</f>
-        <v>1262</v>
+    <row r="28" spans="1:13" hidden="1">
+      <c r="A28" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>-100</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I28" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="2"/>
+        <v>-727</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" hidden="1">
+      <c r="A29" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>-100</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="3">
+        <v>4195</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="2"/>
+        <v>-577</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" hidden="1">
+      <c r="A30" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="3">
+        <v>4155</v>
+      </c>
+      <c r="I30" s="2">
+        <v>8.42</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="2"/>
+        <v>842</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" hidden="1">
+      <c r="A31" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="3">
+        <v>4190</v>
+      </c>
+      <c r="I31" s="2">
+        <v>7.27</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" si="2"/>
+        <v>727</v>
+      </c>
+      <c r="M31" s="5">
+        <f>SUM(K28:K31)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" hidden="1">
+      <c r="A32" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>-100</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="1">
+        <v>44337</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="3">
+        <v>200</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="K32" s="4">
+        <f t="shared" si="2"/>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" hidden="1">
+      <c r="A33" s="1">
+        <v>44302</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>-100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1">
+        <v>44337</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="3">
+        <v>30</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>-100</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="3">
+        <v>4155</v>
+      </c>
+      <c r="I34" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="K34" s="4">
+        <f t="shared" si="2"/>
+        <v>-340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>-100</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="3">
+        <v>4190</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K35" s="4">
+        <f t="shared" si="2"/>
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2.42</v>
+      </c>
+      <c r="K36" s="4">
+        <f t="shared" si="2"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>100</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="1">
+        <v>44305</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4195</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="K37" s="4">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="M37" s="5">
+        <f>SUM(K34:K37)</f>
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>100</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" s="3">
+        <v>2255</v>
+      </c>
+      <c r="I38" s="2">
+        <v>31.58</v>
+      </c>
+      <c r="K38" s="4">
+        <f t="shared" si="2"/>
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>100</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="3">
+        <v>2215</v>
+      </c>
+      <c r="I39" s="2">
+        <v>44.53</v>
+      </c>
+      <c r="K39" s="4">
+        <f t="shared" si="2"/>
+        <v>4453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>-100</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="3">
+        <v>2260</v>
+      </c>
+      <c r="I40" s="2">
+        <v>29.45</v>
+      </c>
+      <c r="K40" s="4">
+        <f t="shared" si="2"/>
+        <v>-2945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>-100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="3">
+        <v>2210</v>
+      </c>
+      <c r="I41" s="2">
+        <v>42.51</v>
+      </c>
+      <c r="K41" s="4">
+        <f t="shared" si="2"/>
+        <v>-4251</v>
+      </c>
+      <c r="M41" s="5">
+        <f>SUM(K38:K41)</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>-100</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" s="3">
+        <v>4125</v>
+      </c>
+      <c r="I42" s="2">
+        <v>14.97</v>
+      </c>
+      <c r="K42" s="4">
+        <f t="shared" si="2"/>
+        <v>-1497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>-100</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="3">
+        <v>4175</v>
+      </c>
+      <c r="I43" s="2">
+        <v>12.27</v>
+      </c>
+      <c r="K43" s="4">
+        <f t="shared" si="2"/>
+        <v>-1227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="3">
+        <v>4130</v>
+      </c>
+      <c r="I44" s="2">
+        <v>16.37</v>
+      </c>
+      <c r="K44" s="4">
+        <f t="shared" si="2"/>
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>100</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I45" s="2">
+        <v>14.27</v>
+      </c>
+      <c r="K45" s="4">
+        <f t="shared" si="2"/>
+        <v>1427</v>
+      </c>
+      <c r="M45" s="5">
+        <f>SUM(K42:K45)</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>100</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
+        <v>41</v>
+      </c>
+      <c r="I46" s="2">
+        <v>63.41</v>
+      </c>
+      <c r="K46" s="4">
+        <f t="shared" si="2"/>
+        <v>6341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1">
+        <v>44306</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>-100</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="1">
+        <v>44428</v>
+      </c>
+      <c r="G47" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" s="3">
+        <v>62.5</v>
+      </c>
+      <c r="I47" s="2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="K47" s="4">
+        <f t="shared" si="2"/>
+        <v>-486.00000000000006</v>
+      </c>
+      <c r="M47" s="5">
+        <f>SUM(K46:K47)</f>
+        <v>5855</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="E48" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="3">
+        <v>61.5</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="K48" s="4">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>-100</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="1">
+        <v>44337</v>
+      </c>
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="3">
+        <v>130</v>
+      </c>
+      <c r="I49" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="K49" s="4">
+        <f t="shared" si="2"/>
+        <v>-595</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>100</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="G50" t="s">
+        <v>41</v>
+      </c>
+      <c r="I50" s="2">
+        <v>132.1</v>
+      </c>
+      <c r="K50" s="4">
+        <f t="shared" si="2"/>
+        <v>13210</v>
+      </c>
+      <c r="M50" s="5">
+        <f>SUM(K49:K50)</f>
+        <v>12615</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>-100</v>
+      </c>
+      <c r="E51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" s="2">
+        <v>22.84</v>
+      </c>
+      <c r="K51" s="4">
+        <f t="shared" si="2"/>
+        <v>-2284</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>-100</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G52" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="3">
+        <v>250</v>
+      </c>
+      <c r="I52" s="2">
+        <v>2.19</v>
+      </c>
+      <c r="K52" s="4">
+        <f t="shared" si="2"/>
+        <v>-219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>-100</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G53" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="3">
+        <v>255</v>
+      </c>
+      <c r="I53" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="K53" s="4">
+        <f t="shared" si="2"/>
+        <v>-280</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>100</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G54" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="3">
+        <v>255</v>
+      </c>
+      <c r="I54" s="2">
+        <v>3.48</v>
+      </c>
+      <c r="K54" s="4">
+        <f t="shared" si="2"/>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G55" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="3">
+        <v>250</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1.61</v>
+      </c>
+      <c r="K55" s="4">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="M55" s="5">
+        <f>SUM(K52:K55)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>-100</v>
+      </c>
+      <c r="E56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G56" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="3">
+        <v>717.5</v>
+      </c>
+      <c r="I56" s="2">
+        <v>30.05</v>
+      </c>
+      <c r="K56" s="4">
+        <f t="shared" si="2"/>
+        <v>-3005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57">
+        <v>-100</v>
+      </c>
+      <c r="E57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G57" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" s="3">
+        <v>765</v>
+      </c>
+      <c r="I57" s="2">
+        <v>32.450000000000003</v>
+      </c>
+      <c r="K57" s="4">
+        <f t="shared" si="2"/>
+        <v>-3245.0000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F58" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G58" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="3">
+        <v>720</v>
+      </c>
+      <c r="I58" s="2">
+        <v>30.85</v>
+      </c>
+      <c r="K58" s="4">
+        <f t="shared" si="2"/>
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>100</v>
+      </c>
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G59" t="s">
+        <v>23</v>
+      </c>
+      <c r="H59" s="3">
+        <v>760</v>
+      </c>
+      <c r="I59" s="2">
+        <v>34.75</v>
+      </c>
+      <c r="K59" s="4">
+        <f t="shared" si="2"/>
+        <v>3475</v>
+      </c>
+      <c r="M59" s="5">
+        <f>SUM(K56:K59)</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>-100</v>
+      </c>
+      <c r="E60" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="3">
+        <v>3290</v>
+      </c>
+      <c r="I60" s="2">
+        <v>64.8</v>
+      </c>
+      <c r="K60" s="4">
+        <f t="shared" si="2"/>
+        <v>-6480</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61">
+        <v>-100</v>
+      </c>
+      <c r="E61" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61" s="3">
+        <v>3405</v>
+      </c>
+      <c r="I61" s="2">
+        <v>50.58</v>
+      </c>
+      <c r="K61" s="4">
+        <f t="shared" si="2"/>
+        <v>-5058</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G62" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="3">
+        <v>3295</v>
+      </c>
+      <c r="I62" s="2">
+        <v>66.91</v>
+      </c>
+      <c r="K62" s="4">
+        <f t="shared" si="2"/>
+        <v>6691</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>100</v>
+      </c>
+      <c r="E63" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G63" t="s">
+        <v>23</v>
+      </c>
+      <c r="H63" s="3">
+        <v>3400</v>
+      </c>
+      <c r="I63" s="2">
+        <v>52.47</v>
+      </c>
+      <c r="K63" s="4">
+        <f t="shared" si="2"/>
+        <v>5247</v>
+      </c>
+      <c r="M63" s="5">
+        <f>SUM(K60:K63)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="66" spans="13:13">
+      <c r="M66" s="5">
+        <f>SUM(M1:M63)</f>
+        <v>21347</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K27">
-    <filterColumn colId="5">
-      <filters>
-        <dateGroupItem year="2021" month="4" day="16" dateTimeGrouping="day"/>
-      </filters>
+  <autoFilter ref="A1:M63">
+    <filterColumn colId="0">
+      <dynamicFilter type="thisWeek" val="44304" maxVal="44311"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 26-Apr-2021, night update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$72</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -175,6 +175,30 @@
   </si>
   <si>
     <t>AMZN</t>
+  </si>
+  <si>
+    <t>1452-70146</t>
+  </si>
+  <si>
+    <t>1452-79806</t>
+  </si>
+  <si>
+    <t>1452-89842</t>
+  </si>
+  <si>
+    <t>SDIV</t>
+  </si>
+  <si>
+    <t>ASSIGNMENT</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>EXERCISED</t>
   </si>
 </sst>
 </file>
@@ -529,16 +553,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M66" sqref="M66"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
@@ -547,7 +571,7 @@
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -1081,7 +1105,7 @@
         <v>4.28</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" ref="K15:K63" si="2">D15*I15</f>
+        <f t="shared" ref="K15:K75" si="2">D15*I15</f>
         <v>-428</v>
       </c>
       <c r="M15" s="5">
@@ -1704,7 +1728,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" hidden="1">
       <c r="A34" s="1">
         <v>44305</v>
       </c>
@@ -1737,7 +1761,7 @@
         <v>-340</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" s="1">
         <v>44305</v>
       </c>
@@ -1770,7 +1794,7 @@
         <v>-62</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" hidden="1">
       <c r="A36" s="1">
         <v>44305</v>
       </c>
@@ -1803,7 +1827,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" s="1">
         <v>44305</v>
       </c>
@@ -1840,7 +1864,7 @@
         <v>-125</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" s="1">
         <v>44305</v>
       </c>
@@ -1873,7 +1897,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" s="1">
         <v>44305</v>
       </c>
@@ -1906,7 +1930,7 @@
         <v>4453</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" s="1">
         <v>44305</v>
       </c>
@@ -1939,7 +1963,7 @@
         <v>-2945</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="1">
         <v>44305</v>
       </c>
@@ -2041,6 +2065,9 @@
         <f t="shared" si="2"/>
         <v>-1227</v>
       </c>
+      <c r="L43" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1">
@@ -2107,12 +2134,15 @@
         <f t="shared" si="2"/>
         <v>1427</v>
       </c>
+      <c r="L45" t="s">
+        <v>57</v>
+      </c>
       <c r="M45" s="5">
         <f>SUM(K42:K45)</f>
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" s="1">
         <v>44306</v>
       </c>
@@ -2139,7 +2169,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" s="1">
         <v>44306</v>
       </c>
@@ -2209,7 +2239,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" s="1">
         <v>44307</v>
       </c>
@@ -2242,7 +2272,7 @@
         <v>-595</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" hidden="1">
       <c r="A50" s="1">
         <v>44307</v>
       </c>
@@ -2273,7 +2303,7 @@
         <v>12615</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" s="1">
         <v>44307</v>
       </c>
@@ -2300,7 +2330,7 @@
         <v>-2284</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" s="1">
         <v>44308</v>
       </c>
@@ -2333,7 +2363,7 @@
         <v>-219</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" hidden="1">
       <c r="A53" s="1">
         <v>44308</v>
       </c>
@@ -2366,7 +2396,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" hidden="1">
       <c r="A54" s="1">
         <v>44308</v>
       </c>
@@ -2399,7 +2429,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" hidden="1">
       <c r="A55" s="1">
         <v>44308</v>
       </c>
@@ -2436,7 +2466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" hidden="1">
       <c r="A56" s="1">
         <v>44308</v>
       </c>
@@ -2469,7 +2499,7 @@
         <v>-3005</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" s="1">
         <v>44308</v>
       </c>
@@ -2502,7 +2532,7 @@
         <v>-3245.0000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" hidden="1">
       <c r="A58" s="1">
         <v>44308</v>
       </c>
@@ -2535,7 +2565,7 @@
         <v>3085</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" hidden="1">
       <c r="A59" s="1">
         <v>44308</v>
       </c>
@@ -2572,7 +2602,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" s="1">
         <v>44308</v>
       </c>
@@ -2605,7 +2635,7 @@
         <v>-6480</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="1">
         <v>44308</v>
       </c>
@@ -2638,7 +2668,7 @@
         <v>-5058</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" s="1">
         <v>44308</v>
       </c>
@@ -2671,7 +2701,7 @@
         <v>6691</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" s="1">
         <v>44308</v>
       </c>
@@ -2708,16 +2738,393 @@
         <v>400</v>
       </c>
     </row>
-    <row r="66" spans="13:13">
-      <c r="M66" s="5">
-        <f>SUM(M1:M63)</f>
-        <v>21347</v>
+    <row r="64" spans="1:13" hidden="1">
+      <c r="A64" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>100</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G64" t="s">
+        <v>23</v>
+      </c>
+      <c r="H64" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I64" s="2">
+        <v>22.83</v>
+      </c>
+      <c r="K64" s="4">
+        <f t="shared" si="2"/>
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" hidden="1">
+      <c r="A65" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>100</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G65" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I65" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="K65" s="4">
+        <f t="shared" si="2"/>
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" hidden="1">
+      <c r="A66" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>-100</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G66" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="3">
+        <v>4175</v>
+      </c>
+      <c r="I66" s="2">
+        <v>20.46</v>
+      </c>
+      <c r="K66" s="4">
+        <f t="shared" si="2"/>
+        <v>-2046</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" hidden="1">
+      <c r="A67" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>-100</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G67" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="3">
+        <v>4135</v>
+      </c>
+      <c r="I67" s="2">
+        <v>23.36</v>
+      </c>
+      <c r="K67" s="4">
+        <f t="shared" si="2"/>
+        <v>-2336</v>
+      </c>
+      <c r="M67" s="5">
+        <f>SUM(K64:K67)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" hidden="1">
+      <c r="A68" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>100</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="1">
+        <v>44312</v>
+      </c>
+      <c r="G68" t="s">
+        <v>23</v>
+      </c>
+      <c r="H68" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I68" s="2">
+        <v>6.83</v>
+      </c>
+      <c r="K68" s="4">
+        <f t="shared" si="2"/>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" hidden="1">
+      <c r="A69" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>100</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="1">
+        <v>44312</v>
+      </c>
+      <c r="G69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I69" s="2">
+        <v>8.83</v>
+      </c>
+      <c r="K69" s="4">
+        <f t="shared" si="2"/>
+        <v>883</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" hidden="1">
+      <c r="A70" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>-100</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1">
+        <v>44312</v>
+      </c>
+      <c r="G70" t="s">
+        <v>23</v>
+      </c>
+      <c r="H70" s="3">
+        <v>4175</v>
+      </c>
+      <c r="I70" s="2">
+        <v>5.25</v>
+      </c>
+      <c r="K70" s="4">
+        <f t="shared" si="2"/>
+        <v>-525</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" hidden="1">
+      <c r="A71" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>-100</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="1">
+        <v>44312</v>
+      </c>
+      <c r="G71" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="3">
+        <v>3135</v>
+      </c>
+      <c r="I71" s="2">
+        <v>7.51</v>
+      </c>
+      <c r="K71" s="4">
+        <f t="shared" si="2"/>
+        <v>-751</v>
+      </c>
+      <c r="M71" s="5">
+        <f>SUM(K68:K71)</f>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" hidden="1">
+      <c r="A72" s="1">
+        <v>44278</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>-100</v>
+      </c>
+      <c r="E72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G72" t="s">
+        <v>41</v>
+      </c>
+      <c r="I72" s="2">
+        <v>14.1</v>
+      </c>
+      <c r="K72" s="4">
+        <f t="shared" si="2"/>
+        <v>-1410</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73">
+        <v>-100</v>
+      </c>
+      <c r="E73" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" t="s">
+        <v>41</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="K73" s="4">
+        <f t="shared" si="2"/>
+        <v>-6150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74">
+        <v>-100</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" t="s">
+        <v>58</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I74" s="2">
+        <v>4170</v>
+      </c>
+      <c r="K74" s="4">
+        <f t="shared" si="2"/>
+        <v>-417000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75">
+        <v>100</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" t="s">
+        <v>58</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I75" s="2">
+        <v>4175</v>
+      </c>
+      <c r="K75" s="4">
+        <f t="shared" si="2"/>
+        <v>417500</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M63">
-    <filterColumn colId="0">
-      <dynamicFilter type="thisWeek" val="44304" maxVal="44311"/>
+  <autoFilter ref="A1:M72">
+    <filterColumn colId="0"/>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="23-Apr-2021"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 28-Apr-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$75</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -199,6 +199,39 @@
   </si>
   <si>
     <t>EXERCISED</t>
+  </si>
+  <si>
+    <t>1455-82915</t>
+  </si>
+  <si>
+    <t>1455-75007</t>
+  </si>
+  <si>
+    <t>Establish COVERED CALL</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>1455-98133</t>
+  </si>
+  <si>
+    <t>COIN</t>
+  </si>
+  <si>
+    <t>1456-78859</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>Roll out CSP for additional credits 24</t>
+  </si>
+  <si>
+    <t>Realized profit before expiry date.</t>
   </si>
 </sst>
 </file>
@@ -552,12 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -609,441 +641,437 @@
       <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" hidden="1">
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
-        <v>44301</v>
+        <v>44293</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1">
-        <v>44302</v>
+        <v>44293</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="3">
-        <v>4150</v>
+        <v>4070</v>
       </c>
       <c r="I2" s="2">
-        <v>5.57</v>
+        <v>2.38</v>
       </c>
       <c r="K2" s="4">
-        <f t="shared" ref="K2:K3" si="0">D2*I2</f>
-        <v>557</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" hidden="1">
+        <f>D2*I2</f>
+        <v>-238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
-        <v>44301</v>
+        <v>44293</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1">
-        <v>44302</v>
+        <v>44293</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="3">
-        <v>4145</v>
+        <v>4075</v>
       </c>
       <c r="I3" s="2">
-        <v>4.62</v>
+        <v>3.53</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" si="0"/>
-        <v>-462</v>
+        <f>D3*I3</f>
+        <v>353</v>
       </c>
       <c r="M3" s="5">
         <f>SUM(K2:K3)</f>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" hidden="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
-        <v>44301</v>
+        <v>44293</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1">
-        <v>44302</v>
+        <v>44293</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3">
-        <v>4130</v>
+        <v>4090</v>
       </c>
       <c r="I4" s="2">
-        <v>1.05</v>
+        <v>2.4</v>
       </c>
       <c r="K4" s="4">
         <f>D4*I4</f>
-        <v>-105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" hidden="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
-        <v>44301</v>
+        <v>44293</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1">
-        <v>44302</v>
+        <v>44293</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H5" s="3">
-        <v>4120</v>
+        <v>4095</v>
       </c>
       <c r="I5" s="2">
-        <v>0.65</v>
+        <v>1.35</v>
       </c>
       <c r="K5" s="4">
         <f>D5*I5</f>
-        <v>65</v>
+        <v>-135</v>
       </c>
       <c r="M5" s="5">
         <f>SUM(K4:K5)</f>
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" hidden="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
-        <v>44301</v>
+        <v>44295</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>-100</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="1">
-        <v>44302</v>
+        <v>44295</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3">
-        <v>4120</v>
+        <v>4110</v>
       </c>
       <c r="I6" s="2">
-        <v>1.6</v>
+        <v>3.18</v>
       </c>
       <c r="K6" s="4">
         <f>D6*I6</f>
-        <v>-160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" hidden="1">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
-        <v>44301</v>
+        <v>44295</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1">
-        <v>44302</v>
+        <v>44295</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="3">
-        <v>4125</v>
+        <v>4090</v>
       </c>
       <c r="I7" s="2">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="K7" s="4">
         <f>D7*I7</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>-200</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44295</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4115</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="K8" s="4">
+        <f>D8*I8</f>
+        <v>-350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1">
+        <v>44295</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>-200</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44295</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4085</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.93</v>
+      </c>
+      <c r="K9" s="4">
+        <f>D9*I9</f>
+        <v>-386</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="5">
+        <f>SUM(K6:K9)</f>
+        <v>420</v>
+      </c>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1">
+        <v>44298</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
         <v>200</v>
       </c>
-      <c r="M7" s="5">
-        <f>SUM(K6:K7)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" hidden="1">
-      <c r="A8" s="1">
-        <v>44300</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>-100</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44302</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3">
-        <v>4125</v>
-      </c>
-      <c r="I8" s="2">
-        <v>6.85</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" ref="K8:K14" si="1">D8*I8</f>
-        <v>-685</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" hidden="1">
-      <c r="A9" s="1">
-        <v>44300</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1">
-        <v>44302</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="3">
-        <v>4130</v>
-      </c>
-      <c r="I9" s="2">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="1"/>
-        <v>805.00000000000011</v>
-      </c>
-      <c r="M9" s="5">
-        <f>SUM(K8:K9)</f>
-        <v>120.00000000000011</v>
-      </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" hidden="1">
-      <c r="A10" s="1">
-        <v>44300</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>100</v>
-      </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="1">
-        <v>44300</v>
+        <v>44298</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H10" s="3">
-        <v>4120</v>
+        <v>4135</v>
       </c>
       <c r="I10" s="2">
-        <v>0.87</v>
+        <v>1.62</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="1"/>
-        <v>87</v>
+        <f>D10*I10</f>
+        <v>324</v>
       </c>
       <c r="O10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
-        <v>44300</v>
+        <v>44298</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>-100</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="1">
-        <v>44300</v>
+        <v>44298</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="3">
-        <v>4115</v>
+        <v>4085</v>
       </c>
       <c r="I11" s="2">
-        <v>0.62</v>
+        <v>0.66</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="1"/>
-        <v>-62</v>
-      </c>
-      <c r="M11" s="5">
-        <f>SUM(K10:K11)</f>
-        <v>25</v>
+        <f>D11*I11</f>
+        <v>132</v>
       </c>
       <c r="O11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
-        <v>44299</v>
+        <v>44298</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>-200</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="1">
-        <v>44300</v>
+        <v>44298</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H12" s="3">
-        <v>4115</v>
+        <v>4140</v>
       </c>
       <c r="I12" s="2">
-        <v>6.1</v>
+        <v>0.93</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="1"/>
-        <v>610</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1">
+        <f>D12*I12</f>
+        <v>-186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
-        <v>44299</v>
+        <v>44298</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13">
-        <v>-100</v>
+        <v>-200</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="1">
-        <v>44300</v>
+        <v>44298</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="3">
-        <v>4110</v>
+        <v>4080</v>
       </c>
       <c r="I13" s="2">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="1"/>
-        <v>-500</v>
-      </c>
-      <c r="L13" t="s">
-        <v>27</v>
+        <f>D13*I13</f>
+        <v>-100</v>
       </c>
       <c r="M13" s="5">
-        <f>SUM(K12:K13)</f>
-        <v>110</v>
+        <f>SUM(K10:K13)</f>
+        <v>170</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>44298</v>
       </c>
@@ -1072,11 +1100,11 @@
         <v>5.3</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="1"/>
+        <f>D14*I14</f>
         <v>530</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>44298</v>
       </c>
@@ -1105,7 +1133,7 @@
         <v>4.28</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" ref="K15:K75" si="2">D15*I15</f>
+        <f>D15*I15</f>
         <v>-428</v>
       </c>
       <c r="M15" s="5">
@@ -1113,420 +1141,430 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1">
+        <v>44300</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4115</v>
+      </c>
+      <c r="I16" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="K16" s="4">
+        <f>D16*I16</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1">
+        <v>44299</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>-100</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>44300</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4110</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="4">
+        <f>D17*I17</f>
+        <v>-500</v>
+      </c>
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="5">
+        <f>SUM(K16:K17)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>44300</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4120</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="K18" s="4">
+        <f>D18*I18</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>-100</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44300</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4115</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K19" s="4">
+        <f>D19*I19</f>
+        <v>-62</v>
+      </c>
+      <c r="M19" s="5">
+        <f>SUM(K18:K19)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>-100</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <v>44302</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="3">
+        <v>4125</v>
+      </c>
+      <c r="I20" s="2">
+        <v>6.85</v>
+      </c>
+      <c r="K20" s="4">
+        <f>D20*I20</f>
+        <v>-685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1">
+        <v>44300</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>44302</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4130</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="K21" s="4">
+        <f>D21*I21</f>
+        <v>805.00000000000011</v>
+      </c>
+      <c r="M21" s="5">
+        <f>SUM(K20:K21)</f>
+        <v>120.00000000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1">
+        <v>44301</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>-100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>44302</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="3">
+        <v>4120</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="K22" s="4">
+        <f>D22*I22</f>
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1">
+        <v>44301</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44302</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="3">
+        <v>4125</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="K23" s="4">
+        <f>D23*I23</f>
         <v>200</v>
       </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="1">
-        <v>44298</v>
-      </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="3">
-        <v>4135</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1.62</v>
-      </c>
-      <c r="K16" s="4">
-        <f t="shared" si="2"/>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" hidden="1">
-      <c r="A17" s="1">
-        <v>44298</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>200</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1">
-        <v>44298</v>
-      </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="3">
-        <v>4085</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="K17" s="4">
-        <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" hidden="1">
-      <c r="A18" s="1">
-        <v>44298</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <v>-200</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="1">
-        <v>44298</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="3">
-        <v>4140</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="K18" s="4">
-        <f t="shared" si="2"/>
-        <v>-186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" hidden="1">
-      <c r="A19" s="1">
-        <v>44298</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>-200</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="1">
-        <v>44298</v>
-      </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="3">
-        <v>4080</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-      <c r="M19" s="5">
-        <f>SUM(K16:K19)</f>
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" hidden="1">
-      <c r="A20" s="1">
-        <v>44295</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>200</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="1">
-        <v>44295</v>
-      </c>
-      <c r="G20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="3">
-        <v>4110</v>
-      </c>
-      <c r="I20" s="2">
-        <v>3.18</v>
-      </c>
-      <c r="K20" s="4">
-        <f t="shared" si="2"/>
-        <v>636</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" hidden="1">
-      <c r="A21" s="1">
-        <v>44295</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>200</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1">
-        <v>44295</v>
-      </c>
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="3">
-        <v>4090</v>
-      </c>
-      <c r="I21" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="K21" s="4">
-        <f t="shared" si="2"/>
-        <v>520</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" hidden="1">
-      <c r="A22" s="1">
-        <v>44295</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>-200</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="1">
-        <v>44295</v>
-      </c>
-      <c r="G22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="3">
-        <v>4115</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="K22" s="4">
-        <f t="shared" si="2"/>
-        <v>-350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" hidden="1">
-      <c r="A23" s="1">
-        <v>44295</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>-200</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="1">
-        <v>44295</v>
-      </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="3">
-        <v>4085</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1.93</v>
-      </c>
-      <c r="K23" s="4">
-        <f t="shared" si="2"/>
-        <v>-386</v>
-      </c>
-      <c r="L23" s="6"/>
       <c r="M23" s="5">
-        <f>SUM(K20:K23)</f>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" hidden="1">
+        <f>SUM(K22:K23)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1">
-        <v>44293</v>
+        <v>44301</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="1">
-        <v>44293</v>
+        <v>44302</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H24" s="3">
-        <v>4090</v>
+        <v>4130</v>
       </c>
       <c r="I24" s="2">
-        <v>2.4</v>
+        <v>1.05</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="2"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" hidden="1">
+        <f>D24*I24</f>
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
-        <v>44293</v>
+        <v>44301</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="1">
-        <v>44293</v>
+        <v>44302</v>
       </c>
       <c r="G25" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H25" s="3">
-        <v>4095</v>
+        <v>4120</v>
       </c>
       <c r="I25" s="2">
-        <v>1.35</v>
+        <v>0.65</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="2"/>
-        <v>-135</v>
+        <f>D25*I25</f>
+        <v>65</v>
       </c>
       <c r="M25" s="5">
         <f>SUM(K24:K25)</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" hidden="1">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1">
-        <v>44293</v>
+        <v>44301</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="1">
-        <v>44293</v>
+        <v>44302</v>
       </c>
       <c r="G26" t="s">
         <v>8</v>
       </c>
       <c r="H26" s="3">
-        <v>4070</v>
+        <v>4150</v>
       </c>
       <c r="I26" s="2">
-        <v>2.38</v>
+        <v>5.57</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="2"/>
-        <v>-238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" hidden="1">
+        <f>D26*I26</f>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="1">
-        <v>44293</v>
+        <v>44301</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D27">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
       </c>
       <c r="F27" s="1">
-        <v>44293</v>
+        <v>44302</v>
       </c>
       <c r="G27" t="s">
         <v>8</v>
       </c>
       <c r="H27" s="3">
-        <v>4075</v>
+        <v>4145</v>
       </c>
       <c r="I27" s="2">
-        <v>3.53</v>
+        <v>4.62</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="2"/>
-        <v>353</v>
+        <f>D27*I27</f>
+        <v>-462</v>
       </c>
       <c r="M27" s="5">
         <f>SUM(K26:K27)</f>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" hidden="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="1">
         <v>44302</v>
       </c>
@@ -1555,11 +1593,11 @@
         <v>7.27</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="2"/>
+        <f>D28*I28</f>
         <v>-727</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" s="1">
         <v>44302</v>
       </c>
@@ -1588,11 +1626,11 @@
         <v>5.77</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="2"/>
+        <f>D29*I29</f>
         <v>-577</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="1">
         <v>44302</v>
       </c>
@@ -1621,11 +1659,11 @@
         <v>8.42</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="2"/>
+        <f>D30*I30</f>
         <v>842</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="1">
         <v>44302</v>
       </c>
@@ -1654,7 +1692,7 @@
         <v>7.27</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="2"/>
+        <f>D31*I31</f>
         <v>727</v>
       </c>
       <c r="M31" s="5">
@@ -1662,7 +1700,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" s="1">
         <v>44302</v>
       </c>
@@ -1691,11 +1729,11 @@
         <v>0.36</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="2"/>
+        <f>D32*I32</f>
         <v>-36</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1">
+    <row r="33" spans="1:13">
       <c r="A33" s="1">
         <v>44302</v>
       </c>
@@ -1724,11 +1762,11 @@
         <v>0.2</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="2"/>
+        <f>D33*I33</f>
         <v>-20</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1">
+    <row r="34" spans="1:13">
       <c r="A34" s="1">
         <v>44305</v>
       </c>
@@ -1757,11 +1795,11 @@
         <v>3.4</v>
       </c>
       <c r="K34" s="4">
-        <f t="shared" si="2"/>
+        <f>D34*I34</f>
         <v>-340</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="1">
         <v>44305</v>
       </c>
@@ -1790,11 +1828,11 @@
         <v>0.62</v>
       </c>
       <c r="K35" s="4">
-        <f t="shared" si="2"/>
+        <f>D35*I35</f>
         <v>-62</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" s="1">
         <v>44305</v>
       </c>
@@ -1823,11 +1861,11 @@
         <v>2.42</v>
       </c>
       <c r="K36" s="4">
-        <f t="shared" si="2"/>
+        <f>D36*I36</f>
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" s="1">
         <v>44305</v>
       </c>
@@ -1856,7 +1894,7 @@
         <v>0.35</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="2"/>
+        <f>D37*I37</f>
         <v>35</v>
       </c>
       <c r="M37" s="5">
@@ -1864,7 +1902,7 @@
         <v>-125</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" s="1">
         <v>44305</v>
       </c>
@@ -1893,11 +1931,11 @@
         <v>31.58</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="2"/>
+        <f>D38*I38</f>
         <v>3158</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" s="1">
         <v>44305</v>
       </c>
@@ -1926,11 +1964,11 @@
         <v>44.53</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="2"/>
+        <f>D39*I39</f>
         <v>4453</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" s="1">
         <v>44305</v>
       </c>
@@ -1959,11 +1997,11 @@
         <v>29.45</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="2"/>
+        <f>D40*I40</f>
         <v>-2945</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" s="1">
         <v>44305</v>
       </c>
@@ -1992,7 +2030,7 @@
         <v>42.51</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" si="2"/>
+        <f>D41*I41</f>
         <v>-4251</v>
       </c>
       <c r="M41" s="5">
@@ -2029,7 +2067,7 @@
         <v>14.97</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="2"/>
+        <f>D42*I42</f>
         <v>-1497</v>
       </c>
     </row>
@@ -2062,7 +2100,7 @@
         <v>12.27</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" si="2"/>
+        <f>D43*I43</f>
         <v>-1227</v>
       </c>
       <c r="L43" t="s">
@@ -2098,7 +2136,7 @@
         <v>16.37</v>
       </c>
       <c r="K44" s="4">
-        <f t="shared" si="2"/>
+        <f>D44*I44</f>
         <v>1637</v>
       </c>
     </row>
@@ -2131,7 +2169,7 @@
         <v>14.27</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="2"/>
+        <f>D45*I45</f>
         <v>1427</v>
       </c>
       <c r="L45" t="s">
@@ -2142,76 +2180,66 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1">
+    <row r="46" spans="1:13">
       <c r="A46" s="1">
-        <v>44306</v>
+        <v>44309</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D46">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>41</v>
+        <v>58</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="I46" s="2">
-        <v>63.41</v>
+        <v>4170</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="2"/>
-        <v>6341</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" hidden="1">
+        <f>D46*I46</f>
+        <v>-417000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="1">
-        <v>44306</v>
+        <v>44309</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D47">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="1">
-        <v>44428</v>
+        <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="3">
-        <v>62.5</v>
+        <v>58</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="I47" s="2">
-        <v>4.8600000000000003</v>
+        <v>4175</v>
       </c>
       <c r="K47" s="4">
-        <f t="shared" si="2"/>
-        <v>-486.00000000000006</v>
-      </c>
-      <c r="M47" s="5">
-        <f>SUM(K46:K47)</f>
-        <v>5855</v>
+        <f>D47*I47</f>
+        <v>417500</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="1">
-        <v>44307</v>
+        <v>44306</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -2222,29 +2250,23 @@
       <c r="E48" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="1">
-        <v>44309</v>
-      </c>
       <c r="G48" t="s">
-        <v>8</v>
-      </c>
-      <c r="H48" s="3">
-        <v>61.5</v>
+        <v>41</v>
       </c>
       <c r="I48" s="2">
-        <v>1.05</v>
+        <v>63.41</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" si="2"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" hidden="1">
+        <f>D48*I48</f>
+        <v>6341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="1">
-        <v>44307</v>
+        <v>44306</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
         <v>10</v>
@@ -2253,31 +2275,35 @@
         <v>-100</v>
       </c>
       <c r="E49" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F49" s="1">
-        <v>44337</v>
+        <v>44428</v>
       </c>
       <c r="G49" t="s">
         <v>23</v>
       </c>
       <c r="H49" s="3">
-        <v>130</v>
+        <v>62.5</v>
       </c>
       <c r="I49" s="2">
-        <v>5.95</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="K49" s="4">
-        <f t="shared" si="2"/>
-        <v>-595</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" hidden="1">
+        <f>D49*I49</f>
+        <v>-486.00000000000006</v>
+      </c>
+      <c r="M49" s="5">
+        <f>SUM(K48:K49)</f>
+        <v>5855</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="1">
         <v>44307</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -2286,150 +2312,144 @@
         <v>100</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="F50" s="1">
+        <v>44309</v>
       </c>
       <c r="G50" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+      <c r="H50" s="3">
+        <v>61.5</v>
       </c>
       <c r="I50" s="2">
-        <v>132.1</v>
+        <v>1.05</v>
       </c>
       <c r="K50" s="4">
-        <f t="shared" si="2"/>
-        <v>13210</v>
-      </c>
-      <c r="M50" s="5">
-        <f>SUM(K49:K50)</f>
-        <v>12615</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" hidden="1">
+        <f>D50*I50</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="1">
-        <v>44307</v>
+        <v>44309</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D51">
         <v>-100</v>
       </c>
       <c r="E51" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G51" t="s">
         <v>41</v>
       </c>
+      <c r="H51" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="I51" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="K51" s="4">
+        <f>D51*I51</f>
+        <v>-6150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>-100</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="1">
+        <v>44337</v>
+      </c>
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="3">
+        <v>130</v>
+      </c>
+      <c r="I52" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="K52" s="4">
+        <f>D52*I52</f>
+        <v>-595</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>100</v>
+      </c>
+      <c r="E53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" s="2">
+        <v>132.1</v>
+      </c>
+      <c r="K53" s="4">
+        <f>D53*I53</f>
+        <v>13210</v>
+      </c>
+      <c r="M53" s="5">
+        <f>SUM(K52:K53)</f>
+        <v>12615</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>-100</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="I54" s="2">
         <v>22.84</v>
       </c>
-      <c r="K51" s="4">
-        <f t="shared" si="2"/>
+      <c r="K54" s="4">
+        <f>D54*I54</f>
         <v>-2284</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
-      <c r="A52" s="1">
-        <v>44308</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52">
-        <v>-100</v>
-      </c>
-      <c r="E52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G52" t="s">
-        <v>8</v>
-      </c>
-      <c r="H52" s="3">
-        <v>250</v>
-      </c>
-      <c r="I52" s="2">
-        <v>2.19</v>
-      </c>
-      <c r="K52" s="4">
-        <f t="shared" si="2"/>
-        <v>-219</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" hidden="1">
-      <c r="A53" s="1">
-        <v>44308</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53">
-        <v>-100</v>
-      </c>
-      <c r="E53" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="1">
-        <v>44316</v>
-      </c>
-      <c r="G53" t="s">
-        <v>8</v>
-      </c>
-      <c r="H53" s="3">
-        <v>255</v>
-      </c>
-      <c r="I53" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="K53" s="4">
-        <f t="shared" si="2"/>
-        <v>-280</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" hidden="1">
-      <c r="A54" s="1">
-        <v>44308</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54">
-        <v>100</v>
-      </c>
-      <c r="E54" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G54" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="3">
-        <v>255</v>
-      </c>
-      <c r="I54" s="2">
-        <v>3.48</v>
-      </c>
-      <c r="K54" s="4">
-        <f t="shared" si="2"/>
-        <v>348</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="1">
         <v>44308</v>
       </c>
@@ -2437,16 +2457,16 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D55">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" s="1">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="G55" t="s">
         <v>8</v>
@@ -2455,23 +2475,19 @@
         <v>250</v>
       </c>
       <c r="I55" s="2">
-        <v>1.61</v>
+        <v>2.19</v>
       </c>
       <c r="K55" s="4">
-        <f t="shared" si="2"/>
-        <v>161</v>
-      </c>
-      <c r="M55" s="5">
-        <f>SUM(K52:K55)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" hidden="1">
+        <f>D55*I55</f>
+        <v>-219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="1">
         <v>44308</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
@@ -2480,64 +2496,64 @@
         <v>-100</v>
       </c>
       <c r="E56" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F56" s="1">
-        <v>44323</v>
+        <v>44316</v>
       </c>
       <c r="G56" t="s">
         <v>8</v>
       </c>
       <c r="H56" s="3">
-        <v>717.5</v>
+        <v>255</v>
       </c>
       <c r="I56" s="2">
-        <v>30.05</v>
+        <v>2.8</v>
       </c>
       <c r="K56" s="4">
-        <f t="shared" si="2"/>
-        <v>-3005</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" hidden="1">
+        <f>D56*I56</f>
+        <v>-280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="1">
         <v>44308</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D57">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E57" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F57" s="1">
         <v>44323</v>
       </c>
       <c r="G57" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H57" s="3">
-        <v>765</v>
+        <v>255</v>
       </c>
       <c r="I57" s="2">
-        <v>32.450000000000003</v>
+        <v>3.48</v>
       </c>
       <c r="K57" s="4">
-        <f t="shared" si="2"/>
-        <v>-3245.0000000000005</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" hidden="1">
+        <f>D57*I57</f>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="1">
         <v>44308</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
@@ -2546,26 +2562,30 @@
         <v>100</v>
       </c>
       <c r="E58" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F58" s="1">
-        <v>44323</v>
+        <v>44316</v>
       </c>
       <c r="G58" t="s">
         <v>8</v>
       </c>
       <c r="H58" s="3">
-        <v>720</v>
+        <v>250</v>
       </c>
       <c r="I58" s="2">
-        <v>30.85</v>
+        <v>1.61</v>
       </c>
       <c r="K58" s="4">
-        <f t="shared" si="2"/>
-        <v>3085</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" hidden="1">
+        <f>D58*I58</f>
+        <v>161</v>
+      </c>
+      <c r="M58" s="5">
+        <f>SUM(K55:K58)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="1">
         <v>44308</v>
       </c>
@@ -2573,10 +2593,10 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D59">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E59" t="s">
         <v>49</v>
@@ -2585,29 +2605,25 @@
         <v>44323</v>
       </c>
       <c r="G59" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H59" s="3">
-        <v>760</v>
+        <v>717.5</v>
       </c>
       <c r="I59" s="2">
-        <v>34.75</v>
+        <v>30.05</v>
       </c>
       <c r="K59" s="4">
-        <f t="shared" si="2"/>
-        <v>3475</v>
-      </c>
-      <c r="M59" s="5">
-        <f>SUM(K56:K59)</f>
-        <v>310</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" hidden="1">
+        <f>D59*I59</f>
+        <v>-3005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="1">
         <v>44308</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
         <v>10</v>
@@ -2616,64 +2632,64 @@
         <v>-100</v>
       </c>
       <c r="E60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F60" s="1">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="G60" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H60" s="3">
-        <v>3290</v>
+        <v>765</v>
       </c>
       <c r="I60" s="2">
-        <v>64.8</v>
+        <v>32.450000000000003</v>
       </c>
       <c r="K60" s="4">
-        <f t="shared" si="2"/>
-        <v>-6480</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" hidden="1">
+        <f>D60*I60</f>
+        <v>-3245.0000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="1">
         <v>44308</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D61">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F61" s="1">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="G61" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H61" s="3">
-        <v>3405</v>
+        <v>720</v>
       </c>
       <c r="I61" s="2">
-        <v>50.58</v>
+        <v>30.85</v>
       </c>
       <c r="K61" s="4">
-        <f t="shared" si="2"/>
-        <v>-5058</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" hidden="1">
+        <f>D61*I61</f>
+        <v>3085</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="1">
         <v>44308</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
@@ -2682,26 +2698,30 @@
         <v>100</v>
       </c>
       <c r="E62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F62" s="1">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="G62" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H62" s="3">
-        <v>3295</v>
+        <v>760</v>
       </c>
       <c r="I62" s="2">
-        <v>66.91</v>
+        <v>34.75</v>
       </c>
       <c r="K62" s="4">
-        <f t="shared" si="2"/>
-        <v>6691</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" hidden="1">
+        <f>D62*I62</f>
+        <v>3475</v>
+      </c>
+      <c r="M62" s="5">
+        <f>SUM(K59:K62)</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="1">
         <v>44308</v>
       </c>
@@ -2709,10 +2729,10 @@
         <v>50</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D63">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E63" t="s">
         <v>51</v>
@@ -2721,38 +2741,34 @@
         <v>44316</v>
       </c>
       <c r="G63" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>3400</v>
+        <v>3290</v>
       </c>
       <c r="I63" s="2">
-        <v>52.47</v>
+        <v>64.8</v>
       </c>
       <c r="K63" s="4">
-        <f t="shared" si="2"/>
-        <v>5247</v>
-      </c>
-      <c r="M63" s="5">
-        <f>SUM(K60:K63)</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" hidden="1">
+        <f>D63*I63</f>
+        <v>-6480</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="1">
-        <v>44309</v>
+        <v>44308</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D64">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E64" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F64" s="1">
         <v>44316</v>
@@ -2761,22 +2777,22 @@
         <v>23</v>
       </c>
       <c r="H64" s="3">
-        <v>4170</v>
+        <v>3405</v>
       </c>
       <c r="I64" s="2">
-        <v>22.83</v>
+        <v>50.58</v>
       </c>
       <c r="K64" s="4">
-        <f t="shared" si="2"/>
-        <v>2283</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" hidden="1">
+        <f>D64*I64</f>
+        <v>-5058</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" s="1">
-        <v>44309</v>
+        <v>44308</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C65" t="s">
         <v>4</v>
@@ -2785,7 +2801,7 @@
         <v>100</v>
       </c>
       <c r="E65" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F65" s="1">
         <v>44316</v>
@@ -2794,31 +2810,31 @@
         <v>8</v>
       </c>
       <c r="H65" s="3">
-        <v>4140</v>
+        <v>3295</v>
       </c>
       <c r="I65" s="2">
-        <v>24.99</v>
+        <v>66.91</v>
       </c>
       <c r="K65" s="4">
-        <f t="shared" si="2"/>
-        <v>2499</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" hidden="1">
+        <f>D65*I65</f>
+        <v>6691</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="1">
-        <v>44309</v>
+        <v>44308</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D66">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E66" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="F66" s="1">
         <v>44316</v>
@@ -2827,17 +2843,21 @@
         <v>23</v>
       </c>
       <c r="H66" s="3">
-        <v>4175</v>
+        <v>3400</v>
       </c>
       <c r="I66" s="2">
-        <v>20.46</v>
+        <v>52.47</v>
       </c>
       <c r="K66" s="4">
-        <f t="shared" si="2"/>
-        <v>-2046</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" hidden="1">
+        <f>D66*I66</f>
+        <v>5247</v>
+      </c>
+      <c r="M66" s="5">
+        <f>SUM(K63:K66)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" s="1">
         <v>44309</v>
       </c>
@@ -2845,10 +2865,10 @@
         <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D67">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E67" t="s">
         <v>6</v>
@@ -2857,29 +2877,25 @@
         <v>44316</v>
       </c>
       <c r="G67" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H67" s="3">
-        <v>4135</v>
+        <v>4170</v>
       </c>
       <c r="I67" s="2">
-        <v>23.36</v>
+        <v>22.83</v>
       </c>
       <c r="K67" s="4">
-        <f t="shared" si="2"/>
-        <v>-2336</v>
-      </c>
-      <c r="M67" s="5">
-        <f>SUM(K64:K67)</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" hidden="1">
+        <f>D67*I67</f>
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" s="1">
         <v>44309</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
@@ -2891,61 +2907,61 @@
         <v>6</v>
       </c>
       <c r="F68" s="1">
-        <v>44312</v>
+        <v>44316</v>
       </c>
       <c r="G68" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H68" s="3">
-        <v>4170</v>
+        <v>4140</v>
       </c>
       <c r="I68" s="2">
-        <v>6.83</v>
+        <v>24.99</v>
       </c>
       <c r="K68" s="4">
-        <f t="shared" si="2"/>
-        <v>683</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" hidden="1">
+        <f>D68*I68</f>
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="1">
         <v>44309</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D69">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E69" t="s">
         <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>44312</v>
+        <v>44316</v>
       </c>
       <c r="G69" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H69" s="3">
-        <v>4140</v>
+        <v>4175</v>
       </c>
       <c r="I69" s="2">
-        <v>8.83</v>
+        <v>20.46</v>
       </c>
       <c r="K69" s="4">
-        <f t="shared" si="2"/>
-        <v>883</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" hidden="1">
+        <f>D69*I69</f>
+        <v>-2046</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" s="1">
         <v>44309</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
         <v>10</v>
@@ -2957,23 +2973,27 @@
         <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>44312</v>
+        <v>44316</v>
       </c>
       <c r="G70" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H70" s="3">
-        <v>4175</v>
+        <v>4135</v>
       </c>
       <c r="I70" s="2">
-        <v>5.25</v>
+        <v>23.36</v>
       </c>
       <c r="K70" s="4">
-        <f t="shared" si="2"/>
-        <v>-525</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" hidden="1">
+        <f>D70*I70</f>
+        <v>-2336</v>
+      </c>
+      <c r="M70" s="5">
+        <f>SUM(K67:K70)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" s="1">
         <v>44309</v>
       </c>
@@ -2981,10 +3001,10 @@
         <v>53</v>
       </c>
       <c r="C71" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D71">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E71" t="s">
         <v>6</v>
@@ -2993,48 +3013,50 @@
         <v>44312</v>
       </c>
       <c r="G71" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H71" s="3">
-        <v>3135</v>
+        <v>4170</v>
       </c>
       <c r="I71" s="2">
-        <v>7.51</v>
+        <v>6.83</v>
       </c>
       <c r="K71" s="4">
-        <f t="shared" si="2"/>
-        <v>-751</v>
-      </c>
-      <c r="M71" s="5">
-        <f>SUM(K68:K71)</f>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" hidden="1">
+        <f>D71*I71</f>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="1">
-        <v>44278</v>
+        <v>44309</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D72">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E72" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="F72" s="1">
+        <v>44312</v>
       </c>
       <c r="G72" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+      <c r="H72" s="3">
+        <v>4140</v>
       </c>
       <c r="I72" s="2">
-        <v>14.1</v>
+        <v>8.83</v>
       </c>
       <c r="K72" s="4">
-        <f t="shared" si="2"/>
-        <v>-1410</v>
+        <f>D72*I72</f>
+        <v>883</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -3042,26 +3064,32 @@
         <v>44309</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
       </c>
       <c r="D73">
         <v>-100</v>
       </c>
       <c r="E73" t="s">
-        <v>40</v>
+        <v>6</v>
+      </c>
+      <c r="F73" s="1">
+        <v>44312</v>
       </c>
       <c r="G73" t="s">
-        <v>41</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>56</v>
+        <v>23</v>
+      </c>
+      <c r="H73" s="3">
+        <v>4175</v>
       </c>
       <c r="I73" s="2">
-        <v>61.5</v>
+        <v>5.25</v>
       </c>
       <c r="K73" s="4">
-        <f t="shared" si="2"/>
-        <v>-6150</v>
+        <f>D73*I73</f>
+        <v>-525</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -3069,7 +3097,10 @@
         <v>44309</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="C74" t="s">
+        <v>10</v>
       </c>
       <c r="D74">
         <v>-100</v>
@@ -3077,18 +3108,25 @@
       <c r="E74" t="s">
         <v>6</v>
       </c>
+      <c r="F74" s="1">
+        <v>44312</v>
+      </c>
       <c r="G74" t="s">
-        <v>58</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>56</v>
+        <v>8</v>
+      </c>
+      <c r="H74" s="3">
+        <v>3135</v>
       </c>
       <c r="I74" s="2">
-        <v>4170</v>
+        <v>7.51</v>
       </c>
       <c r="K74" s="4">
-        <f t="shared" si="2"/>
-        <v>-417000</v>
+        <f>D74*I74</f>
+        <v>-751</v>
+      </c>
+      <c r="M74" s="5">
+        <f>SUM(K71:K74)</f>
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -3096,36 +3134,415 @@
         <v>44309</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
       </c>
       <c r="D75">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E75" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="G75" t="s">
-        <v>58</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="I75" s="2">
+        <v>14.1</v>
+      </c>
+      <c r="K75" s="4">
+        <f>D75*I75</f>
+        <v>-1410</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>-100</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G76" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I76" s="2">
+        <v>17.52</v>
+      </c>
+      <c r="K76" s="4">
+        <f>D76*I76</f>
+        <v>-1752</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>-100</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G77" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" s="3">
+        <v>4205</v>
+      </c>
+      <c r="I77" s="2">
+        <v>16.420000000000002</v>
+      </c>
+      <c r="K77" s="4">
+        <f>D77*I77</f>
+        <v>-1642.0000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G78" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="3">
         <v>4175</v>
       </c>
-      <c r="K75" s="4">
-        <f t="shared" si="2"/>
-        <v>417500</v>
+      <c r="I78" s="2">
+        <v>19.07</v>
+      </c>
+      <c r="K78" s="4">
+        <f>D78*I78</f>
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <v>100</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G79" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I79" s="2">
+        <v>18.77</v>
+      </c>
+      <c r="K79" s="4">
+        <f>D79*I79</f>
+        <v>1877</v>
+      </c>
+      <c r="M79" s="5">
+        <f>SUM(K76:K79)</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>100</v>
+      </c>
+      <c r="E80" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="1">
+        <v>44351</v>
+      </c>
+      <c r="G80" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" s="3">
+        <v>61.5</v>
+      </c>
+      <c r="I80" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="K80" s="4">
+        <f>D80*I80</f>
+        <v>83</v>
+      </c>
+      <c r="M80" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
+      <c r="A81" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>-100</v>
+      </c>
+      <c r="E81" t="s">
+        <v>66</v>
+      </c>
+      <c r="F81" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G81" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="3">
+        <v>295</v>
+      </c>
+      <c r="I81" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="K81" s="4">
+        <f>D81*I81</f>
+        <v>-699</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <v>-100</v>
+      </c>
+      <c r="E82" t="s">
+        <v>66</v>
+      </c>
+      <c r="F82" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G82" t="s">
+        <v>23</v>
+      </c>
+      <c r="H82" s="3">
+        <v>305</v>
+      </c>
+      <c r="I82" s="2">
+        <v>8.35</v>
+      </c>
+      <c r="K82" s="4">
+        <f>D82*I82</f>
+        <v>-835</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>100</v>
+      </c>
+      <c r="E83" t="s">
+        <v>66</v>
+      </c>
+      <c r="F83" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G83" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="3">
+        <v>297.5</v>
+      </c>
+      <c r="I83" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="K83" s="4">
+        <f>D83*I83</f>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>100</v>
+      </c>
+      <c r="E84" t="s">
+        <v>66</v>
+      </c>
+      <c r="F84" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G84" t="s">
+        <v>23</v>
+      </c>
+      <c r="H84" s="3">
+        <v>302.5</v>
+      </c>
+      <c r="I84" s="2">
+        <v>9.34</v>
+      </c>
+      <c r="K84" s="4">
+        <f>D84*I84</f>
+        <v>934</v>
+      </c>
+      <c r="M84" s="5">
+        <f>SUM(K81:K84)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
+      <c r="A85" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>100</v>
+      </c>
+      <c r="E85" t="s">
+        <v>68</v>
+      </c>
+      <c r="F85" s="1">
+        <v>44365</v>
+      </c>
+      <c r="G85" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="3">
+        <v>25</v>
+      </c>
+      <c r="I85" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="K85" s="4">
+        <f>D85*I85</f>
+        <v>325</v>
+      </c>
+      <c r="M85" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
+      <c r="A86" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <v>-100</v>
+      </c>
+      <c r="E86" t="s">
+        <v>68</v>
+      </c>
+      <c r="F86" s="1">
+        <v>44337</v>
+      </c>
+      <c r="G86" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" s="3">
+        <v>25</v>
+      </c>
+      <c r="I86" s="2">
+        <v>3.01</v>
+      </c>
+      <c r="K86" s="4">
+        <f>D86*I86</f>
+        <v>-301</v>
+      </c>
+      <c r="M86" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M72">
+  <autoFilter ref="A1:M75">
     <filterColumn colId="0"/>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="23-Apr-2021"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="5"/>
+    <sortState ref="A2:M75">
+      <sortCondition ref="B1"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update 1 Mei 2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$117</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -232,6 +232,39 @@
   </si>
   <si>
     <t>Realized profit before expiry date.</t>
+  </si>
+  <si>
+    <t>1457-95493</t>
+  </si>
+  <si>
+    <t>1458-26012</t>
+  </si>
+  <si>
+    <t>1458-48871</t>
+  </si>
+  <si>
+    <t>1458-52093</t>
+  </si>
+  <si>
+    <t>1458-65686</t>
+  </si>
+  <si>
+    <t>1460-71088</t>
+  </si>
+  <si>
+    <t>GNL</t>
+  </si>
+  <si>
+    <t>1461-13461</t>
+  </si>
+  <si>
+    <t>1461-18716</t>
+  </si>
+  <si>
+    <t>1461-23681</t>
+  </si>
+  <si>
+    <t>1461-42206</t>
   </si>
 </sst>
 </file>
@@ -585,11 +618,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O86"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M120" sqref="M120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,13 +632,15 @@
     <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="5"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -648,7 +684,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" hidden="1">
       <c r="A2" s="1">
         <v>44293</v>
       </c>
@@ -677,11 +713,11 @@
         <v>2.38</v>
       </c>
       <c r="K2" s="4">
-        <f>D2*I2</f>
+        <f t="shared" ref="K2:K33" si="0">D2*I2</f>
         <v>-238</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" hidden="1">
       <c r="A3" s="1">
         <v>44293</v>
       </c>
@@ -710,7 +746,7 @@
         <v>3.53</v>
       </c>
       <c r="K3" s="4">
-        <f>D3*I3</f>
+        <f t="shared" si="0"/>
         <v>353</v>
       </c>
       <c r="M3" s="5">
@@ -718,7 +754,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" hidden="1">
       <c r="A4" s="1">
         <v>44293</v>
       </c>
@@ -747,11 +783,11 @@
         <v>2.4</v>
       </c>
       <c r="K4" s="4">
-        <f>D4*I4</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" hidden="1">
       <c r="A5" s="1">
         <v>44293</v>
       </c>
@@ -780,7 +816,7 @@
         <v>1.35</v>
       </c>
       <c r="K5" s="4">
-        <f>D5*I5</f>
+        <f t="shared" si="0"/>
         <v>-135</v>
       </c>
       <c r="M5" s="5">
@@ -788,7 +824,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" hidden="1">
       <c r="A6" s="1">
         <v>44295</v>
       </c>
@@ -817,11 +853,11 @@
         <v>3.18</v>
       </c>
       <c r="K6" s="4">
-        <f>D6*I6</f>
+        <f t="shared" si="0"/>
         <v>636</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" hidden="1">
       <c r="A7" s="1">
         <v>44295</v>
       </c>
@@ -850,11 +886,11 @@
         <v>2.6</v>
       </c>
       <c r="K7" s="4">
-        <f>D7*I7</f>
+        <f t="shared" si="0"/>
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" hidden="1">
       <c r="A8" s="1">
         <v>44295</v>
       </c>
@@ -883,11 +919,11 @@
         <v>1.75</v>
       </c>
       <c r="K8" s="4">
-        <f>D8*I8</f>
+        <f t="shared" si="0"/>
         <v>-350</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" hidden="1">
       <c r="A9" s="1">
         <v>44295</v>
       </c>
@@ -916,7 +952,7 @@
         <v>1.93</v>
       </c>
       <c r="K9" s="4">
-        <f>D9*I9</f>
+        <f t="shared" si="0"/>
         <v>-386</v>
       </c>
       <c r="L9" s="6"/>
@@ -926,7 +962,7 @@
       </c>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" hidden="1">
       <c r="A10" s="1">
         <v>44298</v>
       </c>
@@ -955,14 +991,14 @@
         <v>1.62</v>
       </c>
       <c r="K10" s="4">
-        <f>D10*I10</f>
+        <f t="shared" si="0"/>
         <v>324</v>
       </c>
       <c r="O10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" hidden="1">
       <c r="A11" s="1">
         <v>44298</v>
       </c>
@@ -991,14 +1027,14 @@
         <v>0.66</v>
       </c>
       <c r="K11" s="4">
-        <f>D11*I11</f>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="O11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" hidden="1">
       <c r="A12" s="1">
         <v>44298</v>
       </c>
@@ -1027,11 +1063,11 @@
         <v>0.93</v>
       </c>
       <c r="K12" s="4">
-        <f>D12*I12</f>
+        <f t="shared" si="0"/>
         <v>-186</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" hidden="1">
       <c r="A13" s="1">
         <v>44298</v>
       </c>
@@ -1060,7 +1096,7 @@
         <v>0.5</v>
       </c>
       <c r="K13" s="4">
-        <f>D13*I13</f>
+        <f t="shared" si="0"/>
         <v>-100</v>
       </c>
       <c r="M13" s="5">
@@ -1071,7 +1107,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" hidden="1">
       <c r="A14" s="1">
         <v>44298</v>
       </c>
@@ -1100,11 +1136,11 @@
         <v>5.3</v>
       </c>
       <c r="K14" s="4">
-        <f>D14*I14</f>
+        <f t="shared" si="0"/>
         <v>530</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" hidden="1">
       <c r="A15" s="1">
         <v>44298</v>
       </c>
@@ -1133,7 +1169,7 @@
         <v>4.28</v>
       </c>
       <c r="K15" s="4">
-        <f>D15*I15</f>
+        <f t="shared" si="0"/>
         <v>-428</v>
       </c>
       <c r="M15" s="5">
@@ -1141,7 +1177,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" hidden="1">
       <c r="A16" s="1">
         <v>44299</v>
       </c>
@@ -1170,11 +1206,11 @@
         <v>6.1</v>
       </c>
       <c r="K16" s="4">
-        <f>D16*I16</f>
+        <f t="shared" si="0"/>
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" hidden="1">
       <c r="A17" s="1">
         <v>44299</v>
       </c>
@@ -1203,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="4">
-        <f>D17*I17</f>
+        <f t="shared" si="0"/>
         <v>-500</v>
       </c>
       <c r="L17" t="s">
@@ -1214,7 +1250,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" s="1">
         <v>44300</v>
       </c>
@@ -1243,11 +1279,11 @@
         <v>0.87</v>
       </c>
       <c r="K18" s="4">
-        <f>D18*I18</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" s="1">
         <v>44300</v>
       </c>
@@ -1276,7 +1312,7 @@
         <v>0.62</v>
       </c>
       <c r="K19" s="4">
-        <f>D19*I19</f>
+        <f t="shared" si="0"/>
         <v>-62</v>
       </c>
       <c r="M19" s="5">
@@ -1284,7 +1320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" s="1">
         <v>44300</v>
       </c>
@@ -1313,11 +1349,11 @@
         <v>6.85</v>
       </c>
       <c r="K20" s="4">
-        <f>D20*I20</f>
+        <f t="shared" si="0"/>
         <v>-685</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" hidden="1">
       <c r="A21" s="1">
         <v>44300</v>
       </c>
@@ -1346,7 +1382,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="K21" s="4">
-        <f>D21*I21</f>
+        <f t="shared" si="0"/>
         <v>805.00000000000011</v>
       </c>
       <c r="M21" s="5">
@@ -1354,7 +1390,7 @@
         <v>120.00000000000011</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" hidden="1">
       <c r="A22" s="1">
         <v>44301</v>
       </c>
@@ -1383,11 +1419,11 @@
         <v>1.6</v>
       </c>
       <c r="K22" s="4">
-        <f>D22*I22</f>
+        <f t="shared" si="0"/>
         <v>-160</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" hidden="1">
       <c r="A23" s="1">
         <v>44301</v>
       </c>
@@ -1416,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="4">
-        <f>D23*I23</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="M23" s="5">
@@ -1424,7 +1460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" s="1">
         <v>44301</v>
       </c>
@@ -1453,11 +1489,11 @@
         <v>1.05</v>
       </c>
       <c r="K24" s="4">
-        <f>D24*I24</f>
+        <f t="shared" si="0"/>
         <v>-105</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" s="1">
         <v>44301</v>
       </c>
@@ -1486,7 +1522,7 @@
         <v>0.65</v>
       </c>
       <c r="K25" s="4">
-        <f>D25*I25</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="M25" s="5">
@@ -1494,7 +1530,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" s="1">
         <v>44301</v>
       </c>
@@ -1523,11 +1559,11 @@
         <v>5.57</v>
       </c>
       <c r="K26" s="4">
-        <f>D26*I26</f>
+        <f t="shared" si="0"/>
         <v>557</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" hidden="1">
       <c r="A27" s="1">
         <v>44301</v>
       </c>
@@ -1556,7 +1592,7 @@
         <v>4.62</v>
       </c>
       <c r="K27" s="4">
-        <f>D27*I27</f>
+        <f t="shared" si="0"/>
         <v>-462</v>
       </c>
       <c r="M27" s="5">
@@ -1564,7 +1600,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" hidden="1">
       <c r="A28" s="1">
         <v>44302</v>
       </c>
@@ -1593,11 +1629,11 @@
         <v>7.27</v>
       </c>
       <c r="K28" s="4">
-        <f>D28*I28</f>
+        <f t="shared" si="0"/>
         <v>-727</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" hidden="1">
       <c r="A29" s="1">
         <v>44302</v>
       </c>
@@ -1626,11 +1662,11 @@
         <v>5.77</v>
       </c>
       <c r="K29" s="4">
-        <f>D29*I29</f>
+        <f t="shared" si="0"/>
         <v>-577</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" hidden="1">
       <c r="A30" s="1">
         <v>44302</v>
       </c>
@@ -1659,11 +1695,11 @@
         <v>8.42</v>
       </c>
       <c r="K30" s="4">
-        <f>D30*I30</f>
+        <f t="shared" si="0"/>
         <v>842</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" hidden="1">
       <c r="A31" s="1">
         <v>44302</v>
       </c>
@@ -1692,7 +1728,7 @@
         <v>7.27</v>
       </c>
       <c r="K31" s="4">
-        <f>D31*I31</f>
+        <f t="shared" si="0"/>
         <v>727</v>
       </c>
       <c r="M31" s="5">
@@ -1700,7 +1736,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" hidden="1">
       <c r="A32" s="1">
         <v>44302</v>
       </c>
@@ -1729,11 +1765,11 @@
         <v>0.36</v>
       </c>
       <c r="K32" s="4">
-        <f>D32*I32</f>
+        <f t="shared" si="0"/>
         <v>-36</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" hidden="1">
       <c r="A33" s="1">
         <v>44302</v>
       </c>
@@ -1762,11 +1798,11 @@
         <v>0.2</v>
       </c>
       <c r="K33" s="4">
-        <f>D33*I33</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" hidden="1">
       <c r="A34" s="1">
         <v>44305</v>
       </c>
@@ -1795,11 +1831,11 @@
         <v>3.4</v>
       </c>
       <c r="K34" s="4">
-        <f>D34*I34</f>
+        <f t="shared" ref="K34:K65" si="1">D34*I34</f>
         <v>-340</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" s="1">
         <v>44305</v>
       </c>
@@ -1828,11 +1864,11 @@
         <v>0.62</v>
       </c>
       <c r="K35" s="4">
-        <f>D35*I35</f>
+        <f t="shared" si="1"/>
         <v>-62</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" hidden="1">
       <c r="A36" s="1">
         <v>44305</v>
       </c>
@@ -1861,11 +1897,11 @@
         <v>2.42</v>
       </c>
       <c r="K36" s="4">
-        <f>D36*I36</f>
+        <f t="shared" si="1"/>
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" s="1">
         <v>44305</v>
       </c>
@@ -1894,7 +1930,7 @@
         <v>0.35</v>
       </c>
       <c r="K37" s="4">
-        <f>D37*I37</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="M37" s="5">
@@ -1902,7 +1938,7 @@
         <v>-125</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" s="1">
         <v>44305</v>
       </c>
@@ -1931,11 +1967,11 @@
         <v>31.58</v>
       </c>
       <c r="K38" s="4">
-        <f>D38*I38</f>
+        <f t="shared" si="1"/>
         <v>3158</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" s="1">
         <v>44305</v>
       </c>
@@ -1964,11 +2000,11 @@
         <v>44.53</v>
       </c>
       <c r="K39" s="4">
-        <f>D39*I39</f>
+        <f t="shared" si="1"/>
         <v>4453</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" s="1">
         <v>44305</v>
       </c>
@@ -1997,11 +2033,11 @@
         <v>29.45</v>
       </c>
       <c r="K40" s="4">
-        <f>D40*I40</f>
+        <f t="shared" si="1"/>
         <v>-2945</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" s="1">
         <v>44305</v>
       </c>
@@ -2030,7 +2066,7 @@
         <v>42.51</v>
       </c>
       <c r="K41" s="4">
-        <f>D41*I41</f>
+        <f t="shared" si="1"/>
         <v>-4251</v>
       </c>
       <c r="M41" s="5">
@@ -2038,7 +2074,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" s="1">
         <v>44306</v>
       </c>
@@ -2067,11 +2103,11 @@
         <v>14.97</v>
       </c>
       <c r="K42" s="4">
-        <f>D42*I42</f>
+        <f t="shared" si="1"/>
         <v>-1497</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" hidden="1">
       <c r="A43" s="1">
         <v>44306</v>
       </c>
@@ -2100,14 +2136,14 @@
         <v>12.27</v>
       </c>
       <c r="K43" s="4">
-        <f>D43*I43</f>
+        <f t="shared" si="1"/>
         <v>-1227</v>
       </c>
       <c r="L43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" s="1">
         <v>44306</v>
       </c>
@@ -2136,11 +2172,11 @@
         <v>16.37</v>
       </c>
       <c r="K44" s="4">
-        <f>D44*I44</f>
+        <f t="shared" si="1"/>
         <v>1637</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" s="1">
         <v>44306</v>
       </c>
@@ -2169,7 +2205,7 @@
         <v>14.27</v>
       </c>
       <c r="K45" s="4">
-        <f>D45*I45</f>
+        <f t="shared" si="1"/>
         <v>1427</v>
       </c>
       <c r="L45" t="s">
@@ -2180,7 +2216,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" s="1">
         <v>44309</v>
       </c>
@@ -2188,7 +2224,7 @@
         <v>38</v>
       </c>
       <c r="D46">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E46" t="s">
         <v>6</v>
@@ -2203,11 +2239,11 @@
         <v>4170</v>
       </c>
       <c r="K46" s="4">
-        <f>D46*I46</f>
-        <v>-417000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <f t="shared" si="1"/>
+        <v>417000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" s="1">
         <v>44309</v>
       </c>
@@ -2215,7 +2251,7 @@
         <v>38</v>
       </c>
       <c r="D47">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -2230,11 +2266,15 @@
         <v>4175</v>
       </c>
       <c r="K47" s="4">
-        <f>D47*I47</f>
-        <v>417500</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+        <f t="shared" si="1"/>
+        <v>-417500</v>
+      </c>
+      <c r="M47" s="5">
+        <f>K46+K47</f>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" hidden="1">
       <c r="A48" s="1">
         <v>44306</v>
       </c>
@@ -2257,11 +2297,11 @@
         <v>63.41</v>
       </c>
       <c r="K48" s="4">
-        <f>D48*I48</f>
+        <f t="shared" si="1"/>
         <v>6341</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" s="1">
         <v>44306</v>
       </c>
@@ -2290,7 +2330,7 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="K49" s="4">
-        <f>D49*I49</f>
+        <f t="shared" si="1"/>
         <v>-486.00000000000006</v>
       </c>
       <c r="M49" s="5">
@@ -2298,7 +2338,7 @@
         <v>5855</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" hidden="1">
       <c r="A50" s="1">
         <v>44307</v>
       </c>
@@ -2327,11 +2367,11 @@
         <v>1.05</v>
       </c>
       <c r="K50" s="4">
-        <f>D50*I50</f>
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" s="1">
         <v>44309</v>
       </c>
@@ -2354,11 +2394,11 @@
         <v>61.5</v>
       </c>
       <c r="K51" s="4">
-        <f>D51*I51</f>
+        <f t="shared" si="1"/>
         <v>-6150</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" s="1">
         <v>44307</v>
       </c>
@@ -2387,11 +2427,11 @@
         <v>5.95</v>
       </c>
       <c r="K52" s="4">
-        <f>D52*I52</f>
+        <f t="shared" si="1"/>
         <v>-595</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" hidden="1">
       <c r="A53" s="1">
         <v>44307</v>
       </c>
@@ -2414,7 +2454,7 @@
         <v>132.1</v>
       </c>
       <c r="K53" s="4">
-        <f>D53*I53</f>
+        <f t="shared" si="1"/>
         <v>13210</v>
       </c>
       <c r="M53" s="5">
@@ -2422,7 +2462,7 @@
         <v>12615</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" hidden="1">
       <c r="A54" s="1">
         <v>44307</v>
       </c>
@@ -2445,11 +2485,11 @@
         <v>22.84</v>
       </c>
       <c r="K54" s="4">
-        <f>D54*I54</f>
+        <f t="shared" si="1"/>
         <v>-2284</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" hidden="1">
       <c r="A55" s="1">
         <v>44308</v>
       </c>
@@ -2478,11 +2518,11 @@
         <v>2.19</v>
       </c>
       <c r="K55" s="4">
-        <f>D55*I55</f>
+        <f t="shared" si="1"/>
         <v>-219</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" hidden="1">
       <c r="A56" s="1">
         <v>44308</v>
       </c>
@@ -2511,11 +2551,11 @@
         <v>2.8</v>
       </c>
       <c r="K56" s="4">
-        <f>D56*I56</f>
+        <f t="shared" si="1"/>
         <v>-280</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" s="1">
         <v>44308</v>
       </c>
@@ -2544,11 +2584,11 @@
         <v>3.48</v>
       </c>
       <c r="K57" s="4">
-        <f>D57*I57</f>
+        <f t="shared" si="1"/>
         <v>348</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" hidden="1">
       <c r="A58" s="1">
         <v>44308</v>
       </c>
@@ -2577,7 +2617,7 @@
         <v>1.61</v>
       </c>
       <c r="K58" s="4">
-        <f>D58*I58</f>
+        <f t="shared" si="1"/>
         <v>161</v>
       </c>
       <c r="M58" s="5">
@@ -2585,7 +2625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" hidden="1">
       <c r="A59" s="1">
         <v>44308</v>
       </c>
@@ -2614,11 +2654,11 @@
         <v>30.05</v>
       </c>
       <c r="K59" s="4">
-        <f>D59*I59</f>
+        <f t="shared" si="1"/>
         <v>-3005</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" hidden="1">
       <c r="A60" s="1">
         <v>44308</v>
       </c>
@@ -2647,11 +2687,11 @@
         <v>32.450000000000003</v>
       </c>
       <c r="K60" s="4">
-        <f>D60*I60</f>
+        <f t="shared" si="1"/>
         <v>-3245.0000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" hidden="1">
       <c r="A61" s="1">
         <v>44308</v>
       </c>
@@ -2680,11 +2720,11 @@
         <v>30.85</v>
       </c>
       <c r="K61" s="4">
-        <f>D61*I61</f>
+        <f t="shared" si="1"/>
         <v>3085</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" s="1">
         <v>44308</v>
       </c>
@@ -2713,7 +2753,7 @@
         <v>34.75</v>
       </c>
       <c r="K62" s="4">
-        <f>D62*I62</f>
+        <f t="shared" si="1"/>
         <v>3475</v>
       </c>
       <c r="M62" s="5">
@@ -2721,7 +2761,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" s="1">
         <v>44308</v>
       </c>
@@ -2750,11 +2790,11 @@
         <v>64.8</v>
       </c>
       <c r="K63" s="4">
-        <f>D63*I63</f>
+        <f t="shared" si="1"/>
         <v>-6480</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" hidden="1">
       <c r="A64" s="1">
         <v>44308</v>
       </c>
@@ -2783,11 +2823,11 @@
         <v>50.58</v>
       </c>
       <c r="K64" s="4">
-        <f>D64*I64</f>
+        <f t="shared" si="1"/>
         <v>-5058</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" hidden="1">
       <c r="A65" s="1">
         <v>44308</v>
       </c>
@@ -2816,11 +2856,11 @@
         <v>66.91</v>
       </c>
       <c r="K65" s="4">
-        <f>D65*I65</f>
+        <f t="shared" si="1"/>
         <v>6691</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" hidden="1">
       <c r="A66" s="1">
         <v>44308</v>
       </c>
@@ -2849,7 +2889,7 @@
         <v>52.47</v>
       </c>
       <c r="K66" s="4">
-        <f>D66*I66</f>
+        <f t="shared" ref="K66:K117" si="2">D66*I66</f>
         <v>5247</v>
       </c>
       <c r="M66" s="5">
@@ -2857,7 +2897,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" hidden="1">
       <c r="A67" s="1">
         <v>44309</v>
       </c>
@@ -2886,11 +2926,11 @@
         <v>22.83</v>
       </c>
       <c r="K67" s="4">
-        <f>D67*I67</f>
+        <f t="shared" si="2"/>
         <v>2283</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" hidden="1">
       <c r="A68" s="1">
         <v>44309</v>
       </c>
@@ -2919,11 +2959,11 @@
         <v>24.99</v>
       </c>
       <c r="K68" s="4">
-        <f>D68*I68</f>
+        <f t="shared" si="2"/>
         <v>2499</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" hidden="1">
       <c r="A69" s="1">
         <v>44309</v>
       </c>
@@ -2952,11 +2992,11 @@
         <v>20.46</v>
       </c>
       <c r="K69" s="4">
-        <f>D69*I69</f>
+        <f t="shared" si="2"/>
         <v>-2046</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" hidden="1">
       <c r="A70" s="1">
         <v>44309</v>
       </c>
@@ -2985,7 +3025,7 @@
         <v>23.36</v>
       </c>
       <c r="K70" s="4">
-        <f>D70*I70</f>
+        <f t="shared" si="2"/>
         <v>-2336</v>
       </c>
       <c r="M70" s="5">
@@ -2993,7 +3033,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" hidden="1">
       <c r="A71" s="1">
         <v>44309</v>
       </c>
@@ -3022,11 +3062,11 @@
         <v>6.83</v>
       </c>
       <c r="K71" s="4">
-        <f>D71*I71</f>
+        <f t="shared" si="2"/>
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" hidden="1">
       <c r="A72" s="1">
         <v>44309</v>
       </c>
@@ -3055,11 +3095,11 @@
         <v>8.83</v>
       </c>
       <c r="K72" s="4">
-        <f>D72*I72</f>
+        <f t="shared" si="2"/>
         <v>883</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" hidden="1">
       <c r="A73" s="1">
         <v>44309</v>
       </c>
@@ -3088,11 +3128,11 @@
         <v>5.25</v>
       </c>
       <c r="K73" s="4">
-        <f>D73*I73</f>
+        <f t="shared" si="2"/>
         <v>-525</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" hidden="1">
       <c r="A74" s="1">
         <v>44309</v>
       </c>
@@ -3121,7 +3161,7 @@
         <v>7.51</v>
       </c>
       <c r="K74" s="4">
-        <f>D74*I74</f>
+        <f t="shared" si="2"/>
         <v>-751</v>
       </c>
       <c r="M74" s="5">
@@ -3129,7 +3169,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" hidden="1">
       <c r="A75" s="1">
         <v>44309</v>
       </c>
@@ -3152,11 +3192,11 @@
         <v>14.1</v>
       </c>
       <c r="K75" s="4">
-        <f>D75*I75</f>
+        <f t="shared" si="2"/>
         <v>-1410</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" hidden="1">
       <c r="A76" s="1">
         <v>44312</v>
       </c>
@@ -3185,11 +3225,11 @@
         <v>17.52</v>
       </c>
       <c r="K76" s="4">
-        <f>D76*I76</f>
+        <f t="shared" si="2"/>
         <v>-1752</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" hidden="1">
       <c r="A77" s="1">
         <v>44312</v>
       </c>
@@ -3218,11 +3258,11 @@
         <v>16.420000000000002</v>
       </c>
       <c r="K77" s="4">
-        <f>D77*I77</f>
+        <f t="shared" si="2"/>
         <v>-1642.0000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" hidden="1">
       <c r="A78" s="1">
         <v>44312</v>
       </c>
@@ -3251,11 +3291,11 @@
         <v>19.07</v>
       </c>
       <c r="K78" s="4">
-        <f>D78*I78</f>
+        <f t="shared" si="2"/>
         <v>1907</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" hidden="1">
       <c r="A79" s="1">
         <v>44312</v>
       </c>
@@ -3284,7 +3324,7 @@
         <v>18.77</v>
       </c>
       <c r="K79" s="4">
-        <f>D79*I79</f>
+        <f t="shared" si="2"/>
         <v>1877</v>
       </c>
       <c r="M79" s="5">
@@ -3292,7 +3332,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" s="1">
         <v>44312</v>
       </c>
@@ -3321,7 +3361,7 @@
         <v>0.83</v>
       </c>
       <c r="K80" s="4">
-        <f>D80*I80</f>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="M80" s="5" t="s">
@@ -3348,17 +3388,21 @@
         <v>44316</v>
       </c>
       <c r="G81" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H81" s="3">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="I81" s="2">
-        <v>6.99</v>
+        <v>8.35</v>
       </c>
       <c r="K81" s="4">
         <f>D81*I81</f>
-        <v>-699</v>
+        <v>-835</v>
+      </c>
+      <c r="M81" s="5">
+        <f>K81+K82</f>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3369,10 +3413,10 @@
         <v>65</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D82">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E82" t="s">
         <v>66</v>
@@ -3384,14 +3428,14 @@
         <v>23</v>
       </c>
       <c r="H82" s="3">
-        <v>305</v>
+        <v>302.5</v>
       </c>
       <c r="I82" s="2">
-        <v>8.35</v>
+        <v>9.34</v>
       </c>
       <c r="K82" s="4">
         <f>D82*I82</f>
-        <v>-835</v>
+        <v>934</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -3402,10 +3446,10 @@
         <v>65</v>
       </c>
       <c r="C83" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D83">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E83" t="s">
         <v>66</v>
@@ -3417,22 +3461,26 @@
         <v>8</v>
       </c>
       <c r="H83" s="3">
-        <v>297.5</v>
+        <v>295</v>
       </c>
       <c r="I83" s="2">
-        <v>8.1</v>
+        <v>6.99</v>
       </c>
       <c r="K83" s="4">
         <f>D83*I83</f>
-        <v>810</v>
+        <v>-699</v>
+      </c>
+      <c r="M83" s="5">
+        <f>K83+K84</f>
+        <v>-311</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="1">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C84" t="s">
         <v>4</v>
@@ -3447,24 +3495,20 @@
         <v>44316</v>
       </c>
       <c r="G84" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H84" s="3">
-        <v>302.5</v>
+        <v>295</v>
       </c>
       <c r="I84" s="2">
-        <v>9.34</v>
+        <v>3.88</v>
       </c>
       <c r="K84" s="4">
         <f>D84*I84</f>
-        <v>934</v>
-      </c>
-      <c r="M84" s="5">
-        <f>SUM(K81:K84)</f>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" s="1">
         <v>44312</v>
       </c>
@@ -3500,7 +3544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" hidden="1">
       <c r="A86" s="1">
         <v>44312</v>
       </c>
@@ -3536,14 +3580,1088 @@
         <v>70</v>
       </c>
     </row>
+    <row r="87" spans="1:13" hidden="1">
+      <c r="A87" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D87">
+        <v>100</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+      <c r="G87" t="s">
+        <v>58</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I87" s="2">
+        <v>4170</v>
+      </c>
+      <c r="K87" s="4">
+        <f>D87*I87</f>
+        <v>417000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" hidden="1">
+      <c r="A88" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88">
+        <v>-100</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" t="s">
+        <v>58</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I88" s="2">
+        <v>4175</v>
+      </c>
+      <c r="K88" s="4">
+        <f>D88*I88</f>
+        <v>-417500</v>
+      </c>
+      <c r="M88" s="5">
+        <f>SUM(K87:K88)</f>
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" hidden="1">
+      <c r="A89" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>100</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G89" t="s">
+        <v>8</v>
+      </c>
+      <c r="H89" s="3">
+        <v>4160</v>
+      </c>
+      <c r="I89" s="2">
+        <v>11.6</v>
+      </c>
+      <c r="K89" s="4">
+        <f>D89*I89</f>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" hidden="1">
+      <c r="A90" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90">
+        <v>100</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
+      </c>
+      <c r="F90" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G90" t="s">
+        <v>8</v>
+      </c>
+      <c r="H90" s="3">
+        <v>4135</v>
+      </c>
+      <c r="I90" s="2">
+        <v>6.87</v>
+      </c>
+      <c r="K90" s="4">
+        <f>D90*I90</f>
+        <v>687</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" hidden="1">
+      <c r="A91" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91">
+        <v>-100</v>
+      </c>
+      <c r="E91" t="s">
+        <v>6</v>
+      </c>
+      <c r="F91" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G91" t="s">
+        <v>8</v>
+      </c>
+      <c r="H91" s="3">
+        <v>4155</v>
+      </c>
+      <c r="I91" s="2">
+        <v>10.49</v>
+      </c>
+      <c r="K91" s="4">
+        <f>D91*I91</f>
+        <v>-1049</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" hidden="1">
+      <c r="A92" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>-100</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G92" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I92" s="2">
+        <v>7.68</v>
+      </c>
+      <c r="K92" s="4">
+        <f>D92*I92</f>
+        <v>-768</v>
+      </c>
+      <c r="M92" s="5">
+        <f>SUM(K89:K92)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93">
+        <v>100</v>
+      </c>
+      <c r="E93" t="s">
+        <v>66</v>
+      </c>
+      <c r="F93" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G93" t="s">
+        <v>8</v>
+      </c>
+      <c r="H93" s="3">
+        <v>297.5</v>
+      </c>
+      <c r="I93" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="K93" s="4">
+        <f>D93*I93</f>
+        <v>810</v>
+      </c>
+      <c r="M93" s="5">
+        <f>K93+K94</f>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>-100</v>
+      </c>
+      <c r="E94" t="s">
+        <v>66</v>
+      </c>
+      <c r="F94" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G94" t="s">
+        <v>8</v>
+      </c>
+      <c r="H94" s="3">
+        <v>297.5</v>
+      </c>
+      <c r="I94" s="2">
+        <v>4.82</v>
+      </c>
+      <c r="K94" s="4">
+        <f>D94*I94</f>
+        <v>-482</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <v>-100</v>
+      </c>
+      <c r="E95" t="s">
+        <v>66</v>
+      </c>
+      <c r="F95" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G95" t="s">
+        <v>8</v>
+      </c>
+      <c r="H95" s="3">
+        <v>300</v>
+      </c>
+      <c r="I95" s="2">
+        <v>5.72</v>
+      </c>
+      <c r="K95" s="4">
+        <f>D95*I95</f>
+        <v>-572</v>
+      </c>
+      <c r="M95" s="5">
+        <f>K95+K96</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>100</v>
+      </c>
+      <c r="E96" t="s">
+        <v>66</v>
+      </c>
+      <c r="F96" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G96" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="3">
+        <v>302.5</v>
+      </c>
+      <c r="I96" s="2">
+        <v>6.91</v>
+      </c>
+      <c r="K96" s="4">
+        <f>D96*I96</f>
+        <v>691</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" hidden="1">
+      <c r="A97" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97">
+        <v>100</v>
+      </c>
+      <c r="E97" t="s">
+        <v>37</v>
+      </c>
+      <c r="F97" s="1">
+        <v>44314</v>
+      </c>
+      <c r="G97" t="s">
+        <v>8</v>
+      </c>
+      <c r="H97" s="3">
+        <v>2275</v>
+      </c>
+      <c r="I97" s="2">
+        <v>7.23</v>
+      </c>
+      <c r="K97" s="4">
+        <f>D97*I97</f>
+        <v>723</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" hidden="1">
+      <c r="A98" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98">
+        <v>-100</v>
+      </c>
+      <c r="E98" t="s">
+        <v>37</v>
+      </c>
+      <c r="F98" s="1">
+        <v>44314</v>
+      </c>
+      <c r="G98" t="s">
+        <v>8</v>
+      </c>
+      <c r="H98" s="3">
+        <v>2270</v>
+      </c>
+      <c r="I98" s="2">
+        <v>6.15</v>
+      </c>
+      <c r="K98" s="4">
+        <f>D98*I98</f>
+        <v>-615</v>
+      </c>
+      <c r="M98" s="5">
+        <f>SUM(K97:K98)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" hidden="1">
+      <c r="A99" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C99" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>-100</v>
+      </c>
+      <c r="E99" t="s">
+        <v>37</v>
+      </c>
+      <c r="F99" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G99" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" s="3">
+        <v>2250</v>
+      </c>
+      <c r="I99" s="2">
+        <v>20.62</v>
+      </c>
+      <c r="K99" s="4">
+        <f>D99*I99</f>
+        <v>-2062</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" hidden="1">
+      <c r="A100" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100">
+        <v>-100</v>
+      </c>
+      <c r="E100" t="s">
+        <v>37</v>
+      </c>
+      <c r="F100" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G100" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="3">
+        <v>2215</v>
+      </c>
+      <c r="I100" s="2">
+        <v>13.05</v>
+      </c>
+      <c r="K100" s="4">
+        <f>D100*I100</f>
+        <v>-1305</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" hidden="1">
+      <c r="A101" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>100</v>
+      </c>
+      <c r="E101" t="s">
+        <v>37</v>
+      </c>
+      <c r="F101" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G101" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" s="3">
+        <v>2255</v>
+      </c>
+      <c r="I101" s="2">
+        <v>21.93</v>
+      </c>
+      <c r="K101" s="4">
+        <f>D101*I101</f>
+        <v>2193</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" hidden="1">
+      <c r="A102" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>100</v>
+      </c>
+      <c r="E102" t="s">
+        <v>37</v>
+      </c>
+      <c r="F102" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G102" t="s">
+        <v>8</v>
+      </c>
+      <c r="H102" s="3">
+        <v>2210</v>
+      </c>
+      <c r="I102" s="2">
+        <v>12.18</v>
+      </c>
+      <c r="K102" s="4">
+        <f>D102*I102</f>
+        <v>1218</v>
+      </c>
+      <c r="M102" s="5">
+        <f>SUM(K99:K102)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" hidden="1">
+      <c r="A103" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C103" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103">
+        <v>-100</v>
+      </c>
+      <c r="E103" t="s">
+        <v>51</v>
+      </c>
+      <c r="F103" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G103" t="s">
+        <v>8</v>
+      </c>
+      <c r="H103" s="3">
+        <v>3390</v>
+      </c>
+      <c r="I103" s="2">
+        <v>72.849999999999994</v>
+      </c>
+      <c r="K103" s="4">
+        <f>D103*I103</f>
+        <v>-7284.9999999999991</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" hidden="1">
+      <c r="A104" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>-100</v>
+      </c>
+      <c r="E104" t="s">
+        <v>51</v>
+      </c>
+      <c r="F104" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G104" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="3">
+        <v>3295</v>
+      </c>
+      <c r="I104" s="2">
+        <v>33.32</v>
+      </c>
+      <c r="K104" s="4">
+        <f>D104*I104</f>
+        <v>-3332</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" hidden="1">
+      <c r="A105" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>100</v>
+      </c>
+      <c r="E105" t="s">
+        <v>51</v>
+      </c>
+      <c r="F105" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G105" t="s">
+        <v>8</v>
+      </c>
+      <c r="H105" s="3">
+        <v>3395</v>
+      </c>
+      <c r="I105" s="2">
+        <v>75.34</v>
+      </c>
+      <c r="K105" s="4">
+        <f>D105*I105</f>
+        <v>7534</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" hidden="1">
+      <c r="A106" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>100</v>
+      </c>
+      <c r="E106" t="s">
+        <v>51</v>
+      </c>
+      <c r="F106" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G106" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="3">
+        <v>3290</v>
+      </c>
+      <c r="I106" s="2">
+        <v>31.77</v>
+      </c>
+      <c r="K106" s="4">
+        <f>D106*I106</f>
+        <v>3177</v>
+      </c>
+      <c r="M106" s="5">
+        <f>SUM(K103:K106)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" hidden="1">
+      <c r="A107" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107">
+        <v>100</v>
+      </c>
+      <c r="E107" t="s">
+        <v>77</v>
+      </c>
+      <c r="F107" s="1">
+        <v>44484</v>
+      </c>
+      <c r="G107" t="s">
+        <v>8</v>
+      </c>
+      <c r="H107" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="K107" s="4">
+        <f>D107*I107</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" hidden="1">
+      <c r="A108" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C108" t="s">
+        <v>10</v>
+      </c>
+      <c r="D108">
+        <v>-100</v>
+      </c>
+      <c r="E108" t="s">
+        <v>77</v>
+      </c>
+      <c r="F108" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G108" t="s">
+        <v>8</v>
+      </c>
+      <c r="H108" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="I108" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K108" s="4">
+        <f>D108*I108</f>
+        <v>-40</v>
+      </c>
+      <c r="M108" s="5">
+        <f>SUM(K107:K108)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" hidden="1">
+      <c r="A109" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C109" t="s">
+        <v>4</v>
+      </c>
+      <c r="D109">
+        <v>100</v>
+      </c>
+      <c r="E109" t="s">
+        <v>49</v>
+      </c>
+      <c r="F109" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G109" t="s">
+        <v>23</v>
+      </c>
+      <c r="H109" s="3">
+        <v>720</v>
+      </c>
+      <c r="I109" s="2">
+        <v>16.25</v>
+      </c>
+      <c r="K109" s="4">
+        <f>D109*I109</f>
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" hidden="1">
+      <c r="A110" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C110" t="s">
+        <v>10</v>
+      </c>
+      <c r="D110">
+        <v>-100</v>
+      </c>
+      <c r="E110" t="s">
+        <v>49</v>
+      </c>
+      <c r="F110" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G110" t="s">
+        <v>23</v>
+      </c>
+      <c r="H110" s="3">
+        <v>722.5</v>
+      </c>
+      <c r="I110" s="2">
+        <v>15.33</v>
+      </c>
+      <c r="K110" s="4">
+        <f>D110*I110</f>
+        <v>-1533</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" hidden="1">
+      <c r="A111" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111">
+        <v>-100</v>
+      </c>
+      <c r="E111" t="s">
+        <v>49</v>
+      </c>
+      <c r="F111" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G111" t="s">
+        <v>23</v>
+      </c>
+      <c r="H111" s="3">
+        <v>760</v>
+      </c>
+      <c r="I111" s="2">
+        <v>5.48</v>
+      </c>
+      <c r="K111" s="4">
+        <f>D111*I111</f>
+        <v>-548</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" hidden="1">
+      <c r="A112" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>100</v>
+      </c>
+      <c r="E112" t="s">
+        <v>49</v>
+      </c>
+      <c r="F112" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G112" t="s">
+        <v>23</v>
+      </c>
+      <c r="H112" s="3">
+        <v>765</v>
+      </c>
+      <c r="I112" s="2">
+        <v>4.72</v>
+      </c>
+      <c r="K112" s="4">
+        <f>D112*I112</f>
+        <v>472</v>
+      </c>
+      <c r="M112" s="5">
+        <f>SUM(K109:K112)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" hidden="1">
+      <c r="A113" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C113" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113">
+        <v>100</v>
+      </c>
+      <c r="E113" t="s">
+        <v>20</v>
+      </c>
+      <c r="F113" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G113" t="s">
+        <v>8</v>
+      </c>
+      <c r="H113" s="3">
+        <v>260</v>
+      </c>
+      <c r="I113" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="K113" s="4">
+        <f>D113*I113</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" hidden="1">
+      <c r="A114" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114">
+        <v>-100</v>
+      </c>
+      <c r="E114" t="s">
+        <v>20</v>
+      </c>
+      <c r="F114" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G114" t="s">
+        <v>8</v>
+      </c>
+      <c r="H114" s="3">
+        <v>262.5</v>
+      </c>
+      <c r="I114" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="K114" s="4">
+        <f>D114*I114</f>
+        <v>-93</v>
+      </c>
+      <c r="M114" s="5">
+        <f>SUM(K113:K114)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" hidden="1">
+      <c r="A115" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C115" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115">
+        <v>100</v>
+      </c>
+      <c r="E115" t="s">
+        <v>37</v>
+      </c>
+      <c r="F115" s="1">
+        <v>44314</v>
+      </c>
+      <c r="G115" t="s">
+        <v>23</v>
+      </c>
+      <c r="H115" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I115" s="2">
+        <v>2.46</v>
+      </c>
+      <c r="K115" s="4">
+        <f>D115*I115</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" hidden="1">
+      <c r="A116" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C116" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116">
+        <v>-100</v>
+      </c>
+      <c r="E116" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="1">
+        <v>44314</v>
+      </c>
+      <c r="G116" t="s">
+        <v>23</v>
+      </c>
+      <c r="H116" s="3">
+        <v>2315</v>
+      </c>
+      <c r="I116" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="K116" s="4">
+        <f>D116*I116</f>
+        <v>-136</v>
+      </c>
+      <c r="M116" s="5">
+        <f>SUM(K115:K116)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" hidden="1">
+      <c r="A117" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117">
+        <v>100</v>
+      </c>
+      <c r="E117" t="s">
+        <v>44</v>
+      </c>
+      <c r="F117" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G117" t="s">
+        <v>8</v>
+      </c>
+      <c r="H117" s="3">
+        <v>129</v>
+      </c>
+      <c r="I117" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="K117" s="4">
+        <f>D117*I117</f>
+        <v>53</v>
+      </c>
+      <c r="M117" s="5">
+        <f>K117</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="O118" s="5"/>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="M119" s="5">
+        <f>M81+M83+M93+M95</f>
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M75">
-    <filterColumn colId="0"/>
-    <filterColumn colId="5"/>
-    <sortState ref="A2:M75">
-      <sortCondition ref="B1"/>
+  <autoFilter ref="A1:M117">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="COIN"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A81:M96">
+      <sortCondition ref="G96"/>
     </sortState>
   </autoFilter>
+  <sortState ref="A81:M120">
+    <sortCondition ref="H1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update 4-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$144</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -265,6 +265,33 @@
   </si>
   <si>
     <t>1461-42206</t>
+  </si>
+  <si>
+    <t>1463-93568</t>
+  </si>
+  <si>
+    <t>1463-95748</t>
+  </si>
+  <si>
+    <t>1464-32193</t>
+  </si>
+  <si>
+    <t>1467-09373</t>
+  </si>
+  <si>
+    <t>1467-13391</t>
+  </si>
+  <si>
+    <t>1467-26853</t>
+  </si>
+  <si>
+    <t>1467-38684</t>
+  </si>
+  <si>
+    <t>1467-71429</t>
+  </si>
+  <si>
+    <t>NDX</t>
   </si>
 </sst>
 </file>
@@ -618,12 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:O144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M120" sqref="M120"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -684,7 +710,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1">
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>44293</v>
       </c>
@@ -717,7 +743,7 @@
         <v>-238</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>44293</v>
       </c>
@@ -754,7 +780,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>44293</v>
       </c>
@@ -787,7 +813,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>44293</v>
       </c>
@@ -824,7 +850,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1">
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
         <v>44295</v>
       </c>
@@ -857,7 +883,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1">
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
         <v>44295</v>
       </c>
@@ -890,7 +916,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1">
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
         <v>44295</v>
       </c>
@@ -923,7 +949,7 @@
         <v>-350</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1">
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
         <v>44295</v>
       </c>
@@ -962,7 +988,7 @@
       </c>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15" hidden="1">
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
         <v>44298</v>
       </c>
@@ -998,7 +1024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
         <v>44298</v>
       </c>
@@ -1034,7 +1060,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <v>44298</v>
       </c>
@@ -1067,7 +1093,7 @@
         <v>-186</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1">
+    <row r="13" spans="1:15">
       <c r="A13" s="1">
         <v>44298</v>
       </c>
@@ -1107,7 +1133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1">
+    <row r="14" spans="1:15">
       <c r="A14" s="1">
         <v>44298</v>
       </c>
@@ -1140,7 +1166,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1">
+    <row r="15" spans="1:15">
       <c r="A15" s="1">
         <v>44298</v>
       </c>
@@ -1177,7 +1203,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
         <v>44299</v>
       </c>
@@ -1210,7 +1236,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1">
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>44299</v>
       </c>
@@ -1250,7 +1276,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>44300</v>
       </c>
@@ -1283,7 +1309,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1">
+    <row r="19" spans="1:13">
       <c r="A19" s="1">
         <v>44300</v>
       </c>
@@ -1320,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1">
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>44300</v>
       </c>
@@ -1353,7 +1379,7 @@
         <v>-685</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1">
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>44300</v>
       </c>
@@ -1390,7 +1416,7 @@
         <v>120.00000000000011</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1">
+    <row r="22" spans="1:13">
       <c r="A22" s="1">
         <v>44301</v>
       </c>
@@ -1423,7 +1449,7 @@
         <v>-160</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1">
+    <row r="23" spans="1:13">
       <c r="A23" s="1">
         <v>44301</v>
       </c>
@@ -1460,7 +1486,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1">
+    <row r="24" spans="1:13">
       <c r="A24" s="1">
         <v>44301</v>
       </c>
@@ -1493,7 +1519,7 @@
         <v>-105</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1">
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
         <v>44301</v>
       </c>
@@ -1530,7 +1556,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1">
+    <row r="26" spans="1:13">
       <c r="A26" s="1">
         <v>44301</v>
       </c>
@@ -1563,7 +1589,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" s="1">
         <v>44301</v>
       </c>
@@ -1600,7 +1626,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" s="1">
         <v>44302</v>
       </c>
@@ -1633,7 +1659,7 @@
         <v>-727</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1">
+    <row r="29" spans="1:13">
       <c r="A29" s="1">
         <v>44302</v>
       </c>
@@ -1666,7 +1692,7 @@
         <v>-577</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="1">
         <v>44302</v>
       </c>
@@ -1699,7 +1725,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="1">
         <v>44302</v>
       </c>
@@ -1736,7 +1762,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" s="1">
         <v>44302</v>
       </c>
@@ -1769,7 +1795,7 @@
         <v>-36</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1">
+    <row r="33" spans="1:13">
       <c r="A33" s="1">
         <v>44302</v>
       </c>
@@ -1802,7 +1828,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1">
+    <row r="34" spans="1:13">
       <c r="A34" s="1">
         <v>44305</v>
       </c>
@@ -1835,7 +1861,7 @@
         <v>-340</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="1">
         <v>44305</v>
       </c>
@@ -1868,7 +1894,7 @@
         <v>-62</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" s="1">
         <v>44305</v>
       </c>
@@ -1901,7 +1927,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" s="1">
         <v>44305</v>
       </c>
@@ -1938,7 +1964,7 @@
         <v>-125</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" s="1">
         <v>44305</v>
       </c>
@@ -1971,7 +1997,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" s="1">
         <v>44305</v>
       </c>
@@ -2004,7 +2030,7 @@
         <v>4453</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" s="1">
         <v>44305</v>
       </c>
@@ -2037,7 +2063,7 @@
         <v>-2945</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" s="1">
         <v>44305</v>
       </c>
@@ -2074,7 +2100,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1">
+    <row r="42" spans="1:13">
       <c r="A42" s="1">
         <v>44306</v>
       </c>
@@ -2107,7 +2133,7 @@
         <v>-1497</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" s="1">
         <v>44306</v>
       </c>
@@ -2143,7 +2169,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1">
+    <row r="44" spans="1:13">
       <c r="A44" s="1">
         <v>44306</v>
       </c>
@@ -2176,7 +2202,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1">
+    <row r="45" spans="1:13">
       <c r="A45" s="1">
         <v>44306</v>
       </c>
@@ -2216,7 +2242,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1">
+    <row r="46" spans="1:13">
       <c r="A46" s="1">
         <v>44309</v>
       </c>
@@ -2243,7 +2269,7 @@
         <v>417000</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1">
+    <row r="47" spans="1:13">
       <c r="A47" s="1">
         <v>44309</v>
       </c>
@@ -2274,7 +2300,7 @@
         <v>-500</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1">
+    <row r="48" spans="1:13">
       <c r="A48" s="1">
         <v>44306</v>
       </c>
@@ -2301,7 +2327,7 @@
         <v>6341</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1">
+    <row r="49" spans="1:13">
       <c r="A49" s="1">
         <v>44306</v>
       </c>
@@ -2338,7 +2364,7 @@
         <v>5855</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1">
+    <row r="50" spans="1:13">
       <c r="A50" s="1">
         <v>44307</v>
       </c>
@@ -2371,7 +2397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1">
+    <row r="51" spans="1:13">
       <c r="A51" s="1">
         <v>44309</v>
       </c>
@@ -2398,7 +2424,7 @@
         <v>-6150</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="1">
         <v>44307</v>
       </c>
@@ -2431,7 +2457,7 @@
         <v>-595</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="1">
         <v>44307</v>
       </c>
@@ -2462,7 +2488,7 @@
         <v>12615</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="1">
         <v>44307</v>
       </c>
@@ -2489,7 +2515,7 @@
         <v>-2284</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1">
+    <row r="55" spans="1:13">
       <c r="A55" s="1">
         <v>44308</v>
       </c>
@@ -2522,7 +2548,7 @@
         <v>-219</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="1">
         <v>44308</v>
       </c>
@@ -2555,7 +2581,7 @@
         <v>-280</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1">
+    <row r="57" spans="1:13">
       <c r="A57" s="1">
         <v>44308</v>
       </c>
@@ -2588,7 +2614,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="1">
         <v>44308</v>
       </c>
@@ -2625,7 +2651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1">
+    <row r="59" spans="1:13">
       <c r="A59" s="1">
         <v>44308</v>
       </c>
@@ -2658,7 +2684,7 @@
         <v>-3005</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1">
+    <row r="60" spans="1:13">
       <c r="A60" s="1">
         <v>44308</v>
       </c>
@@ -2691,7 +2717,7 @@
         <v>-3245.0000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1">
+    <row r="61" spans="1:13">
       <c r="A61" s="1">
         <v>44308</v>
       </c>
@@ -2724,7 +2750,7 @@
         <v>3085</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" s="1">
         <v>44308</v>
       </c>
@@ -2761,7 +2787,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="1">
         <v>44308</v>
       </c>
@@ -2794,7 +2820,7 @@
         <v>-6480</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="1">
         <v>44308</v>
       </c>
@@ -2827,7 +2853,7 @@
         <v>-5058</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1">
+    <row r="65" spans="1:13">
       <c r="A65" s="1">
         <v>44308</v>
       </c>
@@ -2860,7 +2886,7 @@
         <v>6691</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1">
+    <row r="66" spans="1:13">
       <c r="A66" s="1">
         <v>44308</v>
       </c>
@@ -2889,7 +2915,7 @@
         <v>52.47</v>
       </c>
       <c r="K66" s="4">
-        <f t="shared" ref="K66:K117" si="2">D66*I66</f>
+        <f t="shared" ref="K66:K80" si="2">D66*I66</f>
         <v>5247</v>
       </c>
       <c r="M66" s="5">
@@ -2897,7 +2923,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1">
+    <row r="67" spans="1:13">
       <c r="A67" s="1">
         <v>44309</v>
       </c>
@@ -2930,7 +2956,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1">
+    <row r="68" spans="1:13">
       <c r="A68" s="1">
         <v>44309</v>
       </c>
@@ -2963,7 +2989,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1">
+    <row r="69" spans="1:13">
       <c r="A69" s="1">
         <v>44309</v>
       </c>
@@ -2996,7 +3022,7 @@
         <v>-2046</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1">
+    <row r="70" spans="1:13">
       <c r="A70" s="1">
         <v>44309</v>
       </c>
@@ -3033,7 +3059,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1">
+    <row r="71" spans="1:13">
       <c r="A71" s="1">
         <v>44309</v>
       </c>
@@ -3066,7 +3092,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1">
+    <row r="72" spans="1:13">
       <c r="A72" s="1">
         <v>44309</v>
       </c>
@@ -3099,7 +3125,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1">
+    <row r="73" spans="1:13">
       <c r="A73" s="1">
         <v>44309</v>
       </c>
@@ -3132,7 +3158,7 @@
         <v>-525</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1">
+    <row r="74" spans="1:13">
       <c r="A74" s="1">
         <v>44309</v>
       </c>
@@ -3169,7 +3195,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1">
+    <row r="75" spans="1:13">
       <c r="A75" s="1">
         <v>44309</v>
       </c>
@@ -3196,7 +3222,7 @@
         <v>-1410</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1">
+    <row r="76" spans="1:13">
       <c r="A76" s="1">
         <v>44312</v>
       </c>
@@ -3229,7 +3255,7 @@
         <v>-1752</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1">
+    <row r="77" spans="1:13">
       <c r="A77" s="1">
         <v>44312</v>
       </c>
@@ -3262,7 +3288,7 @@
         <v>-1642.0000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1">
+    <row r="78" spans="1:13">
       <c r="A78" s="1">
         <v>44312</v>
       </c>
@@ -3295,7 +3321,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1">
+    <row r="79" spans="1:13">
       <c r="A79" s="1">
         <v>44312</v>
       </c>
@@ -3332,7 +3358,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1">
+    <row r="80" spans="1:13">
       <c r="A80" s="1">
         <v>44312</v>
       </c>
@@ -3397,7 +3423,7 @@
         <v>8.35</v>
       </c>
       <c r="K81" s="4">
-        <f>D81*I81</f>
+        <f t="shared" ref="K81:K144" si="3">D81*I81</f>
         <v>-835</v>
       </c>
       <c r="M81" s="5">
@@ -3434,7 +3460,7 @@
         <v>9.34</v>
       </c>
       <c r="K82" s="4">
-        <f>D82*I82</f>
+        <f t="shared" si="3"/>
         <v>934</v>
       </c>
     </row>
@@ -3467,7 +3493,7 @@
         <v>6.99</v>
       </c>
       <c r="K83" s="4">
-        <f>D83*I83</f>
+        <f t="shared" si="3"/>
         <v>-699</v>
       </c>
       <c r="M83" s="5">
@@ -3504,11 +3530,11 @@
         <v>3.88</v>
       </c>
       <c r="K84" s="4">
-        <f>D84*I84</f>
+        <f t="shared" si="3"/>
         <v>388</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1">
+    <row r="85" spans="1:13">
       <c r="A85" s="1">
         <v>44312</v>
       </c>
@@ -3537,14 +3563,14 @@
         <v>3.25</v>
       </c>
       <c r="K85" s="4">
-        <f>D85*I85</f>
+        <f t="shared" si="3"/>
         <v>325</v>
       </c>
       <c r="M85" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1">
+    <row r="86" spans="1:13">
       <c r="A86" s="1">
         <v>44312</v>
       </c>
@@ -3573,14 +3599,14 @@
         <v>3.01</v>
       </c>
       <c r="K86" s="4">
-        <f>D86*I86</f>
+        <f t="shared" si="3"/>
         <v>-301</v>
       </c>
       <c r="M86" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1">
+    <row r="87" spans="1:13">
       <c r="A87" s="1">
         <v>44313</v>
       </c>
@@ -3603,11 +3629,11 @@
         <v>4170</v>
       </c>
       <c r="K87" s="4">
-        <f>D87*I87</f>
+        <f t="shared" si="3"/>
         <v>417000</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1">
+    <row r="88" spans="1:13">
       <c r="A88" s="1">
         <v>44313</v>
       </c>
@@ -3630,7 +3656,7 @@
         <v>4175</v>
       </c>
       <c r="K88" s="4">
-        <f>D88*I88</f>
+        <f t="shared" si="3"/>
         <v>-417500</v>
       </c>
       <c r="M88" s="5">
@@ -3638,7 +3664,7 @@
         <v>-500</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" s="1">
         <v>44313</v>
       </c>
@@ -3667,11 +3693,11 @@
         <v>11.6</v>
       </c>
       <c r="K89" s="4">
-        <f>D89*I89</f>
+        <f t="shared" si="3"/>
         <v>1160</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1">
+    <row r="90" spans="1:13">
       <c r="A90" s="1">
         <v>44313</v>
       </c>
@@ -3700,11 +3726,11 @@
         <v>6.87</v>
       </c>
       <c r="K90" s="4">
-        <f>D90*I90</f>
+        <f t="shared" si="3"/>
         <v>687</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1">
+    <row r="91" spans="1:13">
       <c r="A91" s="1">
         <v>44313</v>
       </c>
@@ -3733,11 +3759,11 @@
         <v>10.49</v>
       </c>
       <c r="K91" s="4">
-        <f>D91*I91</f>
+        <f t="shared" si="3"/>
         <v>-1049</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1">
+    <row r="92" spans="1:13">
       <c r="A92" s="1">
         <v>44313</v>
       </c>
@@ -3766,7 +3792,7 @@
         <v>7.68</v>
       </c>
       <c r="K92" s="4">
-        <f>D92*I92</f>
+        <f t="shared" si="3"/>
         <v>-768</v>
       </c>
       <c r="M92" s="5">
@@ -3803,7 +3829,7 @@
         <v>8.1</v>
       </c>
       <c r="K93" s="4">
-        <f>D93*I93</f>
+        <f t="shared" si="3"/>
         <v>810</v>
       </c>
       <c r="M93" s="5">
@@ -3840,7 +3866,7 @@
         <v>4.82</v>
       </c>
       <c r="K94" s="4">
-        <f>D94*I94</f>
+        <f t="shared" si="3"/>
         <v>-482</v>
       </c>
     </row>
@@ -3873,7 +3899,7 @@
         <v>5.72</v>
       </c>
       <c r="K95" s="4">
-        <f>D95*I95</f>
+        <f t="shared" si="3"/>
         <v>-572</v>
       </c>
       <c r="M95" s="5">
@@ -3910,11 +3936,11 @@
         <v>6.91</v>
       </c>
       <c r="K96" s="4">
-        <f>D96*I96</f>
+        <f t="shared" si="3"/>
         <v>691</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1">
+    <row r="97" spans="1:13">
       <c r="A97" s="1">
         <v>44313</v>
       </c>
@@ -3943,11 +3969,11 @@
         <v>7.23</v>
       </c>
       <c r="K97" s="4">
-        <f>D97*I97</f>
+        <f t="shared" si="3"/>
         <v>723</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1">
+    <row r="98" spans="1:13">
       <c r="A98" s="1">
         <v>44313</v>
       </c>
@@ -3976,7 +4002,7 @@
         <v>6.15</v>
       </c>
       <c r="K98" s="4">
-        <f>D98*I98</f>
+        <f t="shared" si="3"/>
         <v>-615</v>
       </c>
       <c r="M98" s="5">
@@ -3984,7 +4010,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1">
+    <row r="99" spans="1:13">
       <c r="A99" s="1">
         <v>44313</v>
       </c>
@@ -4013,11 +4039,11 @@
         <v>20.62</v>
       </c>
       <c r="K99" s="4">
-        <f>D99*I99</f>
+        <f t="shared" si="3"/>
         <v>-2062</v>
       </c>
     </row>
-    <row r="100" spans="1:13" hidden="1">
+    <row r="100" spans="1:13">
       <c r="A100" s="1">
         <v>44313</v>
       </c>
@@ -4046,11 +4072,11 @@
         <v>13.05</v>
       </c>
       <c r="K100" s="4">
-        <f>D100*I100</f>
+        <f t="shared" si="3"/>
         <v>-1305</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1">
+    <row r="101" spans="1:13">
       <c r="A101" s="1">
         <v>44313</v>
       </c>
@@ -4079,11 +4105,11 @@
         <v>21.93</v>
       </c>
       <c r="K101" s="4">
-        <f>D101*I101</f>
+        <f t="shared" si="3"/>
         <v>2193</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1">
+    <row r="102" spans="1:13">
       <c r="A102" s="1">
         <v>44313</v>
       </c>
@@ -4112,7 +4138,7 @@
         <v>12.18</v>
       </c>
       <c r="K102" s="4">
-        <f>D102*I102</f>
+        <f t="shared" si="3"/>
         <v>1218</v>
       </c>
       <c r="M102" s="5">
@@ -4120,7 +4146,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1">
+    <row r="103" spans="1:13">
       <c r="A103" s="1">
         <v>44313</v>
       </c>
@@ -4149,11 +4175,11 @@
         <v>72.849999999999994</v>
       </c>
       <c r="K103" s="4">
-        <f>D103*I103</f>
+        <f t="shared" si="3"/>
         <v>-7284.9999999999991</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1">
+    <row r="104" spans="1:13">
       <c r="A104" s="1">
         <v>44313</v>
       </c>
@@ -4182,11 +4208,11 @@
         <v>33.32</v>
       </c>
       <c r="K104" s="4">
-        <f>D104*I104</f>
+        <f t="shared" si="3"/>
         <v>-3332</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1">
+    <row r="105" spans="1:13">
       <c r="A105" s="1">
         <v>44313</v>
       </c>
@@ -4215,11 +4241,11 @@
         <v>75.34</v>
       </c>
       <c r="K105" s="4">
-        <f>D105*I105</f>
+        <f t="shared" si="3"/>
         <v>7534</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1">
+    <row r="106" spans="1:13">
       <c r="A106" s="1">
         <v>44313</v>
       </c>
@@ -4248,7 +4274,7 @@
         <v>31.77</v>
       </c>
       <c r="K106" s="4">
-        <f>D106*I106</f>
+        <f t="shared" si="3"/>
         <v>3177</v>
       </c>
       <c r="M106" s="5">
@@ -4256,7 +4282,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1">
+    <row r="107" spans="1:13">
       <c r="A107" s="1">
         <v>44314</v>
       </c>
@@ -4285,11 +4311,11 @@
         <v>0.85</v>
       </c>
       <c r="K107" s="4">
-        <f>D107*I107</f>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1">
+    <row r="108" spans="1:13">
       <c r="A108" s="1">
         <v>44314</v>
       </c>
@@ -4318,7 +4344,7 @@
         <v>0.4</v>
       </c>
       <c r="K108" s="4">
-        <f>D108*I108</f>
+        <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="M108" s="5">
@@ -4326,7 +4352,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1">
+    <row r="109" spans="1:13">
       <c r="A109" s="1">
         <v>44314</v>
       </c>
@@ -4355,11 +4381,11 @@
         <v>16.25</v>
       </c>
       <c r="K109" s="4">
-        <f>D109*I109</f>
+        <f t="shared" si="3"/>
         <v>1625</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1">
+    <row r="110" spans="1:13">
       <c r="A110" s="1">
         <v>44314</v>
       </c>
@@ -4388,11 +4414,11 @@
         <v>15.33</v>
       </c>
       <c r="K110" s="4">
-        <f>D110*I110</f>
+        <f t="shared" si="3"/>
         <v>-1533</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1">
+    <row r="111" spans="1:13">
       <c r="A111" s="1">
         <v>44314</v>
       </c>
@@ -4421,11 +4447,11 @@
         <v>5.48</v>
       </c>
       <c r="K111" s="4">
-        <f>D111*I111</f>
+        <f t="shared" si="3"/>
         <v>-548</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1">
+    <row r="112" spans="1:13">
       <c r="A112" s="1">
         <v>44314</v>
       </c>
@@ -4454,7 +4480,7 @@
         <v>4.72</v>
       </c>
       <c r="K112" s="4">
-        <f>D112*I112</f>
+        <f t="shared" si="3"/>
         <v>472</v>
       </c>
       <c r="M112" s="5">
@@ -4462,7 +4488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1">
+    <row r="113" spans="1:15">
       <c r="A113" s="1">
         <v>44314</v>
       </c>
@@ -4491,11 +4517,11 @@
         <v>1.36</v>
       </c>
       <c r="K113" s="4">
-        <f>D113*I113</f>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:15" hidden="1">
+    <row r="114" spans="1:15">
       <c r="A114" s="1">
         <v>44314</v>
       </c>
@@ -4524,7 +4550,7 @@
         <v>0.93</v>
       </c>
       <c r="K114" s="4">
-        <f>D114*I114</f>
+        <f t="shared" si="3"/>
         <v>-93</v>
       </c>
       <c r="M114" s="5">
@@ -4532,7 +4558,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1">
+    <row r="115" spans="1:15">
       <c r="A115" s="1">
         <v>44314</v>
       </c>
@@ -4561,11 +4587,11 @@
         <v>2.46</v>
       </c>
       <c r="K115" s="4">
-        <f>D115*I115</f>
+        <f t="shared" si="3"/>
         <v>246</v>
       </c>
     </row>
-    <row r="116" spans="1:15" hidden="1">
+    <row r="116" spans="1:15">
       <c r="A116" s="1">
         <v>44314</v>
       </c>
@@ -4594,7 +4620,7 @@
         <v>1.36</v>
       </c>
       <c r="K116" s="4">
-        <f>D116*I116</f>
+        <f t="shared" si="3"/>
         <v>-136</v>
       </c>
       <c r="M116" s="5">
@@ -4602,7 +4628,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1">
+    <row r="117" spans="1:15">
       <c r="A117" s="1">
         <v>44314</v>
       </c>
@@ -4631,7 +4657,7 @@
         <v>0.53</v>
       </c>
       <c r="K117" s="4">
-        <f>D117*I117</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="M117" s="5">
@@ -4640,25 +4666,863 @@
       </c>
     </row>
     <row r="118" spans="1:15">
+      <c r="A118" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118">
+        <v>-100</v>
+      </c>
+      <c r="E118" t="s">
+        <v>49</v>
+      </c>
+      <c r="F118" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G118" t="s">
+        <v>23</v>
+      </c>
+      <c r="H118" s="3">
+        <v>712.5</v>
+      </c>
+      <c r="I118" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="K118" s="4">
+        <f t="shared" si="3"/>
+        <v>-330</v>
+      </c>
       <c r="O118" s="5"/>
     </row>
     <row r="119" spans="1:15">
-      <c r="M119" s="5">
-        <f>M81+M83+M93+M95</f>
-        <v>235</v>
+      <c r="A119" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C119" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119">
+        <v>100</v>
+      </c>
+      <c r="E119" t="s">
+        <v>49</v>
+      </c>
+      <c r="F119" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G119" t="s">
+        <v>23</v>
+      </c>
+      <c r="H119" s="3">
+        <v>710</v>
+      </c>
+      <c r="I119" s="2">
+        <v>3.88</v>
+      </c>
+      <c r="K119" s="4">
+        <f t="shared" si="3"/>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C120" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120">
+        <v>-100</v>
+      </c>
+      <c r="E120" t="s">
+        <v>49</v>
+      </c>
+      <c r="F120" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G120" t="s">
+        <v>8</v>
+      </c>
+      <c r="H120" s="3">
+        <v>680</v>
+      </c>
+      <c r="I120" s="2">
+        <v>3.65</v>
+      </c>
+      <c r="K120" s="4">
+        <f t="shared" si="3"/>
+        <v>-365</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121">
+        <v>100</v>
+      </c>
+      <c r="E121" t="s">
+        <v>49</v>
+      </c>
+      <c r="F121" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G121" t="s">
+        <v>8</v>
+      </c>
+      <c r="H121" s="3">
+        <v>677.5</v>
+      </c>
+      <c r="I121" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="K121" s="4">
+        <f t="shared" si="3"/>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C122" t="s">
+        <v>4</v>
+      </c>
+      <c r="D122">
+        <v>100</v>
+      </c>
+      <c r="E122" t="s">
+        <v>51</v>
+      </c>
+      <c r="F122" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G122" t="s">
+        <v>8</v>
+      </c>
+      <c r="H122" s="3">
+        <v>3340</v>
+      </c>
+      <c r="I122" s="2">
+        <v>19.45</v>
+      </c>
+      <c r="K122" s="4">
+        <f t="shared" si="3"/>
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15">
+      <c r="A123" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C123" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123">
+        <v>-100</v>
+      </c>
+      <c r="E123" t="s">
+        <v>51</v>
+      </c>
+      <c r="F123" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G123" t="s">
+        <v>8</v>
+      </c>
+      <c r="H123" s="3">
+        <v>3335</v>
+      </c>
+      <c r="I123" s="2">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="K123" s="4">
+        <f t="shared" si="3"/>
+        <v>-1835.0000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15">
+      <c r="A124" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C124" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124">
+        <v>-100</v>
+      </c>
+      <c r="E124" t="s">
+        <v>44</v>
+      </c>
+      <c r="F124" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G124" t="s">
+        <v>8</v>
+      </c>
+      <c r="H124" s="3">
+        <v>129</v>
+      </c>
+      <c r="I124" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="K124" s="4">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="A125" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C125" t="s">
+        <v>4</v>
+      </c>
+      <c r="D125">
+        <v>100</v>
+      </c>
+      <c r="E125" t="s">
+        <v>44</v>
+      </c>
+      <c r="F125" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G125" t="s">
+        <v>8</v>
+      </c>
+      <c r="H125" s="3">
+        <v>130</v>
+      </c>
+      <c r="I125" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="K125" s="4">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C126" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126">
+        <v>100</v>
+      </c>
+      <c r="E126" t="s">
+        <v>66</v>
+      </c>
+      <c r="F126" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G126" t="s">
+        <v>8</v>
+      </c>
+      <c r="H126" s="3">
+        <v>292.5</v>
+      </c>
+      <c r="I126" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="K126" s="4">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C127" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127">
+        <v>-100</v>
+      </c>
+      <c r="E127" t="s">
+        <v>6</v>
+      </c>
+      <c r="F127" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G127" t="s">
+        <v>23</v>
+      </c>
+      <c r="H127" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I127" s="2">
+        <v>2.97</v>
+      </c>
+      <c r="K127" s="4">
+        <f t="shared" si="3"/>
+        <v>-297</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128">
+        <v>-100</v>
+      </c>
+      <c r="E128" t="s">
+        <v>6</v>
+      </c>
+      <c r="F128" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G128" t="s">
+        <v>8</v>
+      </c>
+      <c r="H128" s="3">
+        <v>4175</v>
+      </c>
+      <c r="I128" s="2">
+        <v>3.47</v>
+      </c>
+      <c r="K128" s="4">
+        <f t="shared" si="3"/>
+        <v>-347</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C129" t="s">
+        <v>4</v>
+      </c>
+      <c r="D129">
+        <v>100</v>
+      </c>
+      <c r="E129" t="s">
+        <v>6</v>
+      </c>
+      <c r="F129" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G129" t="s">
+        <v>23</v>
+      </c>
+      <c r="H129" s="3">
+        <v>4205</v>
+      </c>
+      <c r="I129" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="K129" s="4">
+        <f t="shared" si="3"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C130" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>100</v>
+      </c>
+      <c r="E130" t="s">
+        <v>6</v>
+      </c>
+      <c r="F130" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G130" t="s">
+        <v>8</v>
+      </c>
+      <c r="H130" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I130" s="2">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="K130" s="4">
+        <f t="shared" si="3"/>
+        <v>252.99999999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C131" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131">
+        <v>-100</v>
+      </c>
+      <c r="E131" t="s">
+        <v>49</v>
+      </c>
+      <c r="F131" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G131" t="s">
+        <v>23</v>
+      </c>
+      <c r="H131" s="3">
+        <v>710</v>
+      </c>
+      <c r="I131" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="K131" s="4">
+        <f t="shared" si="3"/>
+        <v>-97</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132">
+        <v>-100</v>
+      </c>
+      <c r="E132" t="s">
+        <v>49</v>
+      </c>
+      <c r="F132" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G132" t="s">
+        <v>8</v>
+      </c>
+      <c r="H132" s="3">
+        <v>680</v>
+      </c>
+      <c r="I132" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="K132" s="4">
+        <f t="shared" si="3"/>
+        <v>-87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
+      <c r="A133" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" t="s">
+        <v>4</v>
+      </c>
+      <c r="D133">
+        <v>100</v>
+      </c>
+      <c r="E133" t="s">
+        <v>49</v>
+      </c>
+      <c r="F133" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G133" t="s">
+        <v>23</v>
+      </c>
+      <c r="H133" s="3">
+        <v>712.5</v>
+      </c>
+      <c r="I133" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="K133" s="4">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
+      <c r="A134" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C134" t="s">
+        <v>4</v>
+      </c>
+      <c r="D134">
+        <v>100</v>
+      </c>
+      <c r="E134" t="s">
+        <v>49</v>
+      </c>
+      <c r="F134" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G134" t="s">
+        <v>8</v>
+      </c>
+      <c r="H134" s="3">
+        <v>677.5</v>
+      </c>
+      <c r="I134" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="K134" s="4">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
+      <c r="A135" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C135" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135">
+        <v>-100</v>
+      </c>
+      <c r="E135" t="s">
+        <v>90</v>
+      </c>
+      <c r="F135" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G135" t="s">
+        <v>8</v>
+      </c>
+      <c r="H135" s="3">
+        <v>13760</v>
+      </c>
+      <c r="I135" s="2">
+        <v>3</v>
+      </c>
+      <c r="K135" s="4">
+        <f t="shared" si="3"/>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
+      <c r="A136" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136">
+        <v>-100</v>
+      </c>
+      <c r="E136" t="s">
+        <v>90</v>
+      </c>
+      <c r="F136" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G136" t="s">
+        <v>23</v>
+      </c>
+      <c r="H136" s="3">
+        <v>14070</v>
+      </c>
+      <c r="I136" s="2">
+        <v>1.65</v>
+      </c>
+      <c r="K136" s="4">
+        <f t="shared" si="3"/>
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
+      <c r="A137" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C137" t="s">
+        <v>4</v>
+      </c>
+      <c r="D137">
+        <v>100</v>
+      </c>
+      <c r="E137" t="s">
+        <v>90</v>
+      </c>
+      <c r="F137" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G137" t="s">
+        <v>8</v>
+      </c>
+      <c r="H137" s="3">
+        <v>13770</v>
+      </c>
+      <c r="I137" s="2">
+        <v>3.39</v>
+      </c>
+      <c r="K137" s="4">
+        <f t="shared" si="3"/>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
+      <c r="A138" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C138" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138">
+        <v>100</v>
+      </c>
+      <c r="E138" t="s">
+        <v>90</v>
+      </c>
+      <c r="F138" s="1">
+        <v>44316</v>
+      </c>
+      <c r="G138" t="s">
+        <v>23</v>
+      </c>
+      <c r="H138" s="3">
+        <v>14040</v>
+      </c>
+      <c r="I138" s="2">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="K138" s="4">
+        <f t="shared" si="3"/>
+        <v>249.00000000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
+      <c r="A139" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D139">
+        <v>100</v>
+      </c>
+      <c r="E139" t="s">
+        <v>6</v>
+      </c>
+      <c r="G139" t="s">
+        <v>58</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I139" s="2">
+        <v>4170</v>
+      </c>
+      <c r="K139" s="4">
+        <f t="shared" si="3"/>
+        <v>417000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
+      <c r="A140" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D140">
+        <v>-100</v>
+      </c>
+      <c r="E140" t="s">
+        <v>6</v>
+      </c>
+      <c r="G140" t="s">
+        <v>58</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I140" s="2">
+        <v>4175</v>
+      </c>
+      <c r="K140" s="4">
+        <f t="shared" si="3"/>
+        <v>-417500</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
+      <c r="A141" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D141">
+        <v>100</v>
+      </c>
+      <c r="E141" t="s">
+        <v>66</v>
+      </c>
+      <c r="G141" t="s">
+        <v>41</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I141" s="2">
+        <v>302.5</v>
+      </c>
+      <c r="K141" s="4">
+        <f t="shared" si="3"/>
+        <v>30250</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
+      <c r="A142" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D142">
+        <v>-100</v>
+      </c>
+      <c r="E142" t="s">
+        <v>66</v>
+      </c>
+      <c r="G142" t="s">
+        <v>41</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I142" s="2">
+        <v>300</v>
+      </c>
+      <c r="K142" s="4">
+        <f t="shared" si="3"/>
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
+      <c r="A143" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D143">
+        <v>100</v>
+      </c>
+      <c r="E143" t="s">
+        <v>51</v>
+      </c>
+      <c r="G143" t="s">
+        <v>41</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I143" s="2">
+        <v>3405</v>
+      </c>
+      <c r="K143" s="4">
+        <f t="shared" si="3"/>
+        <v>340500</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
+      <c r="A144" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D144">
+        <v>-100</v>
+      </c>
+      <c r="E144" t="s">
+        <v>51</v>
+      </c>
+      <c r="G144" t="s">
+        <v>41</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I144" s="2">
+        <v>340</v>
+      </c>
+      <c r="K144" s="4">
+        <f t="shared" si="3"/>
+        <v>-34000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M117">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="COIN"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A81:M96">
-      <sortCondition ref="G96"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M144"/>
   <sortState ref="A81:M120">
     <sortCondition ref="H1"/>
   </sortState>

</xml_diff>

<commit_message>
Update 8-Mei-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="131">
   <si>
     <t>Date</t>
   </si>
@@ -358,6 +358,60 @@
   </si>
   <si>
     <t>Buy stock. Collect monthly dividend</t>
+  </si>
+  <si>
+    <t>1475-35669</t>
+  </si>
+  <si>
+    <t>1475-46921</t>
+  </si>
+  <si>
+    <t>1475-50272</t>
+  </si>
+  <si>
+    <t>1475-51771</t>
+  </si>
+  <si>
+    <t>1476-15086</t>
+  </si>
+  <si>
+    <t>1475-21836</t>
+  </si>
+  <si>
+    <t>1478-50655</t>
+  </si>
+  <si>
+    <t>1478-60903</t>
+  </si>
+  <si>
+    <t>1478-72081</t>
+  </si>
+  <si>
+    <t>1478-65729</t>
+  </si>
+  <si>
+    <t>1478-71147</t>
+  </si>
+  <si>
+    <t>1480-77927</t>
+  </si>
+  <si>
+    <t>1480-86526</t>
+  </si>
+  <si>
+    <t>1480-88590</t>
+  </si>
+  <si>
+    <t>1480-97989</t>
+  </si>
+  <si>
+    <t>1481-01456</t>
+  </si>
+  <si>
+    <t>1481-33736</t>
+  </si>
+  <si>
+    <t>1481-42873</t>
   </si>
 </sst>
 </file>
@@ -387,12 +441,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -408,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -416,6 +476,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -711,11 +777,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O280"/>
+  <dimension ref="A1:O333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
+      <pane ySplit="1" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -730,7 +796,7 @@
     <col min="8" max="8" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3651,7 +3717,7 @@
         <v>8.35</v>
       </c>
       <c r="K116" s="4">
-        <f t="shared" ref="K116:K266" si="3">D116*I116</f>
+        <f t="shared" ref="K116:K270" si="3">D116*I116</f>
         <v>-835</v>
       </c>
     </row>
@@ -5658,73 +5724,37 @@
       </c>
     </row>
     <row r="212" spans="1:12">
-      <c r="L212" s="6"/>
-    </row>
-    <row r="213" spans="1:12">
-      <c r="A213" s="1">
+      <c r="A212" s="1">
         <v>44319</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C213" t="s">
-        <v>4</v>
-      </c>
-      <c r="D213">
-        <v>100</v>
-      </c>
-      <c r="E213" t="s">
+      <c r="B212" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C212" t="s">
+        <v>10</v>
+      </c>
+      <c r="D212">
+        <v>-100</v>
+      </c>
+      <c r="E212" t="s">
         <v>87</v>
       </c>
-      <c r="F213" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G213" t="s">
-        <v>23</v>
-      </c>
-      <c r="H213" s="3">
-        <v>14190</v>
-      </c>
-      <c r="I213" s="2">
-        <v>12.45</v>
-      </c>
-      <c r="K213" s="4">
-        <f t="shared" si="3"/>
-        <v>1245</v>
+      <c r="G212" t="s">
+        <v>57</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I212" s="2">
+        <v>13600</v>
+      </c>
+      <c r="K212" s="4">
+        <f>D212*I212</f>
+        <v>-1360000</v>
       </c>
     </row>
     <row r="214" spans="1:12">
-      <c r="A214" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C214" t="s">
-        <v>10</v>
-      </c>
-      <c r="D214">
-        <v>-100</v>
-      </c>
-      <c r="E214" t="s">
-        <v>87</v>
-      </c>
-      <c r="F214" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G214" t="s">
-        <v>23</v>
-      </c>
-      <c r="H214" s="3">
-        <v>14200</v>
-      </c>
-      <c r="I214" s="2">
-        <v>11.55</v>
-      </c>
-      <c r="K214" s="4">
-        <f t="shared" si="3"/>
-        <v>-1155</v>
-      </c>
+      <c r="L214" s="6"/>
     </row>
     <row r="215" spans="1:12">
       <c r="A215" s="1">
@@ -5743,20 +5773,20 @@
         <v>87</v>
       </c>
       <c r="F215" s="1">
-        <v>44319</v>
+        <v>44323</v>
       </c>
       <c r="G215" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H215" s="3">
-        <v>13570</v>
+        <v>14190</v>
       </c>
       <c r="I215" s="2">
-        <v>30.78</v>
+        <v>12.45</v>
       </c>
       <c r="K215" s="4">
         <f t="shared" si="3"/>
-        <v>3078</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="216" spans="1:12">
@@ -5776,91 +5806,91 @@
         <v>87</v>
       </c>
       <c r="F216" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G216" t="s">
+        <v>23</v>
+      </c>
+      <c r="H216" s="3">
+        <v>14200</v>
+      </c>
+      <c r="I216" s="2">
+        <v>11.55</v>
+      </c>
+      <c r="K216" s="4">
+        <f t="shared" si="3"/>
+        <v>-1155</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
+      <c r="A217" s="1">
         <v>44319</v>
       </c>
-      <c r="G216" t="s">
-        <v>8</v>
-      </c>
-      <c r="H216" s="3">
-        <v>13540</v>
-      </c>
-      <c r="I216" s="2">
-        <v>27.1</v>
-      </c>
-      <c r="K216" s="4">
-        <f t="shared" si="3"/>
-        <v>-2710</v>
-      </c>
-      <c r="L216" s="6"/>
-    </row>
-    <row r="217" spans="1:12">
-      <c r="L217" s="6"/>
+      <c r="B217" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C217" t="s">
+        <v>4</v>
+      </c>
+      <c r="D217">
+        <v>100</v>
+      </c>
+      <c r="E217" t="s">
+        <v>87</v>
+      </c>
+      <c r="F217" s="1">
+        <v>44319</v>
+      </c>
+      <c r="G217" t="s">
+        <v>8</v>
+      </c>
+      <c r="H217" s="3">
+        <v>13570</v>
+      </c>
+      <c r="I217" s="2">
+        <v>30.78</v>
+      </c>
+      <c r="K217" s="4">
+        <f t="shared" si="3"/>
+        <v>3078</v>
+      </c>
     </row>
     <row r="218" spans="1:12">
       <c r="A218" s="1">
         <v>44319</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C218" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D218">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E218" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="F218" s="1">
-        <v>44321</v>
+        <v>44319</v>
       </c>
       <c r="G218" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H218" s="3">
-        <v>4250</v>
+        <v>13540</v>
       </c>
       <c r="I218" s="2">
-        <v>2.06</v>
+        <v>27.1</v>
       </c>
       <c r="K218" s="4">
         <f t="shared" si="3"/>
-        <v>206</v>
-      </c>
+        <v>-2710</v>
+      </c>
+      <c r="L218" s="6"/>
     </row>
     <row r="219" spans="1:12">
-      <c r="A219" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C219" t="s">
-        <v>4</v>
-      </c>
-      <c r="D219">
-        <v>100</v>
-      </c>
-      <c r="E219" t="s">
-        <v>6</v>
-      </c>
-      <c r="F219" s="1">
-        <v>44321</v>
-      </c>
-      <c r="G219" t="s">
-        <v>8</v>
-      </c>
-      <c r="H219" s="3">
-        <v>4150</v>
-      </c>
-      <c r="I219" s="2">
-        <v>4.22</v>
-      </c>
-      <c r="K219" s="4">
-        <f t="shared" si="3"/>
-        <v>422</v>
-      </c>
+      <c r="L219" s="6"/>
     </row>
     <row r="220" spans="1:12">
       <c r="A220" s="1">
@@ -5870,10 +5900,10 @@
         <v>90</v>
       </c>
       <c r="C220" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D220">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E220" t="s">
         <v>6</v>
@@ -5885,14 +5915,14 @@
         <v>23</v>
       </c>
       <c r="H220" s="3">
-        <v>4255</v>
+        <v>4250</v>
       </c>
       <c r="I220" s="2">
-        <v>1.57</v>
+        <v>2.06</v>
       </c>
       <c r="K220" s="4">
         <f t="shared" si="3"/>
-        <v>-157</v>
+        <v>206</v>
       </c>
     </row>
     <row r="221" spans="1:12">
@@ -5903,10 +5933,10 @@
         <v>90</v>
       </c>
       <c r="C221" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D221">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E221" t="s">
         <v>6</v>
@@ -5918,85 +5948,85 @@
         <v>8</v>
       </c>
       <c r="H221" s="3">
-        <v>4145</v>
+        <v>4150</v>
       </c>
       <c r="I221" s="2">
-        <v>3.71</v>
+        <v>4.22</v>
       </c>
       <c r="K221" s="4">
         <f t="shared" si="3"/>
-        <v>-371</v>
-      </c>
-      <c r="L221" s="6"/>
+        <v>422</v>
+      </c>
     </row>
     <row r="222" spans="1:12">
-      <c r="L222" s="6"/>
+      <c r="A222" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C222" t="s">
+        <v>10</v>
+      </c>
+      <c r="D222">
+        <v>-100</v>
+      </c>
+      <c r="E222" t="s">
+        <v>6</v>
+      </c>
+      <c r="F222" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G222" t="s">
+        <v>23</v>
+      </c>
+      <c r="H222" s="3">
+        <v>4255</v>
+      </c>
+      <c r="I222" s="2">
+        <v>1.57</v>
+      </c>
+      <c r="K222" s="4">
+        <f t="shared" si="3"/>
+        <v>-157</v>
+      </c>
     </row>
     <row r="223" spans="1:12">
       <c r="A223" s="1">
         <v>44319</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C223" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D223">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E223" t="s">
         <v>6</v>
       </c>
       <c r="F223" s="1">
-        <v>44319</v>
+        <v>44321</v>
       </c>
       <c r="G223" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H223" s="3">
-        <v>4225</v>
+        <v>4145</v>
       </c>
       <c r="I223" s="2">
-        <v>1.34</v>
+        <v>3.71</v>
       </c>
       <c r="K223" s="4">
         <f t="shared" si="3"/>
-        <v>134</v>
-      </c>
+        <v>-371</v>
+      </c>
+      <c r="L223" s="6"/>
     </row>
     <row r="224" spans="1:12">
-      <c r="A224" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C224" t="s">
-        <v>4</v>
-      </c>
-      <c r="D224">
-        <v>100</v>
-      </c>
-      <c r="E224" t="s">
-        <v>6</v>
-      </c>
-      <c r="F224" s="1">
-        <v>44319</v>
-      </c>
-      <c r="G224" t="s">
-        <v>8</v>
-      </c>
-      <c r="H224" s="3">
-        <v>4180</v>
-      </c>
-      <c r="I224" s="2">
-        <v>1.05</v>
-      </c>
-      <c r="K224" s="4">
-        <f t="shared" si="3"/>
-        <v>105</v>
-      </c>
+      <c r="L224" s="6"/>
     </row>
     <row r="225" spans="1:13">
       <c r="A225" s="1">
@@ -6006,10 +6036,10 @@
         <v>91</v>
       </c>
       <c r="C225" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D225">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E225" t="s">
         <v>6</v>
@@ -6021,14 +6051,14 @@
         <v>23</v>
       </c>
       <c r="H225" s="3">
-        <v>4230</v>
+        <v>4225</v>
       </c>
       <c r="I225" s="2">
-        <v>0.72</v>
+        <v>1.34</v>
       </c>
       <c r="K225" s="4">
         <f t="shared" si="3"/>
-        <v>-72</v>
+        <v>134</v>
       </c>
     </row>
     <row r="226" spans="1:13">
@@ -6039,10 +6069,10 @@
         <v>91</v>
       </c>
       <c r="C226" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D226">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E226" t="s">
         <v>6</v>
@@ -6054,35 +6084,64 @@
         <v>8</v>
       </c>
       <c r="H226" s="3">
-        <v>4175</v>
+        <v>4180</v>
       </c>
       <c r="I226" s="2">
-        <v>0.77</v>
+        <v>1.05</v>
       </c>
       <c r="K226" s="4">
         <f t="shared" si="3"/>
-        <v>-77</v>
-      </c>
-      <c r="L226" s="6"/>
+        <v>105</v>
+      </c>
     </row>
     <row r="227" spans="1:13">
-      <c r="L227" s="6"/>
+      <c r="A227" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C227" t="s">
+        <v>10</v>
+      </c>
+      <c r="D227">
+        <v>-100</v>
+      </c>
+      <c r="E227" t="s">
+        <v>6</v>
+      </c>
+      <c r="F227" s="1">
+        <v>44319</v>
+      </c>
+      <c r="G227" t="s">
+        <v>23</v>
+      </c>
+      <c r="H227" s="3">
+        <v>4230</v>
+      </c>
+      <c r="I227" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="K227" s="4">
+        <f t="shared" si="3"/>
+        <v>-72</v>
+      </c>
     </row>
     <row r="228" spans="1:13">
       <c r="A228" s="1">
         <v>44319</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C228" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D228">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E228" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="F228" s="1">
         <v>44319</v>
@@ -6091,118 +6150,89 @@
         <v>8</v>
       </c>
       <c r="H228" s="3">
+        <v>4175</v>
+      </c>
+      <c r="I228" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K228" s="4">
+        <f t="shared" si="3"/>
+        <v>-77</v>
+      </c>
+      <c r="L228" s="6"/>
+    </row>
+    <row r="229" spans="1:13">
+      <c r="L229" s="6"/>
+    </row>
+    <row r="230" spans="1:13">
+      <c r="A230" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C230" t="s">
+        <v>4</v>
+      </c>
+      <c r="D230">
+        <v>100</v>
+      </c>
+      <c r="E230" t="s">
+        <v>36</v>
+      </c>
+      <c r="F230" s="1">
+        <v>44319</v>
+      </c>
+      <c r="G230" t="s">
+        <v>8</v>
+      </c>
+      <c r="H230" s="3">
         <v>2260</v>
       </c>
-      <c r="I228" s="2">
+      <c r="I230" s="2">
         <v>1.79</v>
       </c>
-      <c r="K228" s="4">
+      <c r="K230" s="4">
         <f t="shared" si="3"/>
         <v>179</v>
       </c>
-    </row>
-    <row r="229" spans="1:13">
-      <c r="A229" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C229" t="s">
-        <v>10</v>
-      </c>
-      <c r="D229">
-        <v>-100</v>
-      </c>
-      <c r="E229" t="s">
-        <v>36</v>
-      </c>
-      <c r="F229" s="1">
-        <v>44319</v>
-      </c>
-      <c r="G229" t="s">
-        <v>8</v>
-      </c>
-      <c r="H229" s="3">
-        <v>2250</v>
-      </c>
-      <c r="I229" s="2">
-        <v>0.84</v>
-      </c>
-      <c r="K229" s="4">
-        <f t="shared" si="3"/>
-        <v>-84</v>
-      </c>
-      <c r="L229" s="6"/>
-    </row>
-    <row r="230" spans="1:13">
-      <c r="L230" s="6"/>
     </row>
     <row r="231" spans="1:13">
       <c r="A231" s="1">
         <v>44319</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C231" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D231">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E231" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F231" s="1">
-        <v>44323</v>
+        <v>44319</v>
       </c>
       <c r="G231" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="H231" s="3">
-        <v>4265</v>
+        <v>2250</v>
       </c>
       <c r="I231" s="2">
-        <v>2.25</v>
+        <v>0.84</v>
       </c>
       <c r="K231" s="4">
         <f t="shared" si="3"/>
-        <v>225</v>
-      </c>
+        <v>-84</v>
+      </c>
+      <c r="L231" s="6"/>
     </row>
     <row r="232" spans="1:13">
-      <c r="A232" s="1">
-        <v>44319</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C232" t="s">
-        <v>4</v>
-      </c>
-      <c r="D232">
-        <v>100</v>
-      </c>
-      <c r="E232" t="s">
-        <v>6</v>
-      </c>
-      <c r="F232" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G232" t="s">
-        <v>8</v>
-      </c>
-      <c r="H232" s="3">
-        <v>4140</v>
-      </c>
-      <c r="I232" s="2">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="K232" s="4">
-        <f t="shared" si="3"/>
-        <v>1003.9999999999999</v>
-      </c>
+      <c r="L232" s="6"/>
     </row>
     <row r="233" spans="1:13">
       <c r="A233" s="1">
@@ -6212,10 +6242,10 @@
         <v>93</v>
       </c>
       <c r="C233" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D233">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E233" t="s">
         <v>6</v>
@@ -6227,14 +6257,14 @@
         <v>23</v>
       </c>
       <c r="H233" s="3">
-        <v>4270</v>
+        <v>4265</v>
       </c>
       <c r="I233" s="2">
-        <v>1.8</v>
+        <v>2.25</v>
       </c>
       <c r="K233" s="4">
         <f t="shared" si="3"/>
-        <v>-180</v>
+        <v>225</v>
       </c>
     </row>
     <row r="234" spans="1:13">
@@ -6245,10 +6275,10 @@
         <v>93</v>
       </c>
       <c r="C234" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D234">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E234" t="s">
         <v>6</v>
@@ -6260,26 +6290,55 @@
         <v>8</v>
       </c>
       <c r="H234" s="3">
-        <v>4135</v>
+        <v>4140</v>
       </c>
       <c r="I234" s="2">
-        <v>9.2899999999999991</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="K234" s="4">
         <f t="shared" si="3"/>
-        <v>-928.99999999999989</v>
-      </c>
-      <c r="L234" s="6"/>
+        <v>1003.9999999999999</v>
+      </c>
     </row>
     <row r="235" spans="1:13">
-      <c r="L235" s="6"/>
+      <c r="A235" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C235" t="s">
+        <v>10</v>
+      </c>
+      <c r="D235">
+        <v>-100</v>
+      </c>
+      <c r="E235" t="s">
+        <v>6</v>
+      </c>
+      <c r="F235" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G235" t="s">
+        <v>23</v>
+      </c>
+      <c r="H235" s="3">
+        <v>4270</v>
+      </c>
+      <c r="I235" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="K235" s="4">
+        <f t="shared" si="3"/>
+        <v>-180</v>
+      </c>
     </row>
     <row r="236" spans="1:13">
       <c r="A236" s="1">
         <v>44319</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C236" t="s">
         <v>10</v>
@@ -6288,28 +6347,35 @@
         <v>-100</v>
       </c>
       <c r="E236" t="s">
-        <v>95</v>
+        <v>6</v>
+      </c>
+      <c r="F236" s="1">
+        <v>44323</v>
       </c>
       <c r="G236" t="s">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="H236" s="3">
+        <v>4135</v>
       </c>
       <c r="I236" s="2">
-        <v>17.98</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="K236" s="4">
         <f t="shared" si="3"/>
-        <v>-1798</v>
-      </c>
-      <c r="M236" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>-928.99999999999989</v>
+      </c>
+      <c r="L236" s="6"/>
+    </row>
+    <row r="237" spans="1:13">
+      <c r="L237" s="6"/>
     </row>
     <row r="238" spans="1:13">
       <c r="A238" s="1">
         <v>44319</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C238" t="s">
         <v>10</v>
@@ -6318,17 +6384,17 @@
         <v>-100</v>
       </c>
       <c r="E238" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G238" t="s">
         <v>40</v>
       </c>
       <c r="I238" s="2">
-        <v>16.940000000000001</v>
+        <v>17.98</v>
       </c>
       <c r="K238" s="4">
         <f t="shared" si="3"/>
-        <v>-1694.0000000000002</v>
+        <v>-1798</v>
       </c>
       <c r="M238" s="5" t="s">
         <v>112</v>
@@ -6336,10 +6402,10 @@
     </row>
     <row r="240" spans="1:13">
       <c r="A240" s="1">
-        <v>44320</v>
+        <v>44319</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C240" t="s">
         <v>10</v>
@@ -6348,56 +6414,20 @@
         <v>-100</v>
       </c>
       <c r="E240" t="s">
-        <v>87</v>
-      </c>
-      <c r="F240" s="1">
-        <v>44321</v>
+        <v>97</v>
       </c>
       <c r="G240" t="s">
-        <v>23</v>
-      </c>
-      <c r="H240" s="3">
-        <v>13620</v>
+        <v>40</v>
       </c>
       <c r="I240" s="2">
-        <v>31.72</v>
+        <v>16.940000000000001</v>
       </c>
       <c r="K240" s="4">
         <f t="shared" si="3"/>
-        <v>-3172</v>
-      </c>
-    </row>
-    <row r="241" spans="1:13">
-      <c r="A241" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C241" t="s">
-        <v>10</v>
-      </c>
-      <c r="D241">
-        <v>-100</v>
-      </c>
-      <c r="E241" t="s">
-        <v>87</v>
-      </c>
-      <c r="F241" s="1">
-        <v>44321</v>
-      </c>
-      <c r="G241" t="s">
-        <v>23</v>
-      </c>
-      <c r="H241" s="3">
-        <v>14110</v>
-      </c>
-      <c r="I241" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="K241" s="4">
-        <f t="shared" si="3"/>
-        <v>-40</v>
+        <v>-1694.0000000000002</v>
+      </c>
+      <c r="M240" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="242" spans="1:13">
@@ -6408,10 +6438,10 @@
         <v>98</v>
       </c>
       <c r="C242" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D242">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E242" t="s">
         <v>87</v>
@@ -6423,14 +6453,14 @@
         <v>23</v>
       </c>
       <c r="H242" s="3">
-        <v>13600</v>
+        <v>13620</v>
       </c>
       <c r="I242" s="2">
-        <v>37.17</v>
+        <v>31.72</v>
       </c>
       <c r="K242" s="4">
         <f t="shared" si="3"/>
-        <v>3717</v>
+        <v>-3172</v>
       </c>
     </row>
     <row r="243" spans="1:13">
@@ -6441,10 +6471,10 @@
         <v>98</v>
       </c>
       <c r="C243" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D243">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E243" t="s">
         <v>87</v>
@@ -6456,29 +6486,55 @@
         <v>23</v>
       </c>
       <c r="H243" s="3">
-        <v>14130</v>
+        <v>14110</v>
       </c>
       <c r="I243" s="2">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="K243" s="4">
         <f t="shared" si="3"/>
-        <v>35</v>
-      </c>
-      <c r="L243" s="6"/>
-      <c r="M243" s="5" t="s">
-        <v>111</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="244" spans="1:13">
-      <c r="L244" s="6"/>
+      <c r="A244" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C244" t="s">
+        <v>4</v>
+      </c>
+      <c r="D244">
+        <v>100</v>
+      </c>
+      <c r="E244" t="s">
+        <v>87</v>
+      </c>
+      <c r="F244" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G244" t="s">
+        <v>23</v>
+      </c>
+      <c r="H244" s="3">
+        <v>13600</v>
+      </c>
+      <c r="I244" s="2">
+        <v>37.17</v>
+      </c>
+      <c r="K244" s="4">
+        <f t="shared" si="3"/>
+        <v>3717</v>
+      </c>
     </row>
     <row r="245" spans="1:13">
       <c r="A245" s="1">
         <v>44320</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C245" t="s">
         <v>4</v>
@@ -6490,54 +6546,27 @@
         <v>87</v>
       </c>
       <c r="F245" s="1">
-        <v>44323</v>
+        <v>44321</v>
       </c>
       <c r="G245" t="s">
         <v>23</v>
       </c>
       <c r="H245" s="3">
-        <v>13570</v>
+        <v>14130</v>
       </c>
       <c r="I245" s="2">
-        <v>84.53</v>
+        <v>0.35</v>
       </c>
       <c r="K245" s="4">
         <f t="shared" si="3"/>
-        <v>8453</v>
+        <v>35</v>
+      </c>
+      <c r="L245" s="6"/>
+      <c r="M245" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="246" spans="1:13">
-      <c r="A246" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C246" t="s">
-        <v>10</v>
-      </c>
-      <c r="D246">
-        <v>-100</v>
-      </c>
-      <c r="E246" t="s">
-        <v>87</v>
-      </c>
-      <c r="F246" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G246" t="s">
-        <v>23</v>
-      </c>
-      <c r="H246" s="3">
-        <v>13575</v>
-      </c>
-      <c r="I246" s="2">
-        <v>82.45</v>
-      </c>
-      <c r="K246" s="4">
-        <f t="shared" si="3"/>
-        <v>-8245</v>
-      </c>
       <c r="L246" s="6"/>
     </row>
     <row r="247" spans="1:13">
@@ -6548,10 +6577,10 @@
         <v>99</v>
       </c>
       <c r="C247" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D247">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E247" t="s">
         <v>87</v>
@@ -6563,14 +6592,14 @@
         <v>23</v>
       </c>
       <c r="H247" s="3">
-        <v>14190</v>
+        <v>13570</v>
       </c>
       <c r="I247" s="2">
-        <v>1.83</v>
+        <v>84.53</v>
       </c>
       <c r="K247" s="4">
         <f t="shared" si="3"/>
-        <v>-183</v>
+        <v>8453</v>
       </c>
     </row>
     <row r="248" spans="1:13">
@@ -6581,10 +6610,10 @@
         <v>99</v>
       </c>
       <c r="C248" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D248">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E248" t="s">
         <v>87</v>
@@ -6596,38 +6625,65 @@
         <v>23</v>
       </c>
       <c r="H248" s="3">
-        <v>14200</v>
+        <v>13575</v>
       </c>
       <c r="I248" s="2">
-        <v>1.75</v>
+        <v>82.45</v>
       </c>
       <c r="K248" s="4">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>-8245</v>
       </c>
       <c r="L248" s="6"/>
-      <c r="M248" s="5" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="249" spans="1:13">
-      <c r="L249" s="6"/>
+      <c r="A249" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C249" t="s">
+        <v>10</v>
+      </c>
+      <c r="D249">
+        <v>-100</v>
+      </c>
+      <c r="E249" t="s">
+        <v>87</v>
+      </c>
+      <c r="F249" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G249" t="s">
+        <v>23</v>
+      </c>
+      <c r="H249" s="3">
+        <v>14190</v>
+      </c>
+      <c r="I249" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="K249" s="4">
+        <f t="shared" si="3"/>
+        <v>-183</v>
+      </c>
     </row>
     <row r="250" spans="1:13">
       <c r="A250" s="1">
         <v>44320</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C250" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D250">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E250" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="F250" s="1">
         <v>44323</v>
@@ -6636,48 +6692,22 @@
         <v>23</v>
       </c>
       <c r="H250" s="3">
-        <v>720</v>
+        <v>14200</v>
       </c>
       <c r="I250" s="2">
         <v>1.75</v>
       </c>
       <c r="K250" s="4">
         <f t="shared" si="3"/>
-        <v>-175</v>
+        <v>175</v>
+      </c>
+      <c r="L250" s="6"/>
+      <c r="M250" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="251" spans="1:13">
-      <c r="A251" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C251" t="s">
-        <v>10</v>
-      </c>
-      <c r="D251">
-        <v>-100</v>
-      </c>
-      <c r="E251" t="s">
-        <v>48</v>
-      </c>
-      <c r="F251" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G251" t="s">
-        <v>8</v>
-      </c>
-      <c r="H251" s="3">
-        <v>720</v>
-      </c>
-      <c r="I251" s="2">
-        <v>61.29</v>
-      </c>
-      <c r="K251" s="4">
-        <f t="shared" si="3"/>
-        <v>-6129</v>
-      </c>
+      <c r="L251" s="6"/>
     </row>
     <row r="252" spans="1:13">
       <c r="A252" s="1">
@@ -6687,10 +6717,10 @@
         <v>100</v>
       </c>
       <c r="C252" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D252">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E252" t="s">
         <v>48</v>
@@ -6702,14 +6732,14 @@
         <v>23</v>
       </c>
       <c r="H252" s="3">
-        <v>722.5</v>
+        <v>720</v>
       </c>
       <c r="I252" s="2">
-        <v>1.56</v>
+        <v>1.75</v>
       </c>
       <c r="K252" s="4">
         <f t="shared" si="3"/>
-        <v>156</v>
+        <v>-175</v>
       </c>
     </row>
     <row r="253" spans="1:13">
@@ -6720,10 +6750,10 @@
         <v>100</v>
       </c>
       <c r="C253" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D253">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E253" t="s">
         <v>48</v>
@@ -6735,90 +6765,120 @@
         <v>8</v>
       </c>
       <c r="H253" s="3">
-        <v>717.5</v>
+        <v>720</v>
       </c>
       <c r="I253" s="2">
-        <v>58.95</v>
+        <v>61.29</v>
       </c>
       <c r="K253" s="4">
         <f t="shared" si="3"/>
-        <v>5895</v>
-      </c>
-      <c r="L253" s="6"/>
-      <c r="M253" s="5" t="s">
-        <v>110</v>
+        <v>-6129</v>
       </c>
     </row>
     <row r="254" spans="1:13">
-      <c r="L254" s="6"/>
+      <c r="A254" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C254" t="s">
+        <v>4</v>
+      </c>
+      <c r="D254">
+        <v>100</v>
+      </c>
+      <c r="E254" t="s">
+        <v>48</v>
+      </c>
+      <c r="F254" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G254" t="s">
+        <v>23</v>
+      </c>
+      <c r="H254" s="3">
+        <v>722.5</v>
+      </c>
+      <c r="I254" s="2">
+        <v>1.56</v>
+      </c>
+      <c r="K254" s="4">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
     </row>
     <row r="255" spans="1:13">
       <c r="A255" s="1">
         <v>44320</v>
       </c>
       <c r="B255" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C255" t="s">
+        <v>4</v>
+      </c>
+      <c r="D255">
+        <v>100</v>
+      </c>
+      <c r="E255" t="s">
+        <v>48</v>
+      </c>
+      <c r="F255" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G255" t="s">
+        <v>8</v>
+      </c>
+      <c r="H255" s="3">
+        <v>717.5</v>
+      </c>
+      <c r="I255" s="2">
+        <v>58.95</v>
+      </c>
+      <c r="K255" s="4">
+        <f t="shared" si="3"/>
+        <v>5895</v>
+      </c>
+      <c r="L255" s="6"/>
+      <c r="M255" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13">
+      <c r="L256" s="6"/>
+    </row>
+    <row r="257" spans="1:13">
+      <c r="A257" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B257" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C255" t="s">
-        <v>4</v>
-      </c>
-      <c r="D255">
-        <v>100</v>
-      </c>
-      <c r="E255" t="s">
+      <c r="C257" t="s">
+        <v>4</v>
+      </c>
+      <c r="D257">
+        <v>100</v>
+      </c>
+      <c r="E257" t="s">
         <v>43</v>
       </c>
-      <c r="F255" s="1">
+      <c r="F257" s="1">
         <v>44365</v>
       </c>
-      <c r="G255" t="s">
-        <v>8</v>
-      </c>
-      <c r="H255" s="3">
+      <c r="G257" t="s">
+        <v>8</v>
+      </c>
+      <c r="H257" s="3">
         <v>130</v>
       </c>
-      <c r="I255" s="2">
+      <c r="I257" s="2">
         <v>6.46</v>
       </c>
-      <c r="K255" s="4">
+      <c r="K257" s="4">
         <f t="shared" si="3"/>
         <v>646</v>
-      </c>
-    </row>
-    <row r="256" spans="1:13">
-      <c r="A256" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C256" t="s">
-        <v>10</v>
-      </c>
-      <c r="D256">
-        <v>-100</v>
-      </c>
-      <c r="E256" t="s">
-        <v>43</v>
-      </c>
-      <c r="F256" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G256" t="s">
-        <v>8</v>
-      </c>
-      <c r="H256" s="3">
-        <v>130</v>
-      </c>
-      <c r="I256" s="2">
-        <v>3.59</v>
-      </c>
-      <c r="K256" s="4">
-        <f t="shared" si="3"/>
-        <v>-359</v>
-      </c>
-      <c r="M256" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="258" spans="1:13">
@@ -6826,68 +6886,68 @@
         <v>44320</v>
       </c>
       <c r="B258" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C258" t="s">
+        <v>10</v>
+      </c>
+      <c r="D258">
+        <v>-100</v>
+      </c>
+      <c r="E258" t="s">
+        <v>43</v>
+      </c>
+      <c r="F258" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G258" t="s">
+        <v>8</v>
+      </c>
+      <c r="H258" s="3">
+        <v>130</v>
+      </c>
+      <c r="I258" s="2">
+        <v>3.59</v>
+      </c>
+      <c r="K258" s="4">
+        <f t="shared" si="3"/>
+        <v>-359</v>
+      </c>
+      <c r="M258" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13">
+      <c r="A260" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B260" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C258" t="s">
-        <v>10</v>
-      </c>
-      <c r="D258">
-        <v>-100</v>
-      </c>
-      <c r="E258" t="s">
+      <c r="C260" t="s">
+        <v>10</v>
+      </c>
+      <c r="D260">
+        <v>-100</v>
+      </c>
+      <c r="E260" t="s">
         <v>39</v>
       </c>
-      <c r="F258" s="1">
+      <c r="F260" s="1">
         <v>44351</v>
       </c>
-      <c r="G258" t="s">
-        <v>23</v>
-      </c>
-      <c r="H258" s="3">
+      <c r="G260" t="s">
+        <v>23</v>
+      </c>
+      <c r="H260" s="3">
         <v>61.5</v>
       </c>
-      <c r="I258" s="2">
+      <c r="I260" s="2">
         <v>0.26</v>
       </c>
-      <c r="K258" s="4">
+      <c r="K260" s="4">
         <f t="shared" si="3"/>
         <v>-26</v>
-      </c>
-    </row>
-    <row r="259" spans="1:13">
-      <c r="A259" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C259" t="s">
-        <v>4</v>
-      </c>
-      <c r="D259">
-        <v>100</v>
-      </c>
-      <c r="E259" t="s">
-        <v>39</v>
-      </c>
-      <c r="F259" s="1">
-        <v>44428</v>
-      </c>
-      <c r="G259" t="s">
-        <v>23</v>
-      </c>
-      <c r="H259" s="3">
-        <v>60</v>
-      </c>
-      <c r="I259" s="2">
-        <v>2</v>
-      </c>
-      <c r="K259" s="4">
-        <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="M259" s="5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="261" spans="1:13">
@@ -6895,65 +6955,35 @@
         <v>44320</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C261" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D261">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E261" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="F261" s="1">
-        <v>44321</v>
+        <v>44428</v>
       </c>
       <c r="G261" t="s">
         <v>23</v>
       </c>
       <c r="H261" s="3">
-        <v>4155</v>
+        <v>60</v>
       </c>
       <c r="I261" s="2">
-        <v>8.84</v>
+        <v>2</v>
       </c>
       <c r="K261" s="4">
         <f t="shared" si="3"/>
-        <v>-884</v>
-      </c>
-    </row>
-    <row r="262" spans="1:13">
-      <c r="A262" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C262" t="s">
-        <v>10</v>
-      </c>
-      <c r="D262">
-        <v>-100</v>
-      </c>
-      <c r="E262" t="s">
-        <v>6</v>
-      </c>
-      <c r="F262" s="1">
-        <v>44321</v>
-      </c>
-      <c r="G262" t="s">
-        <v>23</v>
-      </c>
-      <c r="H262" s="3">
-        <v>4250</v>
-      </c>
-      <c r="I262" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="K262" s="4">
-        <f t="shared" si="3"/>
-        <v>-12</v>
+        <v>200</v>
+      </c>
+      <c r="M261" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="263" spans="1:13">
@@ -6964,10 +6994,10 @@
         <v>103</v>
       </c>
       <c r="C263" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D263">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E263" t="s">
         <v>6</v>
@@ -6979,14 +7009,14 @@
         <v>23</v>
       </c>
       <c r="H263" s="3">
-        <v>4150</v>
+        <v>4155</v>
       </c>
       <c r="I263" s="2">
-        <v>10.59</v>
+        <v>8.84</v>
       </c>
       <c r="K263" s="4">
         <f t="shared" si="3"/>
-        <v>1059</v>
+        <v>-884</v>
       </c>
     </row>
     <row r="264" spans="1:13">
@@ -6997,10 +7027,10 @@
         <v>103</v>
       </c>
       <c r="C264" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D264">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E264" t="s">
         <v>6</v>
@@ -7012,62 +7042,89 @@
         <v>23</v>
       </c>
       <c r="H264" s="3">
-        <v>4255</v>
+        <v>4250</v>
       </c>
       <c r="I264" s="2">
         <v>0.12</v>
       </c>
       <c r="K264" s="4">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="L264" s="6"/>
+        <v>-12</v>
+      </c>
     </row>
     <row r="265" spans="1:13">
-      <c r="L265" s="6"/>
+      <c r="A265" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C265" t="s">
+        <v>4</v>
+      </c>
+      <c r="D265">
+        <v>100</v>
+      </c>
+      <c r="E265" t="s">
+        <v>6</v>
+      </c>
+      <c r="F265" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G265" t="s">
+        <v>23</v>
+      </c>
+      <c r="H265" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I265" s="2">
+        <v>10.59</v>
+      </c>
+      <c r="K265" s="4">
+        <f t="shared" si="3"/>
+        <v>1059</v>
+      </c>
     </row>
     <row r="266" spans="1:13">
       <c r="A266" s="1">
         <v>44320</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C266" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D266">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="E266" t="s">
         <v>6</v>
       </c>
       <c r="F266" s="1">
-        <v>44323</v>
+        <v>44321</v>
       </c>
       <c r="G266" t="s">
         <v>23</v>
       </c>
       <c r="H266" s="3">
-        <v>4145</v>
+        <v>4255</v>
       </c>
       <c r="I266" s="2">
-        <v>23.59</v>
+        <v>0.12</v>
       </c>
       <c r="K266" s="4">
         <f t="shared" si="3"/>
-        <v>-2359</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="L266" s="6"/>
     </row>
     <row r="267" spans="1:13">
       <c r="A267" s="1">
-        <v>44320</v>
+        <v>44321</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C267" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="D267">
         <v>-100</v>
@@ -7075,99 +7132,91 @@
       <c r="E267" t="s">
         <v>6</v>
       </c>
-      <c r="F267" s="1">
-        <v>44323</v>
-      </c>
       <c r="G267" t="s">
-        <v>23</v>
-      </c>
-      <c r="H267" s="3">
-        <v>4265</v>
+        <v>57</v>
+      </c>
+      <c r="H267" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="I267" s="2">
-        <v>0.3</v>
+        <v>4155</v>
       </c>
       <c r="K267" s="4">
-        <f t="shared" ref="K267:K280" si="4">D267*I267</f>
-        <v>-30</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>-415500</v>
+      </c>
+      <c r="L267" s="6"/>
     </row>
     <row r="268" spans="1:13">
       <c r="A268" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D268">
+        <v>100</v>
+      </c>
+      <c r="E268" t="s">
+        <v>6</v>
+      </c>
+      <c r="G268" t="s">
+        <v>57</v>
+      </c>
+      <c r="H268" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I268" s="2">
+        <v>4150</v>
+      </c>
+      <c r="K268" s="4">
+        <f t="shared" si="3"/>
+        <v>415000</v>
+      </c>
+      <c r="L268" s="6"/>
+    </row>
+    <row r="269" spans="1:13">
+      <c r="L269" s="6"/>
+    </row>
+    <row r="270" spans="1:13">
+      <c r="A270" s="1">
         <v>44320</v>
       </c>
-      <c r="B268" s="1" t="s">
+      <c r="B270" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C268" t="s">
-        <v>4</v>
-      </c>
-      <c r="D268">
-        <v>100</v>
-      </c>
-      <c r="E268" t="s">
-        <v>6</v>
-      </c>
-      <c r="F268" s="1">
+      <c r="C270" t="s">
+        <v>10</v>
+      </c>
+      <c r="D270">
+        <v>-100</v>
+      </c>
+      <c r="E270" t="s">
+        <v>6</v>
+      </c>
+      <c r="F270" s="1">
         <v>44323</v>
       </c>
-      <c r="G268" t="s">
-        <v>23</v>
-      </c>
-      <c r="H268" s="3">
-        <v>4140</v>
-      </c>
-      <c r="I268" s="2">
-        <v>26.29</v>
-      </c>
-      <c r="K268" s="4">
-        <f t="shared" si="4"/>
-        <v>2629</v>
-      </c>
-    </row>
-    <row r="269" spans="1:13">
-      <c r="A269" s="1">
-        <v>44320</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C269" t="s">
-        <v>4</v>
-      </c>
-      <c r="D269">
-        <v>100</v>
-      </c>
-      <c r="E269" t="s">
-        <v>6</v>
-      </c>
-      <c r="F269" s="1">
-        <v>44323</v>
-      </c>
-      <c r="G269" t="s">
-        <v>23</v>
-      </c>
-      <c r="H269" s="3">
-        <v>4270</v>
-      </c>
-      <c r="I269" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="K269" s="4">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="L269" s="6"/>
-    </row>
-    <row r="270" spans="1:13">
-      <c r="L270" s="6"/>
+      <c r="G270" t="s">
+        <v>23</v>
+      </c>
+      <c r="H270" s="3">
+        <v>4145</v>
+      </c>
+      <c r="I270" s="2">
+        <v>23.59</v>
+      </c>
+      <c r="K270" s="4">
+        <f t="shared" si="3"/>
+        <v>-2359</v>
+      </c>
     </row>
     <row r="271" spans="1:13">
       <c r="A271" s="1">
         <v>44320</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C271" t="s">
         <v>10</v>
@@ -7176,23 +7225,23 @@
         <v>-100</v>
       </c>
       <c r="E271" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F271" s="1">
         <v>44323</v>
       </c>
       <c r="G271" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H271" s="3">
-        <v>252.5</v>
+        <v>4265</v>
       </c>
       <c r="I271" s="2">
-        <v>6.82</v>
+        <v>0.3</v>
       </c>
       <c r="K271" s="4">
-        <f t="shared" si="4"/>
-        <v>-682</v>
+        <f t="shared" ref="K271:K284" si="4">D271*I271</f>
+        <v>-30</v>
       </c>
     </row>
     <row r="272" spans="1:13">
@@ -7200,7 +7249,7 @@
         <v>44320</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C272" t="s">
         <v>4</v>
@@ -7209,227 +7258,1825 @@
         <v>100</v>
       </c>
       <c r="E272" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F272" s="1">
         <v>44323</v>
       </c>
       <c r="G272" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="H272" s="3">
-        <v>250</v>
+        <v>4140</v>
       </c>
       <c r="I272" s="2">
-        <v>4.82</v>
+        <v>26.29</v>
       </c>
       <c r="K272" s="4">
         <f t="shared" si="4"/>
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13">
+      <c r="A273" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C273" t="s">
+        <v>4</v>
+      </c>
+      <c r="D273">
+        <v>100</v>
+      </c>
+      <c r="E273" t="s">
+        <v>6</v>
+      </c>
+      <c r="F273" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G273" t="s">
+        <v>23</v>
+      </c>
+      <c r="H273" s="3">
+        <v>4270</v>
+      </c>
+      <c r="I273" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="K273" s="4">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="L273" s="6"/>
+    </row>
+    <row r="274" spans="1:13">
+      <c r="L274" s="6"/>
+    </row>
+    <row r="275" spans="1:13">
+      <c r="A275" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C275" t="s">
+        <v>10</v>
+      </c>
+      <c r="D275">
+        <v>-100</v>
+      </c>
+      <c r="E275" t="s">
+        <v>20</v>
+      </c>
+      <c r="F275" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G275" t="s">
+        <v>8</v>
+      </c>
+      <c r="H275" s="3">
+        <v>252.5</v>
+      </c>
+      <c r="I275" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="K275" s="4">
+        <f t="shared" si="4"/>
+        <v>-682</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13">
+      <c r="A276" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C276" t="s">
+        <v>4</v>
+      </c>
+      <c r="D276">
+        <v>100</v>
+      </c>
+      <c r="E276" t="s">
+        <v>20</v>
+      </c>
+      <c r="F276" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G276" t="s">
+        <v>8</v>
+      </c>
+      <c r="H276" s="3">
+        <v>250</v>
+      </c>
+      <c r="I276" s="2">
+        <v>4.82</v>
+      </c>
+      <c r="K276" s="4">
+        <f t="shared" si="4"/>
         <v>482</v>
       </c>
-      <c r="L272" s="6"/>
-    </row>
-    <row r="273" spans="1:12">
-      <c r="L273" s="6"/>
-    </row>
-    <row r="274" spans="1:12">
-      <c r="A274" s="1">
+      <c r="L276" s="6"/>
+    </row>
+    <row r="277" spans="1:13">
+      <c r="L277" s="6"/>
+    </row>
+    <row r="278" spans="1:13">
+      <c r="A278" s="1">
         <v>44320</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="B278" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C274" t="s">
-        <v>10</v>
-      </c>
-      <c r="D274">
-        <v>-100</v>
-      </c>
-      <c r="E274" t="s">
+      <c r="C278" t="s">
+        <v>10</v>
+      </c>
+      <c r="D278">
+        <v>-100</v>
+      </c>
+      <c r="E278" t="s">
         <v>20</v>
       </c>
-      <c r="F274" s="1">
+      <c r="F278" s="1">
         <v>44323</v>
       </c>
-      <c r="G274" t="s">
-        <v>23</v>
-      </c>
-      <c r="H274" s="3">
+      <c r="G278" t="s">
+        <v>23</v>
+      </c>
+      <c r="H278" s="3">
         <v>257.5</v>
       </c>
-      <c r="I274" s="2">
+      <c r="I278" s="2">
         <v>0.13</v>
       </c>
-      <c r="K274" s="4">
+      <c r="K278" s="4">
         <f t="shared" si="4"/>
         <v>-13</v>
       </c>
     </row>
-    <row r="275" spans="1:12">
-      <c r="A275" s="1">
+    <row r="279" spans="1:13">
+      <c r="A279" s="1">
         <v>44320</v>
       </c>
-      <c r="B275" s="1" t="s">
+      <c r="B279" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C275" t="s">
-        <v>10</v>
-      </c>
-      <c r="D275">
-        <v>-100</v>
-      </c>
-      <c r="E275" t="s">
+      <c r="C279" t="s">
+        <v>10</v>
+      </c>
+      <c r="D279">
+        <v>-100</v>
+      </c>
+      <c r="E279" t="s">
         <v>20</v>
       </c>
-      <c r="F275" s="1">
+      <c r="F279" s="1">
         <v>44323</v>
       </c>
-      <c r="G275" t="s">
-        <v>23</v>
-      </c>
-      <c r="H275" s="3">
+      <c r="G279" t="s">
+        <v>23</v>
+      </c>
+      <c r="H279" s="3">
         <v>260</v>
       </c>
-      <c r="I275" s="2">
+      <c r="I279" s="2">
         <v>0.08</v>
       </c>
-      <c r="K275" s="4">
+      <c r="K279" s="4">
         <f t="shared" si="4"/>
         <v>-8</v>
       </c>
     </row>
-    <row r="276" spans="1:12">
-      <c r="A276" s="1">
+    <row r="280" spans="1:13">
+      <c r="A280" s="1">
         <v>44320</v>
       </c>
-      <c r="B276" s="1" t="s">
+      <c r="B280" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C276" t="s">
-        <v>4</v>
-      </c>
-      <c r="D276">
-        <v>100</v>
-      </c>
-      <c r="E276" t="s">
+      <c r="C280" t="s">
+        <v>4</v>
+      </c>
+      <c r="D280">
+        <v>100</v>
+      </c>
+      <c r="E280" t="s">
         <v>20</v>
       </c>
-      <c r="F276" s="1">
+      <c r="F280" s="1">
         <v>44323</v>
       </c>
-      <c r="G276" t="s">
-        <v>23</v>
-      </c>
-      <c r="H276" s="3">
+      <c r="G280" t="s">
+        <v>23</v>
+      </c>
+      <c r="H280" s="3">
         <v>255</v>
       </c>
-      <c r="I276" s="2">
+      <c r="I280" s="2">
         <v>0.22</v>
       </c>
-      <c r="K276" s="4">
+      <c r="K280" s="4">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
     </row>
-    <row r="277" spans="1:12">
-      <c r="A277" s="1">
+    <row r="281" spans="1:13">
+      <c r="A281" s="1">
         <v>44320</v>
       </c>
-      <c r="B277" s="1" t="s">
+      <c r="B281" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C277" t="s">
-        <v>4</v>
-      </c>
-      <c r="D277">
-        <v>100</v>
-      </c>
-      <c r="E277" t="s">
+      <c r="C281" t="s">
+        <v>4</v>
+      </c>
+      <c r="D281">
+        <v>100</v>
+      </c>
+      <c r="E281" t="s">
         <v>20</v>
       </c>
-      <c r="F277" s="1">
+      <c r="F281" s="1">
         <v>44323</v>
       </c>
-      <c r="G277" t="s">
-        <v>23</v>
-      </c>
-      <c r="H277" s="3">
+      <c r="G281" t="s">
+        <v>23</v>
+      </c>
+      <c r="H281" s="3">
         <v>262.5</v>
       </c>
-      <c r="I277" s="2">
+      <c r="I281" s="2">
         <v>0.05</v>
       </c>
-      <c r="K277" s="4">
+      <c r="K281" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:12">
-      <c r="A279" s="1">
+    <row r="283" spans="1:13">
+      <c r="A283" s="1">
         <v>44320</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B283" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C279" t="s">
-        <v>10</v>
-      </c>
-      <c r="D279">
-        <v>-100</v>
-      </c>
-      <c r="E279" t="s">
+      <c r="C283" t="s">
+        <v>10</v>
+      </c>
+      <c r="D283">
+        <v>-100</v>
+      </c>
+      <c r="E283" t="s">
         <v>87</v>
       </c>
-      <c r="F279" s="1">
+      <c r="F283" s="1">
         <v>44323</v>
       </c>
-      <c r="G279" t="s">
-        <v>8</v>
-      </c>
-      <c r="H279" s="3">
+      <c r="G283" t="s">
+        <v>8</v>
+      </c>
+      <c r="H283" s="3">
         <v>13560</v>
       </c>
-      <c r="I279" s="2">
+      <c r="I283" s="2">
         <v>185.89</v>
       </c>
-      <c r="K279" s="4">
+      <c r="K283" s="4">
         <f t="shared" si="4"/>
         <v>-18589</v>
       </c>
     </row>
-    <row r="280" spans="1:12">
-      <c r="A280" s="1">
+    <row r="284" spans="1:13">
+      <c r="A284" s="1">
         <v>44320</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="B284" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C280" t="s">
-        <v>4</v>
-      </c>
-      <c r="D280">
-        <v>100</v>
-      </c>
-      <c r="E280" t="s">
+      <c r="C284" t="s">
+        <v>4</v>
+      </c>
+      <c r="D284">
+        <v>100</v>
+      </c>
+      <c r="E284" t="s">
         <v>87</v>
       </c>
-      <c r="F280" s="1">
+      <c r="F284" s="1">
         <v>44323</v>
       </c>
-      <c r="G280" t="s">
-        <v>8</v>
-      </c>
-      <c r="H280" s="3">
+      <c r="G284" t="s">
+        <v>8</v>
+      </c>
+      <c r="H284" s="3">
         <v>13540</v>
       </c>
-      <c r="I280" s="2">
+      <c r="I284" s="2">
         <v>174.65</v>
       </c>
-      <c r="K280" s="4">
+      <c r="K284" s="4">
         <f t="shared" si="4"/>
         <v>17465</v>
       </c>
-      <c r="L280" s="6"/>
+      <c r="L284" s="6"/>
+    </row>
+    <row r="286" spans="1:13">
+      <c r="A286" s="7"/>
+      <c r="B286" s="7"/>
+      <c r="C286" s="8"/>
+      <c r="D286" s="8"/>
+      <c r="E286" s="8"/>
+      <c r="F286" s="7"/>
+      <c r="G286" s="8"/>
+      <c r="H286" s="9"/>
+      <c r="I286" s="10"/>
+      <c r="J286" s="8"/>
+      <c r="K286" s="11"/>
+      <c r="L286" s="8"/>
+      <c r="M286" s="12"/>
+    </row>
+    <row r="287" spans="1:13">
+      <c r="A287" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C287" t="s">
+        <v>10</v>
+      </c>
+      <c r="D287">
+        <v>-100</v>
+      </c>
+      <c r="E287" t="s">
+        <v>87</v>
+      </c>
+      <c r="F287" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G287" t="s">
+        <v>23</v>
+      </c>
+      <c r="H287" s="3">
+        <v>13610</v>
+      </c>
+      <c r="I287" s="2">
+        <v>47.1</v>
+      </c>
+      <c r="K287" s="4">
+        <f t="shared" ref="K287:K333" si="5">D287*I287</f>
+        <v>-4710</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12">
+      <c r="A289" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C289" t="s">
+        <v>10</v>
+      </c>
+      <c r="D289">
+        <v>-100</v>
+      </c>
+      <c r="E289" t="s">
+        <v>87</v>
+      </c>
+      <c r="F289" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G289" t="s">
+        <v>23</v>
+      </c>
+      <c r="H289" s="3">
+        <v>13600</v>
+      </c>
+      <c r="I289" s="2">
+        <v>24.1</v>
+      </c>
+      <c r="K289" s="4">
+        <f t="shared" si="5"/>
+        <v>-2410</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12">
+      <c r="A290" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C290" t="s">
+        <v>4</v>
+      </c>
+      <c r="D290">
+        <v>100</v>
+      </c>
+      <c r="E290" t="s">
+        <v>87</v>
+      </c>
+      <c r="F290" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G290" t="s">
+        <v>23</v>
+      </c>
+      <c r="H290" s="3">
+        <v>13620</v>
+      </c>
+      <c r="I290" s="2">
+        <v>17.7</v>
+      </c>
+      <c r="K290" s="4">
+        <f t="shared" si="5"/>
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12">
+      <c r="A291" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C291" t="s">
+        <v>4</v>
+      </c>
+      <c r="D291">
+        <v>100</v>
+      </c>
+      <c r="E291" t="s">
+        <v>87</v>
+      </c>
+      <c r="F291" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G291" t="s">
+        <v>23</v>
+      </c>
+      <c r="H291" s="3">
+        <v>13600</v>
+      </c>
+      <c r="I291" s="2">
+        <v>28.3</v>
+      </c>
+      <c r="K291" s="4">
+        <f t="shared" si="5"/>
+        <v>2830</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12">
+      <c r="A292" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C292" t="s">
+        <v>10</v>
+      </c>
+      <c r="D292">
+        <v>-100</v>
+      </c>
+      <c r="E292" t="s">
+        <v>87</v>
+      </c>
+      <c r="F292" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G292" t="s">
+        <v>8</v>
+      </c>
+      <c r="H292" s="3">
+        <v>13590</v>
+      </c>
+      <c r="I292" s="2">
+        <v>54.8</v>
+      </c>
+      <c r="K292" s="4">
+        <f t="shared" si="5"/>
+        <v>-5480</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12">
+      <c r="A293" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C293" t="s">
+        <v>4</v>
+      </c>
+      <c r="D293">
+        <v>100</v>
+      </c>
+      <c r="E293" t="s">
+        <v>87</v>
+      </c>
+      <c r="F293" s="1">
+        <v>44321</v>
+      </c>
+      <c r="G293" t="s">
+        <v>8</v>
+      </c>
+      <c r="H293" s="3">
+        <v>13575</v>
+      </c>
+      <c r="I293" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="K293" s="4">
+        <f t="shared" si="5"/>
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12">
+      <c r="A294" s="1">
+        <v>44321</v>
+      </c>
+      <c r="D294">
+        <v>100</v>
+      </c>
+      <c r="E294" t="s">
+        <v>87</v>
+      </c>
+      <c r="G294" t="s">
+        <v>57</v>
+      </c>
+      <c r="H294" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I294" s="2">
+        <v>13590</v>
+      </c>
+      <c r="K294" s="4">
+        <f t="shared" si="5"/>
+        <v>1359000</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12">
+      <c r="A296" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C296" t="s">
+        <v>10</v>
+      </c>
+      <c r="D296">
+        <v>-100</v>
+      </c>
+      <c r="E296" t="s">
+        <v>87</v>
+      </c>
+      <c r="F296" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G296" t="s">
+        <v>23</v>
+      </c>
+      <c r="H296" s="3">
+        <v>13570</v>
+      </c>
+      <c r="I296" s="2">
+        <v>123</v>
+      </c>
+      <c r="K296" s="4">
+        <f t="shared" si="5"/>
+        <v>-12300</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12">
+      <c r="A297" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C297" t="s">
+        <v>4</v>
+      </c>
+      <c r="D297">
+        <v>100</v>
+      </c>
+      <c r="E297" t="s">
+        <v>87</v>
+      </c>
+      <c r="F297" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G297" t="s">
+        <v>23</v>
+      </c>
+      <c r="H297" s="3">
+        <v>13575</v>
+      </c>
+      <c r="I297" s="2">
+        <v>119.5</v>
+      </c>
+      <c r="K297" s="4">
+        <f t="shared" si="5"/>
+        <v>11950</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12">
+      <c r="A298" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C298" t="s">
+        <v>10</v>
+      </c>
+      <c r="D298">
+        <v>-100</v>
+      </c>
+      <c r="E298" t="s">
+        <v>87</v>
+      </c>
+      <c r="F298" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G298" t="s">
+        <v>8</v>
+      </c>
+      <c r="H298" s="3">
+        <v>13570</v>
+      </c>
+      <c r="I298" s="2">
+        <v>63.45</v>
+      </c>
+      <c r="K298" s="4">
+        <f t="shared" si="5"/>
+        <v>-6345</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12">
+      <c r="A299" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C299" t="s">
+        <v>4</v>
+      </c>
+      <c r="D299">
+        <v>100</v>
+      </c>
+      <c r="E299" t="s">
+        <v>87</v>
+      </c>
+      <c r="F299" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G299" t="s">
+        <v>8</v>
+      </c>
+      <c r="H299" s="3">
+        <v>13560</v>
+      </c>
+      <c r="I299" s="2">
+        <v>60.15</v>
+      </c>
+      <c r="K299" s="4">
+        <f t="shared" si="5"/>
+        <v>6015</v>
+      </c>
+      <c r="L299" s="6"/>
+    </row>
+    <row r="300" spans="1:12">
+      <c r="A300" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C300" t="s">
+        <v>10</v>
+      </c>
+      <c r="D300">
+        <v>-100</v>
+      </c>
+      <c r="E300" t="s">
+        <v>36</v>
+      </c>
+      <c r="F300" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G300" t="s">
+        <v>8</v>
+      </c>
+      <c r="H300" s="3">
+        <v>2215</v>
+      </c>
+      <c r="I300" s="2">
+        <v>12.88</v>
+      </c>
+      <c r="K300" s="4">
+        <f t="shared" si="5"/>
+        <v>-1288</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12">
+      <c r="A301" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C301" t="s">
+        <v>10</v>
+      </c>
+      <c r="D301">
+        <v>-100</v>
+      </c>
+      <c r="E301" t="s">
+        <v>36</v>
+      </c>
+      <c r="F301" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G301" t="s">
+        <v>23</v>
+      </c>
+      <c r="H301" s="3">
+        <v>2285</v>
+      </c>
+      <c r="I301" s="2">
+        <v>2.87</v>
+      </c>
+      <c r="K301" s="4">
+        <f t="shared" si="5"/>
+        <v>-287</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12">
+      <c r="A302" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C302" t="s">
+        <v>4</v>
+      </c>
+      <c r="D302">
+        <v>100</v>
+      </c>
+      <c r="E302" t="s">
+        <v>36</v>
+      </c>
+      <c r="F302" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G302" t="s">
+        <v>8</v>
+      </c>
+      <c r="H302" s="3">
+        <v>2220</v>
+      </c>
+      <c r="I302" s="2">
+        <v>14.69</v>
+      </c>
+      <c r="K302" s="4">
+        <f t="shared" si="5"/>
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12">
+      <c r="A303" s="1">
+        <v>44321</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C303" t="s">
+        <v>4</v>
+      </c>
+      <c r="D303">
+        <v>100</v>
+      </c>
+      <c r="E303" t="s">
+        <v>36</v>
+      </c>
+      <c r="F303" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G303" t="s">
+        <v>23</v>
+      </c>
+      <c r="H303" s="3">
+        <v>2280</v>
+      </c>
+      <c r="I303" s="2">
+        <v>3.56</v>
+      </c>
+      <c r="K303" s="4">
+        <f t="shared" si="5"/>
+        <v>356</v>
+      </c>
+      <c r="L303" s="6"/>
+    </row>
+    <row r="304" spans="1:12">
+      <c r="A304" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C304" t="s">
+        <v>10</v>
+      </c>
+      <c r="D304">
+        <v>-100</v>
+      </c>
+      <c r="E304" t="s">
+        <v>36</v>
+      </c>
+      <c r="F304" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G304" t="s">
+        <v>23</v>
+      </c>
+      <c r="H304" s="3">
+        <v>2255</v>
+      </c>
+      <c r="I304" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K304" s="4">
+        <f t="shared" si="5"/>
+        <v>-229.99999999999997</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12">
+      <c r="A305" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C305" t="s">
+        <v>4</v>
+      </c>
+      <c r="D305">
+        <v>100</v>
+      </c>
+      <c r="E305" t="s">
+        <v>36</v>
+      </c>
+      <c r="F305" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G305" t="s">
+        <v>23</v>
+      </c>
+      <c r="H305" s="3">
+        <v>2260</v>
+      </c>
+      <c r="I305" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="K305" s="4">
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12">
+      <c r="A306" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C306" t="s">
+        <v>10</v>
+      </c>
+      <c r="D306">
+        <v>-100</v>
+      </c>
+      <c r="E306" t="s">
+        <v>36</v>
+      </c>
+      <c r="F306" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G306" t="s">
+        <v>8</v>
+      </c>
+      <c r="H306" s="3">
+        <v>2220</v>
+      </c>
+      <c r="I306" s="2">
+        <v>20.18</v>
+      </c>
+      <c r="K306" s="4">
+        <f t="shared" si="5"/>
+        <v>-2018</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12">
+      <c r="A307" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C307" t="s">
+        <v>4</v>
+      </c>
+      <c r="D307">
+        <v>100</v>
+      </c>
+      <c r="E307" t="s">
+        <v>36</v>
+      </c>
+      <c r="F307" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G307" t="s">
+        <v>8</v>
+      </c>
+      <c r="H307" s="3">
+        <v>2215</v>
+      </c>
+      <c r="I307" s="2">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="K307" s="4">
+        <f t="shared" si="5"/>
+        <v>1757.9999999999998</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12">
+      <c r="A308" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C308" t="s">
+        <v>10</v>
+      </c>
+      <c r="D308">
+        <v>-100</v>
+      </c>
+      <c r="E308" t="s">
+        <v>36</v>
+      </c>
+      <c r="F308" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G308" t="s">
+        <v>23</v>
+      </c>
+      <c r="H308" s="3">
+        <v>2275</v>
+      </c>
+      <c r="I308" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="K308" s="4">
+        <f t="shared" si="5"/>
+        <v>-71</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12">
+      <c r="A309" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C309" t="s">
+        <v>10</v>
+      </c>
+      <c r="D309">
+        <v>-100</v>
+      </c>
+      <c r="E309" t="s">
+        <v>36</v>
+      </c>
+      <c r="F309" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G309" t="s">
+        <v>23</v>
+      </c>
+      <c r="H309" s="3">
+        <v>2280</v>
+      </c>
+      <c r="I309" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K309" s="4">
+        <f t="shared" si="5"/>
+        <v>-57.999999999999993</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12">
+      <c r="A310" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C310" t="s">
+        <v>4</v>
+      </c>
+      <c r="D310">
+        <v>100</v>
+      </c>
+      <c r="E310" t="s">
+        <v>36</v>
+      </c>
+      <c r="F310" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G310" t="s">
+        <v>23</v>
+      </c>
+      <c r="H310" s="3">
+        <v>2270</v>
+      </c>
+      <c r="I310" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K310" s="4">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12">
+      <c r="A311" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C311" t="s">
+        <v>4</v>
+      </c>
+      <c r="D311">
+        <v>100</v>
+      </c>
+      <c r="E311" t="s">
+        <v>36</v>
+      </c>
+      <c r="F311" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G311" t="s">
+        <v>23</v>
+      </c>
+      <c r="H311" s="3">
+        <v>2285</v>
+      </c>
+      <c r="I311" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="K311" s="4">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12">
+      <c r="A312" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C312" t="s">
+        <v>10</v>
+      </c>
+      <c r="D312">
+        <v>-100</v>
+      </c>
+      <c r="E312" t="s">
+        <v>36</v>
+      </c>
+      <c r="F312" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G312" t="s">
+        <v>8</v>
+      </c>
+      <c r="H312" s="3">
+        <v>2190</v>
+      </c>
+      <c r="I312" s="2">
+        <v>13.03</v>
+      </c>
+      <c r="K312" s="4">
+        <f t="shared" si="5"/>
+        <v>-1303</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12">
+      <c r="A313" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C313" t="s">
+        <v>10</v>
+      </c>
+      <c r="D313">
+        <v>-100</v>
+      </c>
+      <c r="E313" t="s">
+        <v>36</v>
+      </c>
+      <c r="F313" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G313" t="s">
+        <v>23</v>
+      </c>
+      <c r="H313" s="3">
+        <v>2225</v>
+      </c>
+      <c r="I313" s="2">
+        <v>15.83</v>
+      </c>
+      <c r="K313" s="4">
+        <f t="shared" si="5"/>
+        <v>-1583</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12">
+      <c r="A314" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C314" t="s">
+        <v>4</v>
+      </c>
+      <c r="D314">
+        <v>100</v>
+      </c>
+      <c r="E314" t="s">
+        <v>36</v>
+      </c>
+      <c r="F314" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G314" t="s">
+        <v>8</v>
+      </c>
+      <c r="H314" s="3">
+        <v>2195</v>
+      </c>
+      <c r="I314" s="2">
+        <v>14.61</v>
+      </c>
+      <c r="K314" s="4">
+        <f t="shared" si="5"/>
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12">
+      <c r="A315" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C315" t="s">
+        <v>4</v>
+      </c>
+      <c r="D315">
+        <v>100</v>
+      </c>
+      <c r="E315" t="s">
+        <v>36</v>
+      </c>
+      <c r="F315" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G315" t="s">
+        <v>23</v>
+      </c>
+      <c r="H315" s="3">
+        <v>2220</v>
+      </c>
+      <c r="I315" s="2">
+        <v>18.25</v>
+      </c>
+      <c r="K315" s="4">
+        <f t="shared" si="5"/>
+        <v>1825</v>
+      </c>
+      <c r="L315" s="6"/>
+    </row>
+    <row r="316" spans="1:12">
+      <c r="A316" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C316" t="s">
+        <v>10</v>
+      </c>
+      <c r="D316">
+        <v>-100</v>
+      </c>
+      <c r="E316" t="s">
+        <v>6</v>
+      </c>
+      <c r="F316" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G316" t="s">
+        <v>8</v>
+      </c>
+      <c r="H316" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I316" s="2">
+        <v>10.65</v>
+      </c>
+      <c r="K316" s="4">
+        <f t="shared" si="5"/>
+        <v>-1065</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12">
+      <c r="A317" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C317" t="s">
+        <v>10</v>
+      </c>
+      <c r="D317">
+        <v>-100</v>
+      </c>
+      <c r="E317" t="s">
+        <v>6</v>
+      </c>
+      <c r="F317" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G317" t="s">
+        <v>23</v>
+      </c>
+      <c r="H317" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I317" s="2">
+        <v>22</v>
+      </c>
+      <c r="K317" s="4">
+        <f t="shared" si="5"/>
+        <v>-2200</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12">
+      <c r="A318" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C318" t="s">
+        <v>4</v>
+      </c>
+      <c r="D318">
+        <v>100</v>
+      </c>
+      <c r="E318" t="s">
+        <v>6</v>
+      </c>
+      <c r="F318" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G318" t="s">
+        <v>8</v>
+      </c>
+      <c r="H318" s="3">
+        <v>4145</v>
+      </c>
+      <c r="I318" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="K318" s="4">
+        <f t="shared" si="5"/>
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12">
+      <c r="A319" s="1">
+        <v>44322</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C319" t="s">
+        <v>4</v>
+      </c>
+      <c r="D319">
+        <v>100</v>
+      </c>
+      <c r="E319" t="s">
+        <v>6</v>
+      </c>
+      <c r="F319" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G319" t="s">
+        <v>23</v>
+      </c>
+      <c r="H319" s="3">
+        <v>4165</v>
+      </c>
+      <c r="I319" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="K319" s="4">
+        <f t="shared" si="5"/>
+        <v>2510</v>
+      </c>
+      <c r="L319" s="6"/>
+    </row>
+    <row r="320" spans="1:12">
+      <c r="A320" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C320" t="s">
+        <v>10</v>
+      </c>
+      <c r="D320">
+        <v>-100</v>
+      </c>
+      <c r="E320" t="s">
+        <v>20</v>
+      </c>
+      <c r="F320" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G320" t="s">
+        <v>23</v>
+      </c>
+      <c r="H320" s="3">
+        <v>255</v>
+      </c>
+      <c r="I320" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="K320" s="4">
+        <f t="shared" si="5"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11">
+      <c r="A321" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C321" t="s">
+        <v>4</v>
+      </c>
+      <c r="D321">
+        <v>100</v>
+      </c>
+      <c r="E321" t="s">
+        <v>20</v>
+      </c>
+      <c r="F321" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G321" t="s">
+        <v>23</v>
+      </c>
+      <c r="H321" s="3">
+        <v>257.5</v>
+      </c>
+      <c r="I321" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="K321" s="4">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11">
+      <c r="A322" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C322" t="s">
+        <v>4</v>
+      </c>
+      <c r="D322">
+        <v>100</v>
+      </c>
+      <c r="E322" t="s">
+        <v>20</v>
+      </c>
+      <c r="F322" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G322" t="s">
+        <v>8</v>
+      </c>
+      <c r="H322" s="3">
+        <v>252.5</v>
+      </c>
+      <c r="I322" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="K322" s="4">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11">
+      <c r="A323" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C323" t="s">
+        <v>10</v>
+      </c>
+      <c r="D323">
+        <v>-100</v>
+      </c>
+      <c r="E323" t="s">
+        <v>20</v>
+      </c>
+      <c r="F323" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G323" t="s">
+        <v>8</v>
+      </c>
+      <c r="H323" s="3">
+        <v>255</v>
+      </c>
+      <c r="I323" s="2">
+        <v>2.88</v>
+      </c>
+      <c r="K323" s="4">
+        <f t="shared" si="5"/>
+        <v>-288</v>
+      </c>
+    </row>
+    <row r="324" spans="1:11">
+      <c r="A324" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C324" t="s">
+        <v>4</v>
+      </c>
+      <c r="D324">
+        <v>100</v>
+      </c>
+      <c r="E324" t="s">
+        <v>43</v>
+      </c>
+      <c r="F324" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G324" t="s">
+        <v>8</v>
+      </c>
+      <c r="H324" s="3">
+        <v>130</v>
+      </c>
+      <c r="I324" s="2">
+        <v>4.66</v>
+      </c>
+      <c r="K324" s="4">
+        <f t="shared" si="5"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11">
+      <c r="A325" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C325" t="s">
+        <v>10</v>
+      </c>
+      <c r="D325">
+        <v>-100</v>
+      </c>
+      <c r="E325" t="s">
+        <v>43</v>
+      </c>
+      <c r="F325" s="1">
+        <v>44365</v>
+      </c>
+      <c r="G325" t="s">
+        <v>8</v>
+      </c>
+      <c r="H325" s="3">
+        <v>130</v>
+      </c>
+      <c r="I325" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="K325" s="4">
+        <f t="shared" si="5"/>
+        <v>-430</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11">
+      <c r="A326" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C326" t="s">
+        <v>10</v>
+      </c>
+      <c r="D326">
+        <v>-100</v>
+      </c>
+      <c r="E326" t="s">
+        <v>6</v>
+      </c>
+      <c r="F326" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G326" t="s">
+        <v>8</v>
+      </c>
+      <c r="H326" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I326" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K326" s="4">
+        <f t="shared" si="5"/>
+        <v>-28.000000000000004</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11">
+      <c r="A327" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C327" t="s">
+        <v>4</v>
+      </c>
+      <c r="D327">
+        <v>100</v>
+      </c>
+      <c r="E327" t="s">
+        <v>6</v>
+      </c>
+      <c r="F327" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G327" t="s">
+        <v>8</v>
+      </c>
+      <c r="H327" s="3">
+        <v>4135</v>
+      </c>
+      <c r="I327" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="K327" s="4">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11">
+      <c r="A328" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C328" t="s">
+        <v>10</v>
+      </c>
+      <c r="D328">
+        <v>-100</v>
+      </c>
+      <c r="E328" t="s">
+        <v>6</v>
+      </c>
+      <c r="F328" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G328" t="s">
+        <v>8</v>
+      </c>
+      <c r="H328" s="3">
+        <v>4145</v>
+      </c>
+      <c r="I328" s="2">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K328" s="4">
+        <f t="shared" si="5"/>
+        <v>-204.99999999999997</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11">
+      <c r="A329" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C329" t="s">
+        <v>4</v>
+      </c>
+      <c r="D329">
+        <v>100</v>
+      </c>
+      <c r="E329" t="s">
+        <v>6</v>
+      </c>
+      <c r="F329" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G329" t="s">
+        <v>8</v>
+      </c>
+      <c r="H329" s="3">
+        <v>4140</v>
+      </c>
+      <c r="I329" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="K329" s="4">
+        <f t="shared" si="5"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11">
+      <c r="A330" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C330" t="s">
+        <v>4</v>
+      </c>
+      <c r="D330">
+        <v>100</v>
+      </c>
+      <c r="E330" t="s">
+        <v>6</v>
+      </c>
+      <c r="F330" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G330" t="s">
+        <v>8</v>
+      </c>
+      <c r="H330" s="3">
+        <v>4225</v>
+      </c>
+      <c r="I330" s="2">
+        <v>4.62</v>
+      </c>
+      <c r="K330" s="4">
+        <f t="shared" si="5"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11">
+      <c r="A331" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C331" t="s">
+        <v>10</v>
+      </c>
+      <c r="D331">
+        <v>-100</v>
+      </c>
+      <c r="E331" t="s">
+        <v>6</v>
+      </c>
+      <c r="F331" s="1">
+        <v>44323</v>
+      </c>
+      <c r="G331" t="s">
+        <v>8</v>
+      </c>
+      <c r="H331" s="3">
+        <v>4220</v>
+      </c>
+      <c r="I331" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="K331" s="4">
+        <f t="shared" si="5"/>
+        <v>-352</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11">
+      <c r="A332" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C332" t="s">
+        <v>10</v>
+      </c>
+      <c r="D332">
+        <v>-100</v>
+      </c>
+      <c r="E332" t="s">
+        <v>6</v>
+      </c>
+      <c r="F332" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G332" t="s">
+        <v>8</v>
+      </c>
+      <c r="H332" s="3">
+        <v>4215</v>
+      </c>
+      <c r="I332" s="2">
+        <v>7.77</v>
+      </c>
+      <c r="K332" s="4">
+        <f t="shared" si="5"/>
+        <v>-777</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11">
+      <c r="A333" s="1">
+        <v>44323</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C333" t="s">
+        <v>4</v>
+      </c>
+      <c r="D333">
+        <v>100</v>
+      </c>
+      <c r="E333" t="s">
+        <v>6</v>
+      </c>
+      <c r="F333" s="1">
+        <v>44326</v>
+      </c>
+      <c r="G333" t="s">
+        <v>8</v>
+      </c>
+      <c r="H333" s="3">
+        <v>4220</v>
+      </c>
+      <c r="I333" s="2">
+        <v>9.02</v>
+      </c>
+      <c r="K333" s="4">
+        <f t="shared" si="5"/>
+        <v>902</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M3"/>

</xml_diff>

<commit_message>
Update 1-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="209">
   <si>
     <t>Date</t>
   </si>
@@ -589,6 +589,63 @@
   </si>
   <si>
     <t>1508-71048</t>
+  </si>
+  <si>
+    <t>1511-87668</t>
+  </si>
+  <si>
+    <t>1511-88542</t>
+  </si>
+  <si>
+    <t>1511-96435</t>
+  </si>
+  <si>
+    <t>1514-10989</t>
+  </si>
+  <si>
+    <t>1514-17535</t>
+  </si>
+  <si>
+    <t>1514-19827</t>
+  </si>
+  <si>
+    <t>1514-24734</t>
+  </si>
+  <si>
+    <t>1517-12588</t>
+  </si>
+  <si>
+    <t>1517-18557</t>
+  </si>
+  <si>
+    <t>1519-35625</t>
+  </si>
+  <si>
+    <t>1519-39131</t>
+  </si>
+  <si>
+    <t>1519-40552</t>
+  </si>
+  <si>
+    <t>1519-65314</t>
+  </si>
+  <si>
+    <t>1519-65891</t>
+  </si>
+  <si>
+    <t>1522-52805</t>
+  </si>
+  <si>
+    <t>1522-66478</t>
+  </si>
+  <si>
+    <t>1522-94554</t>
+  </si>
+  <si>
+    <t>1522-98714</t>
+  </si>
+  <si>
+    <t>1523-02944</t>
   </si>
 </sst>
 </file>
@@ -954,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O473"/>
+  <dimension ref="A1:O530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A457" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K475" sqref="K475"/>
+      <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K532" sqref="K532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11859,7 +11916,7 @@
         <v>25.28</v>
       </c>
       <c r="K445" s="4">
-        <f t="shared" ref="K445:K473" si="12">D445*I445</f>
+        <f t="shared" ref="K445:K508" si="12">D445*I445</f>
         <v>2528</v>
       </c>
     </row>
@@ -12488,6 +12545,1260 @@
       <c r="K473" s="4">
         <f t="shared" si="12"/>
         <v>-149</v>
+      </c>
+    </row>
+    <row r="475" spans="1:11">
+      <c r="A475" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B475" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C475" t="s">
+        <v>4</v>
+      </c>
+      <c r="D475">
+        <v>100</v>
+      </c>
+      <c r="E475" t="s">
+        <v>6</v>
+      </c>
+      <c r="F475" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G475" t="s">
+        <v>8</v>
+      </c>
+      <c r="H475" s="3">
+        <v>4090</v>
+      </c>
+      <c r="I475" s="2">
+        <v>43.92</v>
+      </c>
+      <c r="K475" s="4">
+        <f t="shared" si="12"/>
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="476" spans="1:11">
+      <c r="A476" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B476" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C476" t="s">
+        <v>10</v>
+      </c>
+      <c r="D476">
+        <v>-100</v>
+      </c>
+      <c r="E476" t="s">
+        <v>6</v>
+      </c>
+      <c r="F476" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G476" t="s">
+        <v>8</v>
+      </c>
+      <c r="H476" s="3">
+        <v>4085</v>
+      </c>
+      <c r="I476" s="2">
+        <v>43.07</v>
+      </c>
+      <c r="K476" s="4">
+        <f t="shared" si="12"/>
+        <v>-4307</v>
+      </c>
+    </row>
+    <row r="478" spans="1:11">
+      <c r="A478" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C478" t="s">
+        <v>4</v>
+      </c>
+      <c r="D478">
+        <v>100</v>
+      </c>
+      <c r="E478" t="s">
+        <v>6</v>
+      </c>
+      <c r="F478" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G478" t="s">
+        <v>8</v>
+      </c>
+      <c r="H478" s="3">
+        <v>4090</v>
+      </c>
+      <c r="I478" s="2">
+        <v>16.829999999999998</v>
+      </c>
+      <c r="K478" s="4">
+        <f t="shared" si="12"/>
+        <v>1682.9999999999998</v>
+      </c>
+    </row>
+    <row r="479" spans="1:11">
+      <c r="A479" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C479" t="s">
+        <v>10</v>
+      </c>
+      <c r="D479">
+        <v>-100</v>
+      </c>
+      <c r="E479" t="s">
+        <v>6</v>
+      </c>
+      <c r="F479" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G479" t="s">
+        <v>8</v>
+      </c>
+      <c r="H479" s="3">
+        <v>4085</v>
+      </c>
+      <c r="I479" s="2">
+        <v>16.28</v>
+      </c>
+      <c r="K479" s="4">
+        <f t="shared" si="12"/>
+        <v>-1628</v>
+      </c>
+    </row>
+    <row r="481" spans="1:11">
+      <c r="A481" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B481" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C481" t="s">
+        <v>10</v>
+      </c>
+      <c r="D481">
+        <v>-100</v>
+      </c>
+      <c r="E481" t="s">
+        <v>36</v>
+      </c>
+      <c r="F481" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G481" t="s">
+        <v>8</v>
+      </c>
+      <c r="H481" s="3">
+        <v>2115</v>
+      </c>
+      <c r="I481" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="K481" s="4">
+        <f t="shared" si="12"/>
+        <v>-2780</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11">
+      <c r="A482" s="1">
+        <v>44340</v>
+      </c>
+      <c r="B482" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C482" t="s">
+        <v>4</v>
+      </c>
+      <c r="D482">
+        <v>100</v>
+      </c>
+      <c r="E482" t="s">
+        <v>36</v>
+      </c>
+      <c r="F482" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G482" t="s">
+        <v>8</v>
+      </c>
+      <c r="H482" s="3">
+        <v>2120</v>
+      </c>
+      <c r="I482" s="2">
+        <v>28.84</v>
+      </c>
+      <c r="K482" s="4">
+        <f t="shared" si="12"/>
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11">
+      <c r="A484" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B484" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C484" t="s">
+        <v>10</v>
+      </c>
+      <c r="D484">
+        <v>-100</v>
+      </c>
+      <c r="E484" t="s">
+        <v>8</v>
+      </c>
+      <c r="F484" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G484" t="s">
+        <v>8</v>
+      </c>
+      <c r="H484" s="3">
+        <v>2120</v>
+      </c>
+      <c r="I484" s="2">
+        <v>23.49</v>
+      </c>
+      <c r="K484" s="4">
+        <f t="shared" si="12"/>
+        <v>-2349</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11">
+      <c r="A485" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B485" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C485" t="s">
+        <v>4</v>
+      </c>
+      <c r="D485">
+        <v>100</v>
+      </c>
+      <c r="E485" t="s">
+        <v>8</v>
+      </c>
+      <c r="F485" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G485" t="s">
+        <v>8</v>
+      </c>
+      <c r="H485" s="3">
+        <v>2105</v>
+      </c>
+      <c r="I485" s="2">
+        <v>20.82</v>
+      </c>
+      <c r="K485" s="4">
+        <f t="shared" si="12"/>
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11">
+      <c r="A487" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B487" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C487" t="s">
+        <v>10</v>
+      </c>
+      <c r="D487">
+        <v>-100</v>
+      </c>
+      <c r="E487" t="s">
+        <v>36</v>
+      </c>
+      <c r="F487" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G487" t="s">
+        <v>23</v>
+      </c>
+      <c r="H487" s="3">
+        <v>2305</v>
+      </c>
+      <c r="I487" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="K487" s="4">
+        <f t="shared" si="12"/>
+        <v>-2720</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11">
+      <c r="A488" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B488" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C488" t="s">
+        <v>4</v>
+      </c>
+      <c r="D488">
+        <v>100</v>
+      </c>
+      <c r="E488" t="s">
+        <v>36</v>
+      </c>
+      <c r="F488" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G488" t="s">
+        <v>23</v>
+      </c>
+      <c r="H488" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I488" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="K488" s="4">
+        <f t="shared" si="12"/>
+        <v>2540</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11">
+      <c r="A490" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B490" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C490" t="s">
+        <v>4</v>
+      </c>
+      <c r="D490">
+        <v>100</v>
+      </c>
+      <c r="E490" t="s">
+        <v>6</v>
+      </c>
+      <c r="F490" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G490" t="s">
+        <v>8</v>
+      </c>
+      <c r="H490" s="3">
+        <v>4100</v>
+      </c>
+      <c r="I490" s="2">
+        <v>14.62</v>
+      </c>
+      <c r="K490" s="4">
+        <f t="shared" si="12"/>
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11">
+      <c r="A491" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B491" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C491" t="s">
+        <v>10</v>
+      </c>
+      <c r="D491">
+        <v>-100</v>
+      </c>
+      <c r="E491" t="s">
+        <v>6</v>
+      </c>
+      <c r="F491" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G491" t="s">
+        <v>8</v>
+      </c>
+      <c r="H491" s="3">
+        <v>4090</v>
+      </c>
+      <c r="I491" s="2">
+        <v>13.47</v>
+      </c>
+      <c r="K491" s="4">
+        <f t="shared" si="12"/>
+        <v>-1347</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11">
+      <c r="A493" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B493" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C493" t="s">
+        <v>4</v>
+      </c>
+      <c r="D493">
+        <v>100</v>
+      </c>
+      <c r="E493" t="s">
+        <v>6</v>
+      </c>
+      <c r="F493" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G493" t="s">
+        <v>8</v>
+      </c>
+      <c r="H493" s="3">
+        <v>4095</v>
+      </c>
+      <c r="I493" s="2">
+        <v>42.47</v>
+      </c>
+      <c r="K493" s="4">
+        <f t="shared" si="12"/>
+        <v>4247</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11">
+      <c r="A494" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B494" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C494" t="s">
+        <v>10</v>
+      </c>
+      <c r="D494">
+        <v>-100</v>
+      </c>
+      <c r="E494" t="s">
+        <v>6</v>
+      </c>
+      <c r="F494" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G494" t="s">
+        <v>8</v>
+      </c>
+      <c r="H494" s="3">
+        <v>4090</v>
+      </c>
+      <c r="I494" s="2">
+        <v>41.57</v>
+      </c>
+      <c r="K494" s="4">
+        <f t="shared" si="12"/>
+        <v>-4157</v>
+      </c>
+    </row>
+    <row r="496" spans="1:11">
+      <c r="A496" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B496" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C496" t="s">
+        <v>4</v>
+      </c>
+      <c r="D496">
+        <v>100</v>
+      </c>
+      <c r="E496" t="s">
+        <v>6</v>
+      </c>
+      <c r="F496" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G496" t="s">
+        <v>8</v>
+      </c>
+      <c r="H496" s="3">
+        <v>4000</v>
+      </c>
+      <c r="I496" s="2">
+        <v>46.22</v>
+      </c>
+      <c r="K496" s="4">
+        <f t="shared" si="12"/>
+        <v>4622</v>
+      </c>
+    </row>
+    <row r="497" spans="1:11">
+      <c r="A497" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B497" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C497" t="s">
+        <v>10</v>
+      </c>
+      <c r="D497">
+        <v>-100</v>
+      </c>
+      <c r="E497" t="s">
+        <v>6</v>
+      </c>
+      <c r="F497" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G497" t="s">
+        <v>8</v>
+      </c>
+      <c r="H497" s="3">
+        <v>3980</v>
+      </c>
+      <c r="I497" s="2">
+        <v>43.32</v>
+      </c>
+      <c r="K497" s="4">
+        <f t="shared" si="12"/>
+        <v>-4332</v>
+      </c>
+    </row>
+    <row r="499" spans="1:11">
+      <c r="A499" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B499" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C499" t="s">
+        <v>4</v>
+      </c>
+      <c r="D499">
+        <v>100</v>
+      </c>
+      <c r="E499" t="s">
+        <v>87</v>
+      </c>
+      <c r="F499" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G499" t="s">
+        <v>8</v>
+      </c>
+      <c r="H499" s="3">
+        <v>13100</v>
+      </c>
+      <c r="I499" s="2">
+        <v>170.75</v>
+      </c>
+      <c r="K499" s="4">
+        <f t="shared" si="12"/>
+        <v>17075</v>
+      </c>
+    </row>
+    <row r="500" spans="1:11">
+      <c r="A500" s="1">
+        <v>44342</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C500" t="s">
+        <v>10</v>
+      </c>
+      <c r="D500">
+        <v>-100</v>
+      </c>
+      <c r="E500" t="s">
+        <v>87</v>
+      </c>
+      <c r="F500" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G500" t="s">
+        <v>8</v>
+      </c>
+      <c r="H500" s="3">
+        <v>13075</v>
+      </c>
+      <c r="I500" s="2">
+        <v>165.95</v>
+      </c>
+      <c r="K500" s="4">
+        <f t="shared" si="12"/>
+        <v>-16595</v>
+      </c>
+    </row>
+    <row r="502" spans="1:11">
+      <c r="A502" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C502" t="s">
+        <v>4</v>
+      </c>
+      <c r="D502">
+        <v>100</v>
+      </c>
+      <c r="E502" t="s">
+        <v>6</v>
+      </c>
+      <c r="F502" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G502" t="s">
+        <v>8</v>
+      </c>
+      <c r="H502" s="3">
+        <v>4100</v>
+      </c>
+      <c r="I502" s="2">
+        <v>34.869999999999997</v>
+      </c>
+      <c r="K502" s="4">
+        <f t="shared" si="12"/>
+        <v>3486.9999999999995</v>
+      </c>
+    </row>
+    <row r="503" spans="1:11">
+      <c r="A503" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C503" t="s">
+        <v>10</v>
+      </c>
+      <c r="D503">
+        <v>-100</v>
+      </c>
+      <c r="E503" t="s">
+        <v>6</v>
+      </c>
+      <c r="F503" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G503" t="s">
+        <v>8</v>
+      </c>
+      <c r="H503" s="3">
+        <v>4095</v>
+      </c>
+      <c r="I503" s="2">
+        <v>34.07</v>
+      </c>
+      <c r="K503" s="4">
+        <f t="shared" si="12"/>
+        <v>-3407</v>
+      </c>
+    </row>
+    <row r="505" spans="1:11">
+      <c r="A505" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B505" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C505" t="s">
+        <v>10</v>
+      </c>
+      <c r="D505">
+        <v>-100</v>
+      </c>
+      <c r="E505" t="s">
+        <v>6</v>
+      </c>
+      <c r="F505" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G505" t="s">
+        <v>8</v>
+      </c>
+      <c r="H505" s="3">
+        <v>4100</v>
+      </c>
+      <c r="I505" s="2">
+        <v>9.08</v>
+      </c>
+      <c r="K505" s="4">
+        <f t="shared" si="12"/>
+        <v>-908</v>
+      </c>
+    </row>
+    <row r="506" spans="1:11">
+      <c r="A506" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C506" t="s">
+        <v>4</v>
+      </c>
+      <c r="D506">
+        <v>100</v>
+      </c>
+      <c r="E506" t="s">
+        <v>6</v>
+      </c>
+      <c r="F506" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G506" t="s">
+        <v>8</v>
+      </c>
+      <c r="H506" s="3">
+        <v>4095</v>
+      </c>
+      <c r="I506" s="2">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="K506" s="4">
+        <f t="shared" si="12"/>
+        <v>863.00000000000011</v>
+      </c>
+    </row>
+    <row r="508" spans="1:11">
+      <c r="A508" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C508" t="s">
+        <v>10</v>
+      </c>
+      <c r="D508">
+        <v>-100</v>
+      </c>
+      <c r="E508" t="s">
+        <v>6</v>
+      </c>
+      <c r="F508" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G508" t="s">
+        <v>8</v>
+      </c>
+      <c r="H508" s="3">
+        <v>4000</v>
+      </c>
+      <c r="I508" s="2">
+        <v>39.630000000000003</v>
+      </c>
+      <c r="K508" s="4">
+        <f t="shared" si="12"/>
+        <v>-3963.0000000000005</v>
+      </c>
+    </row>
+    <row r="509" spans="1:11">
+      <c r="A509" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C509" t="s">
+        <v>4</v>
+      </c>
+      <c r="D509">
+        <v>100</v>
+      </c>
+      <c r="E509" t="s">
+        <v>6</v>
+      </c>
+      <c r="F509" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G509" t="s">
+        <v>8</v>
+      </c>
+      <c r="H509" s="3">
+        <v>3990</v>
+      </c>
+      <c r="I509" s="2">
+        <v>38.229999999999997</v>
+      </c>
+      <c r="K509" s="4">
+        <f t="shared" ref="K509:K530" si="13">D509*I509</f>
+        <v>3822.9999999999995</v>
+      </c>
+    </row>
+    <row r="511" spans="1:11">
+      <c r="A511" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C511" t="s">
+        <v>10</v>
+      </c>
+      <c r="D511">
+        <v>-100</v>
+      </c>
+      <c r="E511" t="s">
+        <v>36</v>
+      </c>
+      <c r="F511" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G511" t="s">
+        <v>8</v>
+      </c>
+      <c r="H511" s="3">
+        <v>2105</v>
+      </c>
+      <c r="I511" s="2">
+        <v>15.18</v>
+      </c>
+      <c r="K511" s="4">
+        <f t="shared" si="13"/>
+        <v>-1518</v>
+      </c>
+    </row>
+    <row r="512" spans="1:11">
+      <c r="A512" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C512" t="s">
+        <v>4</v>
+      </c>
+      <c r="D512">
+        <v>100</v>
+      </c>
+      <c r="E512" t="s">
+        <v>36</v>
+      </c>
+      <c r="F512" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G512" t="s">
+        <v>8</v>
+      </c>
+      <c r="H512" s="3">
+        <v>2110</v>
+      </c>
+      <c r="I512" s="2">
+        <v>15.8</v>
+      </c>
+      <c r="K512" s="4">
+        <f t="shared" si="13"/>
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="514" spans="1:11">
+      <c r="A514" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C514" t="s">
+        <v>10</v>
+      </c>
+      <c r="D514">
+        <v>-100</v>
+      </c>
+      <c r="E514" t="s">
+        <v>36</v>
+      </c>
+      <c r="F514" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G514" t="s">
+        <v>23</v>
+      </c>
+      <c r="H514" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I514" s="2">
+        <v>29.92</v>
+      </c>
+      <c r="K514" s="4">
+        <f t="shared" si="13"/>
+        <v>-2992</v>
+      </c>
+    </row>
+    <row r="515" spans="1:11">
+      <c r="A515" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C515" t="s">
+        <v>4</v>
+      </c>
+      <c r="D515">
+        <v>100</v>
+      </c>
+      <c r="E515" t="s">
+        <v>36</v>
+      </c>
+      <c r="F515" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G515" t="s">
+        <v>23</v>
+      </c>
+      <c r="H515" s="3">
+        <v>2305</v>
+      </c>
+      <c r="I515" s="2">
+        <v>31.97</v>
+      </c>
+      <c r="K515" s="4">
+        <f t="shared" si="13"/>
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="517" spans="1:11">
+      <c r="A517" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C517" t="s">
+        <v>4</v>
+      </c>
+      <c r="D517">
+        <v>100</v>
+      </c>
+      <c r="E517" t="s">
+        <v>6</v>
+      </c>
+      <c r="F517" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G517" t="s">
+        <v>8</v>
+      </c>
+      <c r="H517" s="3">
+        <v>4070</v>
+      </c>
+      <c r="I517" s="2">
+        <v>45.32</v>
+      </c>
+      <c r="K517" s="4">
+        <f t="shared" si="13"/>
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="518" spans="1:11">
+      <c r="A518" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C518" t="s">
+        <v>10</v>
+      </c>
+      <c r="D518">
+        <v>-100</v>
+      </c>
+      <c r="E518" t="s">
+        <v>6</v>
+      </c>
+      <c r="F518" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G518" t="s">
+        <v>8</v>
+      </c>
+      <c r="H518" s="3">
+        <v>3990</v>
+      </c>
+      <c r="I518" s="2">
+        <v>33.82</v>
+      </c>
+      <c r="K518" s="4">
+        <f t="shared" si="13"/>
+        <v>-3382</v>
+      </c>
+    </row>
+    <row r="520" spans="1:11">
+      <c r="A520" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C520" t="s">
+        <v>4</v>
+      </c>
+      <c r="D520">
+        <v>100</v>
+      </c>
+      <c r="E520" t="s">
+        <v>6</v>
+      </c>
+      <c r="F520" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G520" t="s">
+        <v>8</v>
+      </c>
+      <c r="H520" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I520" s="2">
+        <v>10.95</v>
+      </c>
+      <c r="K520" s="4">
+        <f t="shared" si="13"/>
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="521" spans="1:11">
+      <c r="A521" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C521" t="s">
+        <v>10</v>
+      </c>
+      <c r="D521">
+        <v>-100</v>
+      </c>
+      <c r="E521" t="s">
+        <v>6</v>
+      </c>
+      <c r="F521" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G521" t="s">
+        <v>8</v>
+      </c>
+      <c r="H521" s="3">
+        <v>4095</v>
+      </c>
+      <c r="I521" s="2">
+        <v>5.85</v>
+      </c>
+      <c r="K521" s="4">
+        <f t="shared" si="13"/>
+        <v>-585</v>
+      </c>
+    </row>
+    <row r="523" spans="1:11">
+      <c r="A523" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C523" t="s">
+        <v>4</v>
+      </c>
+      <c r="D523">
+        <v>100</v>
+      </c>
+      <c r="E523" t="s">
+        <v>36</v>
+      </c>
+      <c r="F523" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G523" t="s">
+        <v>8</v>
+      </c>
+      <c r="H523" s="3">
+        <v>2100</v>
+      </c>
+      <c r="I523" s="2">
+        <v>13.02</v>
+      </c>
+      <c r="K523" s="4">
+        <f t="shared" si="13"/>
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="524" spans="1:11">
+      <c r="A524" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C524" t="s">
+        <v>10</v>
+      </c>
+      <c r="D524">
+        <v>-100</v>
+      </c>
+      <c r="E524" t="s">
+        <v>36</v>
+      </c>
+      <c r="F524" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G524" t="s">
+        <v>8</v>
+      </c>
+      <c r="H524" s="3">
+        <v>2070</v>
+      </c>
+      <c r="I524" s="2">
+        <v>10.17</v>
+      </c>
+      <c r="K524" s="4">
+        <f t="shared" si="13"/>
+        <v>-1017</v>
+      </c>
+    </row>
+    <row r="526" spans="1:11">
+      <c r="A526" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C526" t="s">
+        <v>4</v>
+      </c>
+      <c r="D526">
+        <v>100</v>
+      </c>
+      <c r="E526" t="s">
+        <v>36</v>
+      </c>
+      <c r="F526" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G526" t="s">
+        <v>23</v>
+      </c>
+      <c r="H526" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I526" s="2">
+        <v>29.78</v>
+      </c>
+      <c r="K526" s="4">
+        <f t="shared" si="13"/>
+        <v>2978</v>
+      </c>
+    </row>
+    <row r="527" spans="1:11">
+      <c r="A527" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C527" t="s">
+        <v>10</v>
+      </c>
+      <c r="D527">
+        <v>-100</v>
+      </c>
+      <c r="E527" t="s">
+        <v>36</v>
+      </c>
+      <c r="F527" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G527" t="s">
+        <v>23</v>
+      </c>
+      <c r="H527" s="3">
+        <v>2340</v>
+      </c>
+      <c r="I527" s="2">
+        <v>19.03</v>
+      </c>
+      <c r="K527" s="4">
+        <f t="shared" si="13"/>
+        <v>-1903</v>
+      </c>
+    </row>
+    <row r="529" spans="1:11">
+      <c r="A529" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C529" t="s">
+        <v>4</v>
+      </c>
+      <c r="D529">
+        <v>100</v>
+      </c>
+      <c r="E529" t="s">
+        <v>6</v>
+      </c>
+      <c r="F529" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G529" t="s">
+        <v>8</v>
+      </c>
+      <c r="H529" s="3">
+        <v>4075</v>
+      </c>
+      <c r="I529" s="2">
+        <v>26.69</v>
+      </c>
+      <c r="K529" s="4">
+        <f t="shared" si="13"/>
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="530" spans="1:11">
+      <c r="A530" s="1">
+        <v>44344</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C530" t="s">
+        <v>10</v>
+      </c>
+      <c r="D530">
+        <v>-100</v>
+      </c>
+      <c r="E530" t="s">
+        <v>6</v>
+      </c>
+      <c r="F530" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G530" t="s">
+        <v>8</v>
+      </c>
+      <c r="H530" s="3">
+        <v>4020</v>
+      </c>
+      <c r="I530" s="2">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="K530" s="4">
+        <f t="shared" si="13"/>
+        <v>-2044.0000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -7,19 +7,19 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Trades" sheetId="1" r:id="rId1"/>
+    <sheet name="Account U27637" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Trades!$A$1:$M$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="221">
   <si>
     <t>Date</t>
   </si>
@@ -646,6 +646,42 @@
   </si>
   <si>
     <t>1523-02944</t>
+  </si>
+  <si>
+    <t>P/L Day</t>
+  </si>
+  <si>
+    <t>P/L YTD</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>Day Trade #</t>
+  </si>
+  <si>
+    <t>Stock BP</t>
+  </si>
+  <si>
+    <t>Option BP</t>
+  </si>
+  <si>
+    <t>Cash Balance</t>
+  </si>
+  <si>
+    <t>Pending Cash</t>
+  </si>
+  <si>
+    <t>Start day BP</t>
+  </si>
+  <si>
+    <t>1526-15652</t>
+  </si>
+  <si>
+    <t>1526-19936</t>
   </si>
 </sst>
 </file>
@@ -702,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -716,6 +752,7 @@
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1011,11 +1048,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O530"/>
+  <dimension ref="A1:O536"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K532" sqref="K532"/>
+      <selection pane="bottomLeft" activeCell="K537" sqref="K537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13335,7 +13372,7 @@
         <v>38.229999999999997</v>
       </c>
       <c r="K509" s="4">
-        <f t="shared" ref="K509:K530" si="13">D509*I509</f>
+        <f t="shared" ref="K509:K536" si="13">D509*I509</f>
         <v>3822.9999999999995</v>
       </c>
     </row>
@@ -13799,6 +13836,138 @@
       <c r="K530" s="4">
         <f t="shared" si="13"/>
         <v>-2044.0000000000002</v>
+      </c>
+    </row>
+    <row r="532" spans="1:11">
+      <c r="A532" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C532" t="s">
+        <v>4</v>
+      </c>
+      <c r="D532">
+        <v>100</v>
+      </c>
+      <c r="E532" t="s">
+        <v>87</v>
+      </c>
+      <c r="F532" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G532" t="s">
+        <v>23</v>
+      </c>
+      <c r="H532" s="3">
+        <v>14100</v>
+      </c>
+      <c r="I532" s="2">
+        <v>107.98</v>
+      </c>
+      <c r="K532" s="4">
+        <f t="shared" si="13"/>
+        <v>10798</v>
+      </c>
+    </row>
+    <row r="533" spans="1:11">
+      <c r="A533" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C533" t="s">
+        <v>10</v>
+      </c>
+      <c r="D533">
+        <v>-100</v>
+      </c>
+      <c r="E533" t="s">
+        <v>87</v>
+      </c>
+      <c r="F533" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G533" t="s">
+        <v>23</v>
+      </c>
+      <c r="H533" s="3">
+        <v>14125</v>
+      </c>
+      <c r="I533" s="2">
+        <v>100.73</v>
+      </c>
+      <c r="K533" s="4">
+        <f t="shared" si="13"/>
+        <v>-10073</v>
+      </c>
+    </row>
+    <row r="535" spans="1:11">
+      <c r="A535" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C535" t="s">
+        <v>4</v>
+      </c>
+      <c r="D535">
+        <v>100</v>
+      </c>
+      <c r="E535" t="s">
+        <v>87</v>
+      </c>
+      <c r="F535" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G535" t="s">
+        <v>8</v>
+      </c>
+      <c r="H535" s="3">
+        <v>13200</v>
+      </c>
+      <c r="I535" s="2">
+        <v>167.58</v>
+      </c>
+      <c r="K535" s="4">
+        <f t="shared" si="13"/>
+        <v>16758</v>
+      </c>
+    </row>
+    <row r="536" spans="1:11">
+      <c r="A536" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C536" t="s">
+        <v>10</v>
+      </c>
+      <c r="D536">
+        <v>-100</v>
+      </c>
+      <c r="E536" t="s">
+        <v>87</v>
+      </c>
+      <c r="F536" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G536" t="s">
+        <v>8</v>
+      </c>
+      <c r="H536" s="3">
+        <v>13100</v>
+      </c>
+      <c r="I536" s="2">
+        <v>146.93</v>
+      </c>
+      <c r="K536" s="4">
+        <f t="shared" si="13"/>
+        <v>-14693</v>
       </c>
     </row>
   </sheetData>
@@ -13813,13 +13982,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="5"/>
+    <col min="7" max="8" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B2" s="13">
+        <v>168.48</v>
+      </c>
+      <c r="C2" s="13">
+        <v>-2227.16</v>
+      </c>
+      <c r="D2" s="5">
+        <v>609</v>
+      </c>
+      <c r="E2" s="5">
+        <v>142</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>49113.89</v>
+      </c>
+      <c r="H2" s="6">
+        <v>24556.94</v>
+      </c>
+      <c r="I2" s="13">
+        <v>51537.17</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>40965.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>44350</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update 4-Jun-2021, end of day updaate
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trades" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>1526-19936</t>
+  </si>
+  <si>
+    <t>Net Liq.</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O536"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K537" sqref="K537"/>
     </sheetView>
@@ -13982,98 +13985,142 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="5"/>
-    <col min="7" max="8" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="5"/>
+    <col min="8" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>44349</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="6">
+        <v>83947.32</v>
+      </c>
+      <c r="C2" s="13">
         <v>168.48</v>
       </c>
-      <c r="C2" s="13">
+      <c r="D2" s="13">
         <v>-2227.16</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>609</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>142</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>49113.89</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>24556.94</v>
       </c>
-      <c r="I2" s="13">
+      <c r="J2" s="13">
         <v>51537.17</v>
       </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
+      <c r="L2" s="6">
         <v>40965.81</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>44350</v>
+      </c>
+      <c r="B3" s="6">
+        <v>82451.95</v>
+      </c>
+      <c r="C3" s="13">
+        <v>-1369.93</v>
+      </c>
+      <c r="D3" s="13">
+        <v>3713.6</v>
+      </c>
+      <c r="E3" s="5">
+        <v>518</v>
+      </c>
+      <c r="F3" s="5">
+        <v>79</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>54596.59</v>
+      </c>
+      <c r="I3" s="6">
+        <v>27298.29</v>
+      </c>
+      <c r="J3" s="13">
+        <v>50660.04</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>29441.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>44351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 5-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>Net Liq.</t>
+  </si>
+  <si>
+    <t>Realized</t>
   </si>
 </sst>
 </file>
@@ -13985,11 +13988,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14002,9 +14005,10 @@
     <col min="10" max="10" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14041,8 +14045,11 @@
       <c r="L1" s="6" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="N1" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>44349</v>
       </c>
@@ -14079,8 +14086,11 @@
       <c r="L2" s="6">
         <v>40965.81</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="N2" s="13">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>44350</v>
       </c>
@@ -14117,10 +14127,49 @@
       <c r="L3" s="6">
         <v>29441.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="N3" s="13">
+        <v>-847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>44351</v>
+      </c>
+      <c r="B4" s="6">
+        <v>86242.17</v>
+      </c>
+      <c r="C4" s="13">
+        <v>-8642.2900000000009</v>
+      </c>
+      <c r="D4" s="13">
+        <v>85.11</v>
+      </c>
+      <c r="E4" s="5">
+        <v>374</v>
+      </c>
+      <c r="F4" s="5">
+        <v>91</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>30926.720000000001</v>
+      </c>
+      <c r="I4" s="6">
+        <v>15463.36</v>
+      </c>
+      <c r="J4" s="13">
+        <v>56241.55</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>36475.32</v>
+      </c>
+      <c r="N4" s="13">
+        <v>3154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 9-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -701,7 +701,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,8 +716,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,6 +735,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -759,6 +773,11 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -13988,11 +14007,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14005,7 +14024,7 @@
     <col min="10" max="10" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="8"/>
+    <col min="14" max="14" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -14170,6 +14189,107 @@
       </c>
       <c r="N4" s="13">
         <v>3154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B5" s="6">
+        <v>85618.77</v>
+      </c>
+      <c r="C5" s="13">
+        <v>-1303.1600000000001</v>
+      </c>
+      <c r="D5" s="13">
+        <v>-527.04999999999995</v>
+      </c>
+      <c r="E5" s="5">
+        <v>547</v>
+      </c>
+      <c r="F5" s="5">
+        <v>185</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>27636.28</v>
+      </c>
+      <c r="I5" s="6">
+        <v>13818.14</v>
+      </c>
+      <c r="J5" s="13">
+        <v>56163.31</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>24642.57</v>
+      </c>
+      <c r="N5" s="13">
+        <v>2578</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B6" s="6">
+        <v>85871.91</v>
+      </c>
+      <c r="C6" s="13">
+        <v>528</v>
+      </c>
+      <c r="D6" s="13">
+        <v>-272.05</v>
+      </c>
+      <c r="E6" s="5">
+        <v>892</v>
+      </c>
+      <c r="F6" s="5">
+        <v>211</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2788.22</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1394.11</v>
+      </c>
+      <c r="J6" s="13">
+        <v>61996.45</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>23549.439999999999</v>
+      </c>
+      <c r="N6" s="13">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18">
+        <f>SUM(N2:N9)</f>
+        <v>9874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 11-Jun-2021, end of day.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -14011,12 +14011,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="5"/>
@@ -14271,6 +14271,88 @@
       </c>
       <c r="N6" s="13">
         <v>1835</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B7" s="6">
+        <v>85746.49</v>
+      </c>
+      <c r="C7" s="13">
+        <v>122</v>
+      </c>
+      <c r="D7" s="13">
+        <v>-383.66</v>
+      </c>
+      <c r="E7" s="5">
+        <v>737</v>
+      </c>
+      <c r="F7" s="5">
+        <v>92</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2067.15</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1033.57</v>
+      </c>
+      <c r="J7" s="13">
+        <v>50986.04</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>10127.15</v>
+      </c>
+      <c r="N7" s="13">
+        <v>-1396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B8" s="6">
+        <v>87134.71</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1247.9000000000001</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1010.24</v>
+      </c>
+      <c r="E8" s="5">
+        <v>560</v>
+      </c>
+      <c r="F8" s="5">
+        <v>64</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5534.64</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2767.32</v>
+      </c>
+      <c r="J8" s="13">
+        <v>51052.36</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>10127.15</v>
+      </c>
+      <c r="N8" s="13">
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -14289,7 +14371,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="18">
         <f>SUM(N2:N9)</f>
-        <v>9874</v>
+        <v>8768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 12-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Trades" sheetId="1" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O536"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K537" sqref="K537"/>
     </sheetView>
@@ -14007,11 +14007,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14020,7 +14020,8 @@
     <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="5"/>
-    <col min="8" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
@@ -14355,23 +14356,69 @@
         <v>290</v>
       </c>
     </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B9" s="6">
+        <v>87459.88</v>
+      </c>
+      <c r="C9" s="13">
+        <v>-72.319999999999993</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1343.92</v>
+      </c>
+      <c r="E9" s="5">
+        <v>163</v>
+      </c>
+      <c r="F9" s="5">
+        <v>22</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>112595.43</v>
+      </c>
+      <c r="I9" s="6">
+        <v>56297.72</v>
+      </c>
+      <c r="J9" s="13">
+        <v>47891.85</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6">
+        <v>10128.81</v>
+      </c>
+      <c r="N9" s="13">
+        <v>519</v>
+      </c>
+    </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="18">
-        <f>SUM(N2:N9)</f>
-        <v>8768</v>
+      <c r="A10" s="1">
+        <v>44361</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18">
+        <f>SUM(N2:N14)</f>
+        <v>9287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 16-Jun-2021, end of day.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="263">
   <si>
     <t>Date</t>
   </si>
@@ -688,6 +688,126 @@
   </si>
   <si>
     <t>Realized</t>
+  </si>
+  <si>
+    <t>1528-66951</t>
+  </si>
+  <si>
+    <t>1528-68079</t>
+  </si>
+  <si>
+    <t>1528-72949</t>
+  </si>
+  <si>
+    <t>1531-95496</t>
+  </si>
+  <si>
+    <t>1532-70126</t>
+  </si>
+  <si>
+    <t>1535-03702</t>
+  </si>
+  <si>
+    <t>1535-10312</t>
+  </si>
+  <si>
+    <t>1535-16212</t>
+  </si>
+  <si>
+    <t>1535-19911</t>
+  </si>
+  <si>
+    <t>1537-80235</t>
+  </si>
+  <si>
+    <t>1537-82413</t>
+  </si>
+  <si>
+    <t>1537-84356</t>
+  </si>
+  <si>
+    <t>1537-87615</t>
+  </si>
+  <si>
+    <t>1538-04287</t>
+  </si>
+  <si>
+    <t>1538-04651</t>
+  </si>
+  <si>
+    <t>1540-67908</t>
+  </si>
+  <si>
+    <t>1540-69812</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>1540-70497</t>
+  </si>
+  <si>
+    <t>1543=14953</t>
+  </si>
+  <si>
+    <t>1543-18897</t>
+  </si>
+  <si>
+    <t>1543-28524</t>
+  </si>
+  <si>
+    <t>1543-30125</t>
+  </si>
+  <si>
+    <t>1543-35904</t>
+  </si>
+  <si>
+    <t>1545-83917</t>
+  </si>
+  <si>
+    <t>1545-84946</t>
+  </si>
+  <si>
+    <t>1545-88427</t>
+  </si>
+  <si>
+    <t>1545-95752</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>1548-71968</t>
+  </si>
+  <si>
+    <t>XND</t>
+  </si>
+  <si>
+    <t>1548-88305</t>
+  </si>
+  <si>
+    <t>1548-91996</t>
+  </si>
+  <si>
+    <t>1548-94581</t>
+  </si>
+  <si>
+    <t>1549-27499</t>
+  </si>
+  <si>
+    <t>1552-08565</t>
+  </si>
+  <si>
+    <t>1552-11174</t>
+  </si>
+  <si>
+    <t>1552-12967</t>
+  </si>
+  <si>
+    <t>1554-22935</t>
+  </si>
+  <si>
+    <t>SPY</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1193,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O536"/>
+  <dimension ref="A1:O643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A520" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K537" sqref="K537"/>
+      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D643" sqref="D643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13397,7 +13517,7 @@
         <v>38.229999999999997</v>
       </c>
       <c r="K509" s="4">
-        <f t="shared" ref="K509:K536" si="13">D509*I509</f>
+        <f t="shared" ref="K509:K574" si="13">D509*I509</f>
         <v>3822.9999999999995</v>
       </c>
     </row>
@@ -13994,6 +14114,2346 @@
         <f t="shared" si="13"/>
         <v>-14693</v>
       </c>
+    </row>
+    <row r="538" spans="1:11">
+      <c r="A538" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B538" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C538" t="s">
+        <v>4</v>
+      </c>
+      <c r="D538">
+        <v>100</v>
+      </c>
+      <c r="E538" t="s">
+        <v>6</v>
+      </c>
+      <c r="F538" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G538" t="s">
+        <v>8</v>
+      </c>
+      <c r="H538" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I538" s="2">
+        <v>7</v>
+      </c>
+      <c r="K538" s="4">
+        <f t="shared" si="13"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="539" spans="1:11">
+      <c r="A539" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B539" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C539" t="s">
+        <v>10</v>
+      </c>
+      <c r="D539">
+        <v>-100</v>
+      </c>
+      <c r="E539" t="s">
+        <v>6</v>
+      </c>
+      <c r="F539" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G539" t="s">
+        <v>8</v>
+      </c>
+      <c r="H539" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I539" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K539" s="4">
+        <f t="shared" si="13"/>
+        <v>-459.99999999999994</v>
+      </c>
+    </row>
+    <row r="541" spans="1:11">
+      <c r="A541" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B541" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C541" t="s">
+        <v>4</v>
+      </c>
+      <c r="D541">
+        <v>100</v>
+      </c>
+      <c r="E541" t="s">
+        <v>6</v>
+      </c>
+      <c r="F541" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G541" t="s">
+        <v>8</v>
+      </c>
+      <c r="H541" s="3">
+        <v>4110</v>
+      </c>
+      <c r="I541" s="2">
+        <v>28.17</v>
+      </c>
+      <c r="K541" s="4">
+        <f t="shared" si="13"/>
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="542" spans="1:11">
+      <c r="A542" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C542" t="s">
+        <v>10</v>
+      </c>
+      <c r="D542">
+        <v>-100</v>
+      </c>
+      <c r="E542" t="s">
+        <v>6</v>
+      </c>
+      <c r="F542" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G542" t="s">
+        <v>8</v>
+      </c>
+      <c r="H542" s="3">
+        <v>4100</v>
+      </c>
+      <c r="I542" s="2">
+        <v>26.67</v>
+      </c>
+      <c r="K542" s="4">
+        <f t="shared" si="13"/>
+        <v>-2667</v>
+      </c>
+    </row>
+    <row r="544" spans="1:11">
+      <c r="A544" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B544" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C544" t="s">
+        <v>10</v>
+      </c>
+      <c r="D544">
+        <v>-100</v>
+      </c>
+      <c r="E544" t="s">
+        <v>87</v>
+      </c>
+      <c r="F544" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G544" t="s">
+        <v>8</v>
+      </c>
+      <c r="H544" s="3">
+        <v>13200</v>
+      </c>
+      <c r="I544" s="2">
+        <v>145.41</v>
+      </c>
+      <c r="K544" s="4">
+        <f t="shared" si="13"/>
+        <v>-14541</v>
+      </c>
+    </row>
+    <row r="545" spans="1:11">
+      <c r="A545" s="1">
+        <v>44349</v>
+      </c>
+      <c r="B545" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C545" t="s">
+        <v>4</v>
+      </c>
+      <c r="D545">
+        <v>100</v>
+      </c>
+      <c r="E545" t="s">
+        <v>87</v>
+      </c>
+      <c r="F545" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G545" t="s">
+        <v>8</v>
+      </c>
+      <c r="H545" s="3">
+        <v>13225</v>
+      </c>
+      <c r="I545" s="2">
+        <v>150.38999999999999</v>
+      </c>
+      <c r="K545" s="4">
+        <f t="shared" si="13"/>
+        <v>15038.999999999998</v>
+      </c>
+    </row>
+    <row r="547" spans="1:11">
+      <c r="A547" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B547" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C547" t="s">
+        <v>10</v>
+      </c>
+      <c r="D547">
+        <v>-100</v>
+      </c>
+      <c r="E547" t="s">
+        <v>6</v>
+      </c>
+      <c r="F547" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G547" t="s">
+        <v>8</v>
+      </c>
+      <c r="H547" s="3">
+        <v>4170</v>
+      </c>
+      <c r="I547" s="2">
+        <v>16.77</v>
+      </c>
+      <c r="K547" s="4">
+        <f t="shared" si="13"/>
+        <v>-1677</v>
+      </c>
+    </row>
+    <row r="548" spans="1:11">
+      <c r="A548" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B548" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C548" t="s">
+        <v>4</v>
+      </c>
+      <c r="D548">
+        <v>100</v>
+      </c>
+      <c r="E548" t="s">
+        <v>6</v>
+      </c>
+      <c r="F548" s="1">
+        <v>44354</v>
+      </c>
+      <c r="G548" t="s">
+        <v>8</v>
+      </c>
+      <c r="H548" s="3">
+        <v>4075</v>
+      </c>
+      <c r="I548" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="K548" s="4">
+        <f t="shared" si="13"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="550" spans="1:11">
+      <c r="A550" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B550" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C550" t="s">
+        <v>10</v>
+      </c>
+      <c r="D550">
+        <v>-100</v>
+      </c>
+      <c r="E550" t="s">
+        <v>36</v>
+      </c>
+      <c r="F550" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G550" t="s">
+        <v>8</v>
+      </c>
+      <c r="H550" s="3">
+        <v>2110</v>
+      </c>
+      <c r="I550" s="2">
+        <v>11.93</v>
+      </c>
+      <c r="K550" s="4">
+        <f t="shared" si="13"/>
+        <v>-1193</v>
+      </c>
+    </row>
+    <row r="551" spans="1:11">
+      <c r="A551" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C551" t="s">
+        <v>4</v>
+      </c>
+      <c r="D551">
+        <v>100</v>
+      </c>
+      <c r="E551" t="s">
+        <v>36</v>
+      </c>
+      <c r="F551" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G551" t="s">
+        <v>8</v>
+      </c>
+      <c r="H551" s="3">
+        <v>2070</v>
+      </c>
+      <c r="I551" s="2">
+        <v>8.68</v>
+      </c>
+      <c r="K551" s="4">
+        <f t="shared" si="13"/>
+        <v>868</v>
+      </c>
+    </row>
+    <row r="553" spans="1:11">
+      <c r="A553" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C553" t="s">
+        <v>4</v>
+      </c>
+      <c r="D553">
+        <v>100</v>
+      </c>
+      <c r="E553" t="s">
+        <v>87</v>
+      </c>
+      <c r="F553" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G553" t="s">
+        <v>8</v>
+      </c>
+      <c r="H553" s="3">
+        <v>13400</v>
+      </c>
+      <c r="I553" s="2">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="K553" s="4">
+        <f t="shared" si="13"/>
+        <v>16180.000000000002</v>
+      </c>
+    </row>
+    <row r="554" spans="1:11">
+      <c r="A554" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C554" t="s">
+        <v>10</v>
+      </c>
+      <c r="D554">
+        <v>-100</v>
+      </c>
+      <c r="E554" t="s">
+        <v>87</v>
+      </c>
+      <c r="F554" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G554" t="s">
+        <v>8</v>
+      </c>
+      <c r="H554" s="3">
+        <v>13225</v>
+      </c>
+      <c r="I554" s="2">
+        <v>124.9</v>
+      </c>
+      <c r="K554" s="4">
+        <f t="shared" si="13"/>
+        <v>-12490</v>
+      </c>
+    </row>
+    <row r="556" spans="1:11">
+      <c r="A556" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C556" t="s">
+        <v>10</v>
+      </c>
+      <c r="D556">
+        <v>-100</v>
+      </c>
+      <c r="E556" t="s">
+        <v>87</v>
+      </c>
+      <c r="F556" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G556" t="s">
+        <v>23</v>
+      </c>
+      <c r="H556" s="3">
+        <v>14200</v>
+      </c>
+      <c r="I556" s="2">
+        <v>84.53</v>
+      </c>
+      <c r="K556" s="4">
+        <f t="shared" si="13"/>
+        <v>-8453</v>
+      </c>
+    </row>
+    <row r="557" spans="1:11">
+      <c r="A557" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C557" t="s">
+        <v>4</v>
+      </c>
+      <c r="D557">
+        <v>100</v>
+      </c>
+      <c r="E557" t="s">
+        <v>87</v>
+      </c>
+      <c r="F557" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G557" t="s">
+        <v>23</v>
+      </c>
+      <c r="H557" s="3">
+        <v>14125</v>
+      </c>
+      <c r="I557" s="2">
+        <v>106.78</v>
+      </c>
+      <c r="K557" s="4">
+        <f t="shared" si="13"/>
+        <v>10678</v>
+      </c>
+    </row>
+    <row r="559" spans="1:11">
+      <c r="A559" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C559" t="s">
+        <v>10</v>
+      </c>
+      <c r="D559">
+        <v>-100</v>
+      </c>
+      <c r="E559" t="s">
+        <v>36</v>
+      </c>
+      <c r="F559" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G559" t="s">
+        <v>23</v>
+      </c>
+      <c r="H559" s="3">
+        <v>2290</v>
+      </c>
+      <c r="I559" s="2">
+        <v>39.9</v>
+      </c>
+      <c r="K559" s="4">
+        <f t="shared" si="13"/>
+        <v>-3990</v>
+      </c>
+    </row>
+    <row r="560" spans="1:11">
+      <c r="A560" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C560" t="s">
+        <v>4</v>
+      </c>
+      <c r="D560">
+        <v>100</v>
+      </c>
+      <c r="E560" t="s">
+        <v>36</v>
+      </c>
+      <c r="F560" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G560" t="s">
+        <v>23</v>
+      </c>
+      <c r="H560" s="3">
+        <v>2300</v>
+      </c>
+      <c r="I560" s="2">
+        <v>34.6</v>
+      </c>
+      <c r="K560" s="4">
+        <f t="shared" si="13"/>
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="562" spans="1:11">
+      <c r="A562" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C562" t="s">
+        <v>4</v>
+      </c>
+      <c r="D562">
+        <v>100</v>
+      </c>
+      <c r="E562" t="s">
+        <v>36</v>
+      </c>
+      <c r="F562" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G562" t="s">
+        <v>8</v>
+      </c>
+      <c r="H562" s="3">
+        <v>2150</v>
+      </c>
+      <c r="I562" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="K562" s="4">
+        <f t="shared" si="13"/>
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="563" spans="1:11">
+      <c r="A563" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C563" t="s">
+        <v>10</v>
+      </c>
+      <c r="D563">
+        <v>-100</v>
+      </c>
+      <c r="E563" t="s">
+        <v>36</v>
+      </c>
+      <c r="F563" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G563" t="s">
+        <v>8</v>
+      </c>
+      <c r="H563" s="3">
+        <v>2135</v>
+      </c>
+      <c r="I563" s="2">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="K563" s="4">
+        <f t="shared" si="13"/>
+        <v>-1614.9999999999998</v>
+      </c>
+    </row>
+    <row r="565" spans="1:11">
+      <c r="A565" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C565" t="s">
+        <v>10</v>
+      </c>
+      <c r="D565">
+        <v>-100</v>
+      </c>
+      <c r="E565" t="s">
+        <v>6</v>
+      </c>
+      <c r="F565" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G565" t="s">
+        <v>8</v>
+      </c>
+      <c r="H565" s="3">
+        <v>4070</v>
+      </c>
+      <c r="I565" s="2">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="K565" s="4">
+        <f t="shared" si="13"/>
+        <v>-3627.0000000000005</v>
+      </c>
+    </row>
+    <row r="566" spans="1:11">
+      <c r="A566" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C566" t="s">
+        <v>4</v>
+      </c>
+      <c r="D566">
+        <v>100</v>
+      </c>
+      <c r="E566" t="s">
+        <v>6</v>
+      </c>
+      <c r="F566" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G566" t="s">
+        <v>8</v>
+      </c>
+      <c r="H566" s="3">
+        <v>4080</v>
+      </c>
+      <c r="I566" s="2">
+        <v>37.82</v>
+      </c>
+      <c r="K566" s="4">
+        <f t="shared" si="13"/>
+        <v>3782</v>
+      </c>
+    </row>
+    <row r="568" spans="1:11">
+      <c r="A568" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C568" t="s">
+        <v>4</v>
+      </c>
+      <c r="D568">
+        <v>100</v>
+      </c>
+      <c r="E568" t="s">
+        <v>6</v>
+      </c>
+      <c r="F568" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G568" t="s">
+        <v>8</v>
+      </c>
+      <c r="H568" s="3">
+        <v>4120</v>
+      </c>
+      <c r="I568" s="2">
+        <v>21.72</v>
+      </c>
+      <c r="K568" s="4">
+        <f t="shared" si="13"/>
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="569" spans="1:11">
+      <c r="A569" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C569" t="s">
+        <v>10</v>
+      </c>
+      <c r="D569">
+        <v>-100</v>
+      </c>
+      <c r="E569" t="s">
+        <v>6</v>
+      </c>
+      <c r="F569" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G569" t="s">
+        <v>8</v>
+      </c>
+      <c r="H569" s="3">
+        <v>4110</v>
+      </c>
+      <c r="I569" s="2">
+        <v>20.37</v>
+      </c>
+      <c r="K569" s="4">
+        <f t="shared" si="13"/>
+        <v>-2037</v>
+      </c>
+    </row>
+    <row r="571" spans="1:11">
+      <c r="A571" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C571" t="s">
+        <v>4</v>
+      </c>
+      <c r="D571">
+        <v>100</v>
+      </c>
+      <c r="E571" t="s">
+        <v>36</v>
+      </c>
+      <c r="F571" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G571" t="s">
+        <v>8</v>
+      </c>
+      <c r="H571" s="3">
+        <v>2170</v>
+      </c>
+      <c r="I571" s="2">
+        <v>13.97</v>
+      </c>
+      <c r="K571" s="4">
+        <f t="shared" si="13"/>
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="572" spans="1:11">
+      <c r="A572" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C572" t="s">
+        <v>10</v>
+      </c>
+      <c r="D572">
+        <v>-100</v>
+      </c>
+      <c r="E572" t="s">
+        <v>36</v>
+      </c>
+      <c r="F572" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G572" t="s">
+        <v>8</v>
+      </c>
+      <c r="H572" s="3">
+        <v>2150</v>
+      </c>
+      <c r="I572" s="2">
+        <v>11.82</v>
+      </c>
+      <c r="K572" s="4">
+        <f t="shared" si="13"/>
+        <v>-1182</v>
+      </c>
+    </row>
+    <row r="574" spans="1:11">
+      <c r="A574" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C574" t="s">
+        <v>4</v>
+      </c>
+      <c r="D574">
+        <v>100</v>
+      </c>
+      <c r="E574" t="s">
+        <v>87</v>
+      </c>
+      <c r="F574" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G574" t="s">
+        <v>23</v>
+      </c>
+      <c r="H574" s="3">
+        <v>14075</v>
+      </c>
+      <c r="I574" s="2">
+        <v>106.15</v>
+      </c>
+      <c r="K574" s="4">
+        <f t="shared" si="13"/>
+        <v>10615</v>
+      </c>
+    </row>
+    <row r="575" spans="1:11">
+      <c r="A575" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B575" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C575" t="s">
+        <v>10</v>
+      </c>
+      <c r="D575">
+        <v>-100</v>
+      </c>
+      <c r="E575" t="s">
+        <v>87</v>
+      </c>
+      <c r="F575" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G575" t="s">
+        <v>23</v>
+      </c>
+      <c r="H575" s="3">
+        <v>14100</v>
+      </c>
+      <c r="I575" s="2">
+        <v>98.15</v>
+      </c>
+      <c r="K575" s="4">
+        <f t="shared" ref="K575:K638" si="14">D575*I575</f>
+        <v>-9815</v>
+      </c>
+    </row>
+    <row r="577" spans="1:11">
+      <c r="A577" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B577" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C577" t="s">
+        <v>10</v>
+      </c>
+      <c r="D577">
+        <v>-100</v>
+      </c>
+      <c r="E577" t="s">
+        <v>36</v>
+      </c>
+      <c r="F577" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G577" t="s">
+        <v>23</v>
+      </c>
+      <c r="H577" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I577" s="2">
+        <v>38.26</v>
+      </c>
+      <c r="K577" s="4">
+        <f t="shared" si="14"/>
+        <v>-3826</v>
+      </c>
+    </row>
+    <row r="578" spans="1:11">
+      <c r="A578" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C578" t="s">
+        <v>4</v>
+      </c>
+      <c r="D578">
+        <v>100</v>
+      </c>
+      <c r="E578" t="s">
+        <v>36</v>
+      </c>
+      <c r="F578" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G578" t="s">
+        <v>23</v>
+      </c>
+      <c r="H578" s="3">
+        <v>2340</v>
+      </c>
+      <c r="I578" s="2">
+        <v>23.41</v>
+      </c>
+      <c r="K578" s="4">
+        <f t="shared" si="14"/>
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="580" spans="1:11">
+      <c r="A580" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C580" t="s">
+        <v>4</v>
+      </c>
+      <c r="D580">
+        <v>100</v>
+      </c>
+      <c r="E580" t="s">
+        <v>20</v>
+      </c>
+      <c r="F580" s="1">
+        <v>44400</v>
+      </c>
+      <c r="G580" t="s">
+        <v>8</v>
+      </c>
+      <c r="H580" s="3">
+        <v>230</v>
+      </c>
+      <c r="I580" s="2">
+        <v>1.82</v>
+      </c>
+      <c r="K580" s="4">
+        <f t="shared" si="14"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="581" spans="1:11">
+      <c r="A581" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C581" t="s">
+        <v>10</v>
+      </c>
+      <c r="D581">
+        <v>-100</v>
+      </c>
+      <c r="E581" t="s">
+        <v>20</v>
+      </c>
+      <c r="F581" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G581" t="s">
+        <v>8</v>
+      </c>
+      <c r="H581" s="3">
+        <v>220</v>
+      </c>
+      <c r="I581" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="K581" s="4">
+        <f t="shared" si="14"/>
+        <v>-69</v>
+      </c>
+    </row>
+    <row r="583" spans="1:11">
+      <c r="A583" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B583" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C583" t="s">
+        <v>4</v>
+      </c>
+      <c r="D583">
+        <v>100</v>
+      </c>
+      <c r="E583" t="s">
+        <v>87</v>
+      </c>
+      <c r="F583" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G583" t="s">
+        <v>8</v>
+      </c>
+      <c r="H583" s="3">
+        <v>13575</v>
+      </c>
+      <c r="I583" s="2">
+        <v>175.6</v>
+      </c>
+      <c r="K583" s="4">
+        <f t="shared" si="14"/>
+        <v>17560</v>
+      </c>
+    </row>
+    <row r="584" spans="1:11">
+      <c r="A584" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B584" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C584" t="s">
+        <v>10</v>
+      </c>
+      <c r="D584">
+        <v>-100</v>
+      </c>
+      <c r="E584" t="s">
+        <v>87</v>
+      </c>
+      <c r="F584" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G584" t="s">
+        <v>8</v>
+      </c>
+      <c r="H584" s="3">
+        <v>13400</v>
+      </c>
+      <c r="I584" s="2">
+        <v>132.6</v>
+      </c>
+      <c r="K584" s="4">
+        <f t="shared" si="14"/>
+        <v>-13260</v>
+      </c>
+    </row>
+    <row r="586" spans="1:11">
+      <c r="A586" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B586" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C586" t="s">
+        <v>10</v>
+      </c>
+      <c r="D586">
+        <v>-100</v>
+      </c>
+      <c r="E586" t="s">
+        <v>240</v>
+      </c>
+      <c r="F586" s="1">
+        <v>44428</v>
+      </c>
+      <c r="G586" t="s">
+        <v>23</v>
+      </c>
+      <c r="H586" s="3">
+        <v>16</v>
+      </c>
+      <c r="I586" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="K586" s="4">
+        <f t="shared" si="14"/>
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="587" spans="1:11">
+      <c r="A587" s="1">
+        <v>44355</v>
+      </c>
+      <c r="B587" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C587" t="s">
+        <v>4</v>
+      </c>
+      <c r="D587">
+        <v>100</v>
+      </c>
+      <c r="E587" t="s">
+        <v>240</v>
+      </c>
+      <c r="G587" t="s">
+        <v>40</v>
+      </c>
+      <c r="I587" s="2">
+        <v>15.69</v>
+      </c>
+      <c r="K587" s="4">
+        <f t="shared" si="14"/>
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="589" spans="1:11">
+      <c r="A589" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B589" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C589" t="s">
+        <v>4</v>
+      </c>
+      <c r="D589">
+        <v>100</v>
+      </c>
+      <c r="E589" t="s">
+        <v>36</v>
+      </c>
+      <c r="F589" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G589" t="s">
+        <v>23</v>
+      </c>
+      <c r="H589" s="3">
+        <v>2290</v>
+      </c>
+      <c r="I589" s="2">
+        <v>71.180000000000007</v>
+      </c>
+      <c r="K589" s="4">
+        <f t="shared" si="14"/>
+        <v>7118.0000000000009</v>
+      </c>
+    </row>
+    <row r="590" spans="1:11">
+      <c r="A590" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C590" t="s">
+        <v>4</v>
+      </c>
+      <c r="D590">
+        <v>100</v>
+      </c>
+      <c r="E590" t="s">
+        <v>36</v>
+      </c>
+      <c r="F590" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G590" t="s">
+        <v>23</v>
+      </c>
+      <c r="H590" s="3">
+        <v>2310</v>
+      </c>
+      <c r="I590" s="2">
+        <v>56.74</v>
+      </c>
+      <c r="K590" s="4">
+        <f t="shared" si="14"/>
+        <v>5674</v>
+      </c>
+    </row>
+    <row r="591" spans="1:11">
+      <c r="A591" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C591" t="s">
+        <v>10</v>
+      </c>
+      <c r="D591">
+        <v>-200</v>
+      </c>
+      <c r="E591" t="s">
+        <v>36</v>
+      </c>
+      <c r="F591" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G591" t="s">
+        <v>23</v>
+      </c>
+      <c r="H591" s="3">
+        <v>2300</v>
+      </c>
+      <c r="I591" s="2">
+        <v>63.86</v>
+      </c>
+      <c r="K591" s="4">
+        <f t="shared" si="14"/>
+        <v>-12772</v>
+      </c>
+    </row>
+    <row r="593" spans="1:11">
+      <c r="A593" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C593" t="s">
+        <v>10</v>
+      </c>
+      <c r="D593">
+        <v>-100</v>
+      </c>
+      <c r="E593" t="s">
+        <v>87</v>
+      </c>
+      <c r="F593" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G593" t="s">
+        <v>23</v>
+      </c>
+      <c r="H593" s="3">
+        <v>14075</v>
+      </c>
+      <c r="I593" s="2">
+        <v>140.81</v>
+      </c>
+      <c r="K593" s="4">
+        <f t="shared" si="14"/>
+        <v>-14081</v>
+      </c>
+    </row>
+    <row r="594" spans="1:11">
+      <c r="A594" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C594" t="s">
+        <v>4</v>
+      </c>
+      <c r="D594">
+        <v>100</v>
+      </c>
+      <c r="E594" t="s">
+        <v>87</v>
+      </c>
+      <c r="F594" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G594" t="s">
+        <v>23</v>
+      </c>
+      <c r="H594" s="3">
+        <v>14200</v>
+      </c>
+      <c r="I594" s="2">
+        <v>95.93</v>
+      </c>
+      <c r="K594" s="4">
+        <f t="shared" si="14"/>
+        <v>9593</v>
+      </c>
+    </row>
+    <row r="595" spans="1:11">
+      <c r="A595" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C595" t="s">
+        <v>10</v>
+      </c>
+      <c r="D595">
+        <v>-100</v>
+      </c>
+      <c r="E595" t="s">
+        <v>87</v>
+      </c>
+      <c r="F595" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G595" t="s">
+        <v>8</v>
+      </c>
+      <c r="H595" s="3">
+        <v>13575</v>
+      </c>
+      <c r="I595" s="2">
+        <v>159.57</v>
+      </c>
+      <c r="K595" s="4">
+        <f t="shared" si="14"/>
+        <v>-15957</v>
+      </c>
+    </row>
+    <row r="596" spans="1:11">
+      <c r="A596" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C596" t="s">
+        <v>4</v>
+      </c>
+      <c r="D596">
+        <v>100</v>
+      </c>
+      <c r="E596" t="s">
+        <v>87</v>
+      </c>
+      <c r="F596" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G596" t="s">
+        <v>8</v>
+      </c>
+      <c r="H596" s="3">
+        <v>13075</v>
+      </c>
+      <c r="I596" s="2">
+        <v>73.2</v>
+      </c>
+      <c r="K596" s="4">
+        <f t="shared" si="14"/>
+        <v>7320</v>
+      </c>
+    </row>
+    <row r="598" spans="1:11">
+      <c r="A598" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C598" t="s">
+        <v>4</v>
+      </c>
+      <c r="D598">
+        <v>200</v>
+      </c>
+      <c r="E598" t="s">
+        <v>6</v>
+      </c>
+      <c r="F598" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G598" t="s">
+        <v>8</v>
+      </c>
+      <c r="H598" s="3">
+        <v>4220</v>
+      </c>
+      <c r="I598" s="2">
+        <v>10.73</v>
+      </c>
+      <c r="K598" s="4">
+        <f t="shared" si="14"/>
+        <v>2146</v>
+      </c>
+    </row>
+    <row r="599" spans="1:11">
+      <c r="A599" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C599" t="s">
+        <v>10</v>
+      </c>
+      <c r="D599">
+        <v>-100</v>
+      </c>
+      <c r="E599" t="s">
+        <v>6</v>
+      </c>
+      <c r="F599" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G599" t="s">
+        <v>8</v>
+      </c>
+      <c r="H599" s="3">
+        <v>4230</v>
+      </c>
+      <c r="I599" s="2">
+        <v>14.18</v>
+      </c>
+      <c r="K599" s="4">
+        <f t="shared" si="14"/>
+        <v>-1418</v>
+      </c>
+    </row>
+    <row r="600" spans="1:11">
+      <c r="A600" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C600" t="s">
+        <v>10</v>
+      </c>
+      <c r="D600">
+        <v>-100</v>
+      </c>
+      <c r="E600" t="s">
+        <v>6</v>
+      </c>
+      <c r="F600" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G600" t="s">
+        <v>8</v>
+      </c>
+      <c r="H600" s="3">
+        <v>4195</v>
+      </c>
+      <c r="I600" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="K600" s="4">
+        <f t="shared" si="14"/>
+        <v>-563</v>
+      </c>
+    </row>
+    <row r="602" spans="1:11">
+      <c r="A602" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C602" t="s">
+        <v>4</v>
+      </c>
+      <c r="D602">
+        <v>100</v>
+      </c>
+      <c r="E602" t="s">
+        <v>6</v>
+      </c>
+      <c r="F602" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G602" t="s">
+        <v>8</v>
+      </c>
+      <c r="H602" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I602" s="2">
+        <v>46.5</v>
+      </c>
+      <c r="K602" s="4">
+        <f t="shared" si="14"/>
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="603" spans="1:11">
+      <c r="A603" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C603" t="s">
+        <v>10</v>
+      </c>
+      <c r="D603">
+        <v>-100</v>
+      </c>
+      <c r="E603" t="s">
+        <v>6</v>
+      </c>
+      <c r="F603" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G603" t="s">
+        <v>8</v>
+      </c>
+      <c r="H603" s="3">
+        <v>4080</v>
+      </c>
+      <c r="I603" s="2">
+        <v>34.1</v>
+      </c>
+      <c r="K603" s="4">
+        <f t="shared" si="14"/>
+        <v>-3410</v>
+      </c>
+    </row>
+    <row r="605" spans="1:11">
+      <c r="A605" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B605" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C605" t="s">
+        <v>10</v>
+      </c>
+      <c r="D605">
+        <v>-100</v>
+      </c>
+      <c r="E605" t="s">
+        <v>36</v>
+      </c>
+      <c r="F605" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G605" t="s">
+        <v>8</v>
+      </c>
+      <c r="H605" s="3">
+        <v>2170</v>
+      </c>
+      <c r="I605" s="2">
+        <v>10.41</v>
+      </c>
+      <c r="K605" s="4">
+        <f t="shared" si="14"/>
+        <v>-1041</v>
+      </c>
+    </row>
+    <row r="606" spans="1:11">
+      <c r="A606" s="1">
+        <v>44356</v>
+      </c>
+      <c r="B606" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C606" t="s">
+        <v>4</v>
+      </c>
+      <c r="D606">
+        <v>100</v>
+      </c>
+      <c r="E606" t="s">
+        <v>36</v>
+      </c>
+      <c r="F606" s="1">
+        <v>44386</v>
+      </c>
+      <c r="G606" t="s">
+        <v>8</v>
+      </c>
+      <c r="H606" s="3">
+        <v>2200</v>
+      </c>
+      <c r="I606" s="2">
+        <v>17.36</v>
+      </c>
+      <c r="K606" s="4">
+        <f t="shared" si="14"/>
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="608" spans="1:11">
+      <c r="A608" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B608" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C608" t="s">
+        <v>10</v>
+      </c>
+      <c r="D608">
+        <v>-200</v>
+      </c>
+      <c r="E608" t="s">
+        <v>6</v>
+      </c>
+      <c r="F608" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G608" t="s">
+        <v>8</v>
+      </c>
+      <c r="H608" s="3">
+        <v>4220</v>
+      </c>
+      <c r="I608" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="K608" s="4">
+        <f t="shared" si="14"/>
+        <v>-903.99999999999989</v>
+      </c>
+    </row>
+    <row r="609" spans="1:11">
+      <c r="A609" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B609" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C609" t="s">
+        <v>4</v>
+      </c>
+      <c r="D609">
+        <v>100</v>
+      </c>
+      <c r="E609" t="s">
+        <v>6</v>
+      </c>
+      <c r="F609" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G609" t="s">
+        <v>8</v>
+      </c>
+      <c r="H609" s="3">
+        <v>4230</v>
+      </c>
+      <c r="I609" s="2">
+        <v>6.49</v>
+      </c>
+      <c r="K609" s="4">
+        <f t="shared" si="14"/>
+        <v>649</v>
+      </c>
+    </row>
+    <row r="610" spans="1:11">
+      <c r="A610" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B610" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C610" t="s">
+        <v>4</v>
+      </c>
+      <c r="D610">
+        <v>100</v>
+      </c>
+      <c r="E610" t="s">
+        <v>6</v>
+      </c>
+      <c r="F610" s="1">
+        <v>44358</v>
+      </c>
+      <c r="G610" t="s">
+        <v>8</v>
+      </c>
+      <c r="H610" s="3">
+        <v>4195</v>
+      </c>
+      <c r="I610" s="2">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K610" s="4">
+        <f t="shared" si="14"/>
+        <v>204.99999999999997</v>
+      </c>
+    </row>
+    <row r="612" spans="1:11">
+      <c r="A612" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B612" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C612" t="s">
+        <v>4</v>
+      </c>
+      <c r="D612">
+        <v>100</v>
+      </c>
+      <c r="E612" t="s">
+        <v>43</v>
+      </c>
+      <c r="F612" s="1">
+        <v>44428</v>
+      </c>
+      <c r="G612" t="s">
+        <v>8</v>
+      </c>
+      <c r="H612" s="3">
+        <v>125</v>
+      </c>
+      <c r="I612" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K612" s="4">
+        <f t="shared" si="14"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="613" spans="1:11">
+      <c r="A613" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B613" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C613" t="s">
+        <v>10</v>
+      </c>
+      <c r="D613">
+        <v>-100</v>
+      </c>
+      <c r="E613" t="s">
+        <v>43</v>
+      </c>
+      <c r="F613" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G613" t="s">
+        <v>8</v>
+      </c>
+      <c r="H613" s="3">
+        <v>130</v>
+      </c>
+      <c r="I613" s="2">
+        <v>3.59</v>
+      </c>
+      <c r="K613" s="4">
+        <f t="shared" si="14"/>
+        <v>-359</v>
+      </c>
+    </row>
+    <row r="615" spans="1:11">
+      <c r="A615" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B615" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C615" t="s">
+        <v>10</v>
+      </c>
+      <c r="D615">
+        <v>-100</v>
+      </c>
+      <c r="E615" t="s">
+        <v>74</v>
+      </c>
+      <c r="F615" s="1">
+        <v>44484</v>
+      </c>
+      <c r="G615" t="s">
+        <v>8</v>
+      </c>
+      <c r="H615" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="I615" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K615" s="4">
+        <f t="shared" si="14"/>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="617" spans="1:11">
+      <c r="A617" s="1">
+        <v>44357</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C617" t="s">
+        <v>4</v>
+      </c>
+      <c r="D617">
+        <v>100</v>
+      </c>
+      <c r="E617" t="s">
+        <v>251</v>
+      </c>
+      <c r="F617" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G617" t="s">
+        <v>8</v>
+      </c>
+      <c r="H617" s="3">
+        <v>29</v>
+      </c>
+      <c r="I617" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="K617" s="4">
+        <f t="shared" si="14"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="619" spans="1:11">
+      <c r="A619" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C619" t="s">
+        <v>4</v>
+      </c>
+      <c r="D619">
+        <v>100</v>
+      </c>
+      <c r="E619" t="s">
+        <v>253</v>
+      </c>
+      <c r="F619" s="1">
+        <v>44400</v>
+      </c>
+      <c r="G619" t="s">
+        <v>8</v>
+      </c>
+      <c r="H619" s="3">
+        <v>134</v>
+      </c>
+      <c r="I619" s="2">
+        <v>1.45</v>
+      </c>
+      <c r="K619" s="4">
+        <f t="shared" si="14"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="621" spans="1:11">
+      <c r="A621" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C621" t="s">
+        <v>10</v>
+      </c>
+      <c r="D621">
+        <v>-100</v>
+      </c>
+      <c r="E621" t="s">
+        <v>36</v>
+      </c>
+      <c r="F621" s="1">
+        <v>44386</v>
+      </c>
+      <c r="G621" t="s">
+        <v>8</v>
+      </c>
+      <c r="H621" s="3">
+        <v>2200</v>
+      </c>
+      <c r="I621" s="2">
+        <v>15.82</v>
+      </c>
+      <c r="K621" s="4">
+        <f t="shared" si="14"/>
+        <v>-1582</v>
+      </c>
+    </row>
+    <row r="623" spans="1:11">
+      <c r="A623" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C623" t="s">
+        <v>4</v>
+      </c>
+      <c r="D623">
+        <v>100</v>
+      </c>
+      <c r="E623" t="s">
+        <v>36</v>
+      </c>
+      <c r="F623" s="1">
+        <v>44379</v>
+      </c>
+      <c r="G623" t="s">
+        <v>8</v>
+      </c>
+      <c r="H623" s="3">
+        <v>2135</v>
+      </c>
+      <c r="I623" s="2">
+        <v>6.85</v>
+      </c>
+      <c r="K623" s="4">
+        <f t="shared" si="14"/>
+        <v>685</v>
+      </c>
+    </row>
+    <row r="624" spans="1:11">
+      <c r="A624" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C624" t="s">
+        <v>10</v>
+      </c>
+      <c r="D624">
+        <v>-100</v>
+      </c>
+      <c r="E624" t="s">
+        <v>36</v>
+      </c>
+      <c r="F624" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G624" t="s">
+        <v>8</v>
+      </c>
+      <c r="H624" s="3">
+        <v>2135</v>
+      </c>
+      <c r="I624" s="2">
+        <v>4.05</v>
+      </c>
+      <c r="K624" s="4">
+        <f t="shared" si="14"/>
+        <v>-405</v>
+      </c>
+    </row>
+    <row r="626" spans="1:11">
+      <c r="A626" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B626" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C626" t="s">
+        <v>10</v>
+      </c>
+      <c r="D626">
+        <v>-100</v>
+      </c>
+      <c r="E626" t="s">
+        <v>6</v>
+      </c>
+      <c r="F626" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G626" t="s">
+        <v>8</v>
+      </c>
+      <c r="H626" s="3">
+        <v>4120</v>
+      </c>
+      <c r="I626" s="2">
+        <v>12.15</v>
+      </c>
+      <c r="K626" s="4">
+        <f t="shared" si="14"/>
+        <v>-1215</v>
+      </c>
+    </row>
+    <row r="627" spans="1:11">
+      <c r="A627" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B627" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C627" t="s">
+        <v>4</v>
+      </c>
+      <c r="D627">
+        <v>100</v>
+      </c>
+      <c r="E627" t="s">
+        <v>6</v>
+      </c>
+      <c r="F627" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G627" t="s">
+        <v>8</v>
+      </c>
+      <c r="H627" s="3">
+        <v>4020</v>
+      </c>
+      <c r="I627" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K627" s="4">
+        <f t="shared" si="14"/>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="629" spans="1:11">
+      <c r="A629" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C629" t="s">
+        <v>10</v>
+      </c>
+      <c r="D629">
+        <v>-100</v>
+      </c>
+      <c r="E629" t="s">
+        <v>6</v>
+      </c>
+      <c r="F629" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G629" t="s">
+        <v>8</v>
+      </c>
+      <c r="H629" s="3">
+        <v>4150</v>
+      </c>
+      <c r="I629" s="2">
+        <v>37.340000000000003</v>
+      </c>
+      <c r="K629" s="4">
+        <f t="shared" si="14"/>
+        <v>-3734.0000000000005</v>
+      </c>
+    </row>
+    <row r="630" spans="1:11">
+      <c r="A630" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C630" t="s">
+        <v>4</v>
+      </c>
+      <c r="D630">
+        <v>100</v>
+      </c>
+      <c r="E630" t="s">
+        <v>6</v>
+      </c>
+      <c r="F630" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G630" t="s">
+        <v>8</v>
+      </c>
+      <c r="H630" s="3">
+        <v>4000</v>
+      </c>
+      <c r="I630" s="2">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="K630" s="4">
+        <f t="shared" si="14"/>
+        <v>1894.0000000000002</v>
+      </c>
+    </row>
+    <row r="632" spans="1:11">
+      <c r="A632" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C632" t="s">
+        <v>4</v>
+      </c>
+      <c r="D632">
+        <v>100</v>
+      </c>
+      <c r="E632" t="s">
+        <v>36</v>
+      </c>
+      <c r="F632" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G632" t="s">
+        <v>8</v>
+      </c>
+      <c r="H632" s="3">
+        <v>2230</v>
+      </c>
+      <c r="I632" s="2">
+        <v>7.82</v>
+      </c>
+      <c r="K632" s="4">
+        <f t="shared" si="14"/>
+        <v>782</v>
+      </c>
+    </row>
+    <row r="633" spans="1:11">
+      <c r="A633" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C633" t="s">
+        <v>10</v>
+      </c>
+      <c r="D633">
+        <v>-100</v>
+      </c>
+      <c r="E633" t="s">
+        <v>36</v>
+      </c>
+      <c r="F633" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G633" t="s">
+        <v>8</v>
+      </c>
+      <c r="H633" s="3">
+        <v>2140</v>
+      </c>
+      <c r="I633" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="K633" s="4">
+        <f t="shared" si="14"/>
+        <v>-332</v>
+      </c>
+    </row>
+    <row r="635" spans="1:11">
+      <c r="A635" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C635" t="s">
+        <v>10</v>
+      </c>
+      <c r="D635">
+        <v>-100</v>
+      </c>
+      <c r="E635" t="s">
+        <v>20</v>
+      </c>
+      <c r="F635" s="1">
+        <v>44400</v>
+      </c>
+      <c r="G635" t="s">
+        <v>8</v>
+      </c>
+      <c r="H635" s="3">
+        <v>230</v>
+      </c>
+      <c r="I635" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="K635" s="4">
+        <f t="shared" si="14"/>
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="636" spans="1:11">
+      <c r="A636" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C636" t="s">
+        <v>4</v>
+      </c>
+      <c r="D636">
+        <v>100</v>
+      </c>
+      <c r="E636" t="s">
+        <v>20</v>
+      </c>
+      <c r="F636" s="1">
+        <v>44407</v>
+      </c>
+      <c r="G636" t="s">
+        <v>8</v>
+      </c>
+      <c r="H636" s="3">
+        <v>237.5</v>
+      </c>
+      <c r="I636" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="K636" s="4">
+        <f t="shared" si="14"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="638" spans="1:11">
+      <c r="A638" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B638" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C638" t="s">
+        <v>10</v>
+      </c>
+      <c r="D638">
+        <v>-100</v>
+      </c>
+      <c r="E638" t="s">
+        <v>43</v>
+      </c>
+      <c r="F638" s="1">
+        <v>44428</v>
+      </c>
+      <c r="G638" t="s">
+        <v>8</v>
+      </c>
+      <c r="H638" s="3">
+        <v>125</v>
+      </c>
+      <c r="I638" s="2">
+        <v>3.57</v>
+      </c>
+      <c r="K638" s="4">
+        <f t="shared" si="14"/>
+        <v>-357</v>
+      </c>
+    </row>
+    <row r="639" spans="1:11">
+      <c r="A639" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B639" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C639" t="s">
+        <v>4</v>
+      </c>
+      <c r="D639">
+        <v>100</v>
+      </c>
+      <c r="E639" t="s">
+        <v>43</v>
+      </c>
+      <c r="F639" s="1">
+        <v>44456</v>
+      </c>
+      <c r="G639" t="s">
+        <v>8</v>
+      </c>
+      <c r="H639" s="3">
+        <v>125</v>
+      </c>
+      <c r="I639" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K639" s="4">
+        <f t="shared" ref="K639:K642" si="15">D639*I639</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="641" spans="1:12">
+      <c r="A641" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B641" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C641" t="s">
+        <v>4</v>
+      </c>
+      <c r="D641">
+        <v>100</v>
+      </c>
+      <c r="E641" t="s">
+        <v>262</v>
+      </c>
+      <c r="F641" s="1">
+        <v>44407</v>
+      </c>
+      <c r="G641" t="s">
+        <v>23</v>
+      </c>
+      <c r="H641" s="3">
+        <v>434</v>
+      </c>
+      <c r="I641" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="K641" s="4">
+        <f t="shared" si="15"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="642" spans="1:12">
+      <c r="A642" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B642" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C642" t="s">
+        <v>10</v>
+      </c>
+      <c r="D642">
+        <v>-100</v>
+      </c>
+      <c r="E642" t="s">
+        <v>262</v>
+      </c>
+      <c r="F642" s="1">
+        <v>44407</v>
+      </c>
+      <c r="G642" t="s">
+        <v>23</v>
+      </c>
+      <c r="H642" s="3">
+        <v>439</v>
+      </c>
+      <c r="I642" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="K642" s="4">
+        <f t="shared" si="15"/>
+        <v>-136</v>
+      </c>
+    </row>
+    <row r="643" spans="1:12">
+      <c r="L643" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M3"/>
@@ -14007,11 +16467,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14401,24 +16861,106 @@
       <c r="A10" s="1">
         <v>44361</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18">
-        <f>SUM(N2:N14)</f>
-        <v>9287</v>
+      <c r="B10" s="6">
+        <v>87185.85</v>
+      </c>
+      <c r="C10" s="13">
+        <v>-451.99</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1076.28</v>
+      </c>
+      <c r="E10" s="5">
+        <v>198</v>
+      </c>
+      <c r="F10" s="5">
+        <v>65</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>95385.87</v>
+      </c>
+      <c r="I10" s="6">
+        <v>47692.94</v>
+      </c>
+      <c r="J10" s="13">
+        <v>48645.62</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6">
+        <v>58200.78</v>
+      </c>
+      <c r="N10" s="13">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B11" s="6">
+        <v>87213.3</v>
+      </c>
+      <c r="C11" s="13">
+        <v>-424.54</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1103.73</v>
+      </c>
+      <c r="E11" s="5">
+        <v>187</v>
+      </c>
+      <c r="F11" s="5">
+        <v>59</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>95174.399999999994</v>
+      </c>
+      <c r="I11" s="6">
+        <v>47587.199999999997</v>
+      </c>
+      <c r="J11" s="13">
+        <v>48645.62</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>58200.78</v>
+      </c>
+      <c r="N11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1">
+        <v>44363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18">
+        <f>SUM(N2:N16)</f>
+        <v>9432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 17-Jun-2021, end of day.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trades" sheetId="1" r:id="rId1"/>
@@ -1195,9 +1195,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O643"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D643" sqref="D643"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A641" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D664" sqref="D664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16467,18 +16467,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="11.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
@@ -16943,24 +16944,60 @@
       <c r="A12" s="1">
         <v>44363</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18">
-        <f>SUM(N2:N16)</f>
-        <v>9432</v>
+      <c r="B12" s="6">
+        <v>86339.82</v>
+      </c>
+      <c r="C12" s="13">
+        <v>-1021.23</v>
+      </c>
+      <c r="D12" s="13">
+        <v>234.43</v>
+      </c>
+      <c r="E12" s="5">
+        <v>452</v>
+      </c>
+      <c r="F12" s="5">
+        <v>60</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>68985.86</v>
+      </c>
+      <c r="I12" s="6">
+        <v>34492.93</v>
+      </c>
+      <c r="J12" s="13">
+        <v>51258.37</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>57346.79</v>
+      </c>
+      <c r="N12" s="13">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18">
+        <f>SUM(N2:N17)</f>
+        <v>9611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 18-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -16471,7 +16471,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16981,6 +16981,47 @@
         <v>179</v>
       </c>
     </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B13" s="6">
+        <v>86563</v>
+      </c>
+      <c r="C13" s="13">
+        <v>188.54</v>
+      </c>
+      <c r="D13" s="13">
+        <v>458.97</v>
+      </c>
+      <c r="E13" s="5">
+        <v>468</v>
+      </c>
+      <c r="F13" s="5">
+        <v>67</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>70016.899999999994</v>
+      </c>
+      <c r="I13" s="6">
+        <v>35008.449999999997</v>
+      </c>
+      <c r="J13" s="13">
+        <v>51308.52</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>44180.4</v>
+      </c>
+      <c r="N13" s="13">
+        <v>36</v>
+      </c>
+    </row>
     <row r="18" spans="1:14">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
@@ -16997,7 +17038,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="18">
         <f>SUM(N2:N17)</f>
-        <v>9611</v>
+        <v>9647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 23-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Trades" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="273">
   <si>
     <t>Date</t>
   </si>
@@ -808,6 +808,36 @@
   </si>
   <si>
     <t>SPY</t>
+  </si>
+  <si>
+    <t>1556-23305</t>
+  </si>
+  <si>
+    <t>1556-30375</t>
+  </si>
+  <si>
+    <t>1556-39276</t>
+  </si>
+  <si>
+    <t>1562-41847</t>
+  </si>
+  <si>
+    <t>1562-58024</t>
+  </si>
+  <si>
+    <t>1562-62576</t>
+  </si>
+  <si>
+    <t>1566-55971</t>
+  </si>
+  <si>
+    <t>1568-38074</t>
+  </si>
+  <si>
+    <t>1568-40055</t>
+  </si>
+  <si>
+    <t>1568-42473</t>
   </si>
 </sst>
 </file>
@@ -1193,11 +1223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O643"/>
+  <dimension ref="A1:O671"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A641" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D664" sqref="D664"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A669" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A692" sqref="A692"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16382,7 +16412,7 @@
         <v>4.5</v>
       </c>
       <c r="K639" s="4">
-        <f t="shared" ref="K639:K642" si="15">D639*I639</f>
+        <f t="shared" ref="K639:K671" si="15">D639*I639</f>
         <v>450</v>
       </c>
     </row>
@@ -16454,6 +16484,666 @@
     </row>
     <row r="643" spans="1:12">
       <c r="L643" s="6"/>
+    </row>
+    <row r="644" spans="1:12">
+      <c r="A644" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B644" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C644" t="s">
+        <v>10</v>
+      </c>
+      <c r="D644">
+        <v>-100</v>
+      </c>
+      <c r="E644" t="s">
+        <v>6</v>
+      </c>
+      <c r="F644" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G644" t="s">
+        <v>8</v>
+      </c>
+      <c r="H644" s="3">
+        <v>4000</v>
+      </c>
+      <c r="I644" s="2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="K644" s="4">
+        <f t="shared" si="15"/>
+        <v>-1739.9999999999998</v>
+      </c>
+    </row>
+    <row r="645" spans="1:12">
+      <c r="A645" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B645" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C645" t="s">
+        <v>4</v>
+      </c>
+      <c r="D645">
+        <v>100</v>
+      </c>
+      <c r="E645" t="s">
+        <v>6</v>
+      </c>
+      <c r="F645" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G645" t="s">
+        <v>8</v>
+      </c>
+      <c r="H645" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I645" s="2">
+        <v>45.4</v>
+      </c>
+      <c r="K645" s="4">
+        <f t="shared" si="15"/>
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="647" spans="1:12">
+      <c r="A647" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B647" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C647" t="s">
+        <v>10</v>
+      </c>
+      <c r="D647">
+        <v>-100</v>
+      </c>
+      <c r="E647" t="s">
+        <v>36</v>
+      </c>
+      <c r="F647" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G647" t="s">
+        <v>8</v>
+      </c>
+      <c r="H647" s="3">
+        <v>2180</v>
+      </c>
+      <c r="I647" s="2">
+        <v>5.97</v>
+      </c>
+      <c r="K647" s="4">
+        <f t="shared" si="15"/>
+        <v>-597</v>
+      </c>
+    </row>
+    <row r="648" spans="1:12">
+      <c r="A648" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C648" t="s">
+        <v>4</v>
+      </c>
+      <c r="D648">
+        <v>100</v>
+      </c>
+      <c r="E648" t="s">
+        <v>36</v>
+      </c>
+      <c r="F648" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G648" t="s">
+        <v>8</v>
+      </c>
+      <c r="H648" s="3">
+        <v>2135</v>
+      </c>
+      <c r="I648" s="2">
+        <v>3.99</v>
+      </c>
+      <c r="K648" s="4">
+        <f t="shared" si="15"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="650" spans="1:12">
+      <c r="A650" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B650" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C650" t="s">
+        <v>10</v>
+      </c>
+      <c r="D650">
+        <v>-100</v>
+      </c>
+      <c r="E650" t="s">
+        <v>36</v>
+      </c>
+      <c r="F650" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G650" t="s">
+        <v>8</v>
+      </c>
+      <c r="H650" s="3">
+        <v>2220</v>
+      </c>
+      <c r="I650" s="2">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="K650" s="4">
+        <f t="shared" si="15"/>
+        <v>-1842.0000000000002</v>
+      </c>
+    </row>
+    <row r="651" spans="1:12">
+      <c r="A651" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B651" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C651" t="s">
+        <v>4</v>
+      </c>
+      <c r="D651">
+        <v>100</v>
+      </c>
+      <c r="E651" t="s">
+        <v>36</v>
+      </c>
+      <c r="F651" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G651" t="s">
+        <v>8</v>
+      </c>
+      <c r="H651" s="3">
+        <v>2180</v>
+      </c>
+      <c r="I651" s="2">
+        <v>9.83</v>
+      </c>
+      <c r="K651" s="4">
+        <f t="shared" si="15"/>
+        <v>983</v>
+      </c>
+    </row>
+    <row r="653" spans="1:12">
+      <c r="A653" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B653" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C653" t="s">
+        <v>10</v>
+      </c>
+      <c r="D653">
+        <v>-100</v>
+      </c>
+      <c r="E653" t="s">
+        <v>36</v>
+      </c>
+      <c r="F653" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G653" t="s">
+        <v>23</v>
+      </c>
+      <c r="H653" s="3">
+        <v>2340</v>
+      </c>
+      <c r="I653" s="2">
+        <v>4.82</v>
+      </c>
+      <c r="K653" s="4">
+        <f t="shared" si="15"/>
+        <v>-482</v>
+      </c>
+    </row>
+    <row r="654" spans="1:12">
+      <c r="A654" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B654" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C654" t="s">
+        <v>4</v>
+      </c>
+      <c r="D654">
+        <v>100</v>
+      </c>
+      <c r="E654" t="s">
+        <v>36</v>
+      </c>
+      <c r="F654" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G654" t="s">
+        <v>23</v>
+      </c>
+      <c r="H654" s="3">
+        <v>2325</v>
+      </c>
+      <c r="I654" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="K654" s="4">
+        <f t="shared" si="15"/>
+        <v>682</v>
+      </c>
+    </row>
+    <row r="656" spans="1:12">
+      <c r="A656" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B656" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C656" t="s">
+        <v>10</v>
+      </c>
+      <c r="D656">
+        <v>-100</v>
+      </c>
+      <c r="E656" t="s">
+        <v>6</v>
+      </c>
+      <c r="F656" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G656" t="s">
+        <v>8</v>
+      </c>
+      <c r="H656" s="3">
+        <v>4210</v>
+      </c>
+      <c r="I656" s="2">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="K656" s="4">
+        <f t="shared" si="15"/>
+        <v>-7459.9999999999991</v>
+      </c>
+    </row>
+    <row r="657" spans="1:11">
+      <c r="A657" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B657" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C657" t="s">
+        <v>4</v>
+      </c>
+      <c r="D657">
+        <v>100</v>
+      </c>
+      <c r="E657" t="s">
+        <v>6</v>
+      </c>
+      <c r="F657" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G657" t="s">
+        <v>8</v>
+      </c>
+      <c r="H657" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I657" s="2">
+        <v>70.55</v>
+      </c>
+      <c r="K657" s="4">
+        <f t="shared" si="15"/>
+        <v>7055</v>
+      </c>
+    </row>
+    <row r="659" spans="1:11">
+      <c r="A659" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B659" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C659" t="s">
+        <v>4</v>
+      </c>
+      <c r="D659">
+        <v>100</v>
+      </c>
+      <c r="E659" t="s">
+        <v>6</v>
+      </c>
+      <c r="F659" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G659" t="s">
+        <v>8</v>
+      </c>
+      <c r="H659" s="3">
+        <v>4205</v>
+      </c>
+      <c r="I659" s="2">
+        <v>53.87</v>
+      </c>
+      <c r="K659" s="4">
+        <f t="shared" si="15"/>
+        <v>5387</v>
+      </c>
+    </row>
+    <row r="660" spans="1:11">
+      <c r="A660" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B660" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C660" t="s">
+        <v>10</v>
+      </c>
+      <c r="D660">
+        <v>-100</v>
+      </c>
+      <c r="E660" t="s">
+        <v>6</v>
+      </c>
+      <c r="F660" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G660" t="s">
+        <v>8</v>
+      </c>
+      <c r="H660" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I660" s="2">
+        <v>52.37</v>
+      </c>
+      <c r="K660" s="4">
+        <f t="shared" si="15"/>
+        <v>-5237</v>
+      </c>
+    </row>
+    <row r="662" spans="1:11">
+      <c r="A662" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B662" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C662" t="s">
+        <v>10</v>
+      </c>
+      <c r="D662">
+        <v>-100</v>
+      </c>
+      <c r="E662" t="s">
+        <v>6</v>
+      </c>
+      <c r="F662" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G662" t="s">
+        <v>8</v>
+      </c>
+      <c r="H662" s="3">
+        <v>4205</v>
+      </c>
+      <c r="I662" s="2">
+        <v>43.28</v>
+      </c>
+      <c r="K662" s="4">
+        <f t="shared" si="15"/>
+        <v>-4328</v>
+      </c>
+    </row>
+    <row r="663" spans="1:11">
+      <c r="A663" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B663" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C663" t="s">
+        <v>4</v>
+      </c>
+      <c r="D663">
+        <v>100</v>
+      </c>
+      <c r="E663" t="s">
+        <v>6</v>
+      </c>
+      <c r="F663" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G663" t="s">
+        <v>8</v>
+      </c>
+      <c r="H663" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I663" s="2">
+        <v>41.88</v>
+      </c>
+      <c r="K663" s="4">
+        <f t="shared" si="15"/>
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="664" spans="1:11">
+      <c r="A664" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B664" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C664" t="s">
+        <v>10</v>
+      </c>
+      <c r="D664">
+        <v>-100</v>
+      </c>
+      <c r="E664" t="s">
+        <v>6</v>
+      </c>
+      <c r="F664" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G664" t="s">
+        <v>8</v>
+      </c>
+      <c r="H664" s="3">
+        <v>4205</v>
+      </c>
+      <c r="I664" s="2">
+        <v>43.28</v>
+      </c>
+      <c r="K664" s="4">
+        <f t="shared" si="15"/>
+        <v>-4328</v>
+      </c>
+    </row>
+    <row r="665" spans="1:11">
+      <c r="A665" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B665" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C665" t="s">
+        <v>4</v>
+      </c>
+      <c r="D665">
+        <v>100</v>
+      </c>
+      <c r="E665" t="s">
+        <v>6</v>
+      </c>
+      <c r="F665" s="1">
+        <v>44393</v>
+      </c>
+      <c r="G665" t="s">
+        <v>8</v>
+      </c>
+      <c r="H665" s="3">
+        <v>4200</v>
+      </c>
+      <c r="I665" s="2">
+        <v>41.88</v>
+      </c>
+      <c r="K665" s="4">
+        <f t="shared" si="15"/>
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="667" spans="1:11">
+      <c r="A667" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B667" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C667" t="s">
+        <v>4</v>
+      </c>
+      <c r="D667">
+        <v>100</v>
+      </c>
+      <c r="E667" t="s">
+        <v>36</v>
+      </c>
+      <c r="F667" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G667" t="s">
+        <v>23</v>
+      </c>
+      <c r="H667" s="3">
+        <v>2320</v>
+      </c>
+      <c r="I667" s="2">
+        <v>3.67</v>
+      </c>
+      <c r="K667" s="4">
+        <f t="shared" si="15"/>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="668" spans="1:11">
+      <c r="A668" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B668" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C668" t="s">
+        <v>10</v>
+      </c>
+      <c r="D668">
+        <v>-100</v>
+      </c>
+      <c r="E668" t="s">
+        <v>36</v>
+      </c>
+      <c r="F668" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G668" t="s">
+        <v>23</v>
+      </c>
+      <c r="H668" s="3">
+        <v>2325</v>
+      </c>
+      <c r="I668" s="2">
+        <v>3.02</v>
+      </c>
+      <c r="K668" s="4">
+        <f t="shared" si="15"/>
+        <v>-302</v>
+      </c>
+    </row>
+    <row r="670" spans="1:11">
+      <c r="A670" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B670" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C670" t="s">
+        <v>4</v>
+      </c>
+      <c r="D670">
+        <v>100</v>
+      </c>
+      <c r="E670" t="s">
+        <v>36</v>
+      </c>
+      <c r="F670" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G670" t="s">
+        <v>8</v>
+      </c>
+      <c r="H670" s="3">
+        <v>2235</v>
+      </c>
+      <c r="I670" s="2">
+        <v>6.84</v>
+      </c>
+      <c r="K670" s="4">
+        <f t="shared" si="15"/>
+        <v>684</v>
+      </c>
+    </row>
+    <row r="671" spans="1:11">
+      <c r="A671" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B671" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C671" t="s">
+        <v>10</v>
+      </c>
+      <c r="D671">
+        <v>-100</v>
+      </c>
+      <c r="E671" t="s">
+        <v>36</v>
+      </c>
+      <c r="F671" s="1">
+        <v>44372</v>
+      </c>
+      <c r="G671" t="s">
+        <v>8</v>
+      </c>
+      <c r="H671" s="3">
+        <v>2230</v>
+      </c>
+      <c r="I671" s="2">
+        <v>6.14</v>
+      </c>
+      <c r="K671" s="4">
+        <f t="shared" si="15"/>
+        <v>-614</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M3"/>
@@ -16467,11 +17157,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16486,7 +17176,7 @@
     <col min="10" max="10" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="13"/>
+    <col min="14" max="14" width="10.140625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -17022,23 +17712,161 @@
         <v>36</v>
       </c>
     </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B14" s="6">
+        <v>86578.97</v>
+      </c>
+      <c r="C14" s="13">
+        <v>376.95</v>
+      </c>
+      <c r="D14" s="13">
+        <v>495.76</v>
+      </c>
+      <c r="E14" s="5">
+        <v>352</v>
+      </c>
+      <c r="F14" s="5">
+        <v>118</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>76712.56</v>
+      </c>
+      <c r="I14" s="6">
+        <v>38356.28</v>
+      </c>
+      <c r="J14" s="13">
+        <v>50380.21</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6">
+        <v>47579.6</v>
+      </c>
+      <c r="N14" s="13">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B15" s="6">
+        <v>86962.35</v>
+      </c>
+      <c r="C15" s="13">
+        <v>760.33</v>
+      </c>
+      <c r="D15" s="13">
+        <v>879.14</v>
+      </c>
+      <c r="E15" s="5">
+        <v>270</v>
+      </c>
+      <c r="F15" s="5">
+        <v>124</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>77431.09</v>
+      </c>
+      <c r="I15" s="6">
+        <v>38715.550000000003</v>
+      </c>
+      <c r="J15" s="13">
+        <v>50380.21</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6">
+        <v>47579.6</v>
+      </c>
+      <c r="N15" s="13">
+        <v>6956</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1">
+        <v>44369</v>
+      </c>
+      <c r="B16" s="6">
+        <v>86962.35</v>
+      </c>
+      <c r="C16" s="13">
+        <v>-817.67</v>
+      </c>
+      <c r="D16" s="13">
+        <v>879.14</v>
+      </c>
+      <c r="E16" s="5">
+        <v>270</v>
+      </c>
+      <c r="F16" s="5">
+        <v>124</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>77429.09</v>
+      </c>
+      <c r="I16" s="6">
+        <v>38714.550000000003</v>
+      </c>
+      <c r="J16" s="13">
+        <v>50380.21</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>47579.6</v>
+      </c>
+      <c r="N16" s="13">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1">
+        <v>44370</v>
+      </c>
+    </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="18">
+      <c r="A18" s="1">
+        <v>44371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1">
+        <v>44372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18">
         <f>SUM(N2:N17)</f>
-        <v>9647</v>
+        <v>18724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 24-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trades" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -894,6 +894,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF37FF41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -908,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -928,6 +934,7 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -935,6 +942,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF37FF41"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1225,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O671"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A669" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A692" sqref="A692"/>
     </sheetView>
@@ -17159,17 +17171,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="11.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="6" bestFit="1" customWidth="1"/>
@@ -17344,7 +17355,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="1">
+      <c r="A5" s="19">
         <v>44354</v>
       </c>
       <c r="B5" s="6">
@@ -17385,7 +17396,7 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="1">
+      <c r="A6" s="19">
         <v>44355</v>
       </c>
       <c r="B6" s="6">
@@ -17426,7 +17437,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="1">
+      <c r="A7" s="19">
         <v>44356</v>
       </c>
       <c r="B7" s="6">
@@ -17467,7 +17478,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="1">
+      <c r="A8" s="19">
         <v>44357</v>
       </c>
       <c r="B8" s="6">
@@ -17508,7 +17519,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="1">
+      <c r="A9" s="19">
         <v>44358</v>
       </c>
       <c r="B9" s="6">
@@ -17754,7 +17765,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="1">
+      <c r="A15" s="19">
         <v>44368</v>
       </c>
       <c r="B15" s="6">
@@ -17795,7 +17806,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1">
+      <c r="A16" s="19">
         <v>44369</v>
       </c>
       <c r="B16" s="6">
@@ -17836,17 +17847,53 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="1">
+      <c r="A17" s="19">
         <v>44370</v>
       </c>
+      <c r="B17" s="6">
+        <v>87595.17</v>
+      </c>
+      <c r="C17" s="13">
+        <v>-101.87</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1521.27</v>
+      </c>
+      <c r="E17" s="5">
+        <v>256</v>
+      </c>
+      <c r="F17" s="5">
+        <v>183</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>72679.360000000001</v>
+      </c>
+      <c r="I17" s="6">
+        <v>36339.68</v>
+      </c>
+      <c r="J17" s="13">
+        <v>50846.9</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
+        <v>45839.38</v>
+      </c>
+      <c r="N17" s="13">
+        <v>896</v>
+      </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="1">
+      <c r="A18" s="19">
         <v>44371</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="1">
+      <c r="A19" s="19">
         <v>44372</v>
       </c>
     </row>
@@ -17866,7 +17913,7 @@
       <c r="M27" s="17"/>
       <c r="N27" s="18">
         <f>SUM(N2:N17)</f>
-        <v>18724</v>
+        <v>19620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 25-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17172,7 +17172,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -17891,6 +17891,42 @@
       <c r="A18" s="19">
         <v>44371</v>
       </c>
+      <c r="B18" s="6">
+        <v>87988.43</v>
+      </c>
+      <c r="C18" s="13">
+        <v>87</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1923.33</v>
+      </c>
+      <c r="E18" s="5">
+        <v>311</v>
+      </c>
+      <c r="F18" s="5">
+        <v>66</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>75865.81</v>
+      </c>
+      <c r="I18" s="6">
+        <v>37932.910000000003</v>
+      </c>
+      <c r="J18" s="13">
+        <v>50174.1</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6">
+        <v>47811.38</v>
+      </c>
+      <c r="N18" s="13">
+        <v>-652</v>
+      </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="19">
@@ -17912,8 +17948,8 @@
       <c r="L27" s="15"/>
       <c r="M27" s="17"/>
       <c r="N27" s="18">
-        <f>SUM(N2:N17)</f>
-        <v>19620</v>
+        <f>SUM(N2:N18)</f>
+        <v>18968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 26-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17173,7 +17173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17932,6 +17932,39 @@
       <c r="A19" s="19">
         <v>44372</v>
       </c>
+      <c r="B19" s="6">
+        <v>88599.86</v>
+      </c>
+      <c r="C19" s="13">
+        <v>-146.41999999999999</v>
+      </c>
+      <c r="D19" s="13">
+        <v>2539.91</v>
+      </c>
+      <c r="E19" s="5">
+        <v>482</v>
+      </c>
+      <c r="F19" s="5">
+        <v>69</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>62569.3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>31284.65</v>
+      </c>
+      <c r="J19" s="13">
+        <v>51678.95</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
+        <v>47811.38</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="14"/>

</xml_diff>

<commit_message>
Update 29-Jun-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17169,11 +17169,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17965,24 +17965,88 @@
       <c r="L19" s="6">
         <v>47811.38</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="18">
-        <f>SUM(N2:N18)</f>
-        <v>18968</v>
+      <c r="N19" s="13">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B20" s="6">
+        <v>89246.09</v>
+      </c>
+      <c r="C20" s="13">
+        <v>74</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3196.94</v>
+      </c>
+      <c r="E20" s="5">
+        <v>482</v>
+      </c>
+      <c r="F20" s="5">
+        <v>76</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>63006.82</v>
+      </c>
+      <c r="I20" s="6">
+        <v>31503.41</v>
+      </c>
+      <c r="J20" s="13">
+        <v>51431.15</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6">
+        <v>41359.019999999997</v>
+      </c>
+      <c r="N20" s="13">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>44376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1">
+        <v>44379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="18">
+        <f>SUM(N2:N30)</f>
+        <v>20284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 30-Jun-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17173,7 +17173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18014,6 +18014,42 @@
       <c r="A21" s="1">
         <v>44376</v>
       </c>
+      <c r="B21" s="6">
+        <v>89112.82</v>
+      </c>
+      <c r="C21" s="13">
+        <v>-654.05999999999995</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3074.87</v>
+      </c>
+      <c r="E21" s="5">
+        <v>544</v>
+      </c>
+      <c r="F21" s="5">
+        <v>71</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>62064.75</v>
+      </c>
+      <c r="I21" s="6">
+        <v>31032.38</v>
+      </c>
+      <c r="J21" s="13">
+        <v>51265.94</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <v>41392.019999999997</v>
+      </c>
+      <c r="N21" s="13">
+        <v>1508</v>
+      </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="1">
@@ -18046,7 +18082,7 @@
       <c r="M31" s="17"/>
       <c r="N31" s="18">
         <f>SUM(N2:N30)</f>
-        <v>20284</v>
+        <v>21792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17173,7 +17173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18055,6 +18055,42 @@
       <c r="A22" s="1">
         <v>44377</v>
       </c>
+      <c r="B22" s="6">
+        <v>89943.39</v>
+      </c>
+      <c r="C22" s="13">
+        <v>169</v>
+      </c>
+      <c r="D22" s="13">
+        <v>3898.99</v>
+      </c>
+      <c r="E22" s="5">
+        <v>470</v>
+      </c>
+      <c r="F22" s="5">
+        <v>84</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <v>63222.9</v>
+      </c>
+      <c r="I22" s="6">
+        <v>31611.45</v>
+      </c>
+      <c r="J22" s="13">
+        <v>51463.63</v>
+      </c>
+      <c r="K22" s="6">
+        <v>0</v>
+      </c>
+      <c r="L22" s="6">
+        <v>40950.699999999997</v>
+      </c>
+      <c r="N22" s="13">
+        <v>183</v>
+      </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="1">
@@ -18082,7 +18118,7 @@
       <c r="M31" s="17"/>
       <c r="N31" s="18">
         <f>SUM(N2:N30)</f>
-        <v>21792</v>
+        <v>21975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 3-Jul-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17169,11 +17169,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18096,29 +18096,126 @@
       <c r="A23" s="1">
         <v>44378</v>
       </c>
+      <c r="B23" s="6">
+        <v>90180.98</v>
+      </c>
+      <c r="C23" s="13">
+        <v>267.99</v>
+      </c>
+      <c r="D23" s="13">
+        <v>4151.97</v>
+      </c>
+      <c r="E23" s="5">
+        <v>402</v>
+      </c>
+      <c r="F23" s="5">
+        <v>88</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6">
+        <v>63286.35</v>
+      </c>
+      <c r="I23" s="6">
+        <v>31643.17</v>
+      </c>
+      <c r="J23" s="13">
+        <v>50577.97</v>
+      </c>
+      <c r="K23" s="6">
+        <v>0</v>
+      </c>
+      <c r="L23" s="6">
+        <v>40950.699999999997</v>
+      </c>
+      <c r="N23" s="13">
+        <v>905</v>
+      </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>44379</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="18">
-        <f>SUM(N2:N30)</f>
-        <v>21975</v>
+      <c r="B24" s="6">
+        <v>91549.81</v>
+      </c>
+      <c r="C24" s="13">
+        <v>130.84</v>
+      </c>
+      <c r="D24" s="13">
+        <v>5531.03</v>
+      </c>
+      <c r="E24" s="5">
+        <v>297</v>
+      </c>
+      <c r="F24" s="5">
+        <v>90</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>64124.14</v>
+      </c>
+      <c r="I24" s="6">
+        <v>32062.07</v>
+      </c>
+      <c r="J24" s="13">
+        <v>50243.72</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
+        <v>41508.54</v>
+      </c>
+      <c r="N24" s="13">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="19">
+        <v>44382</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="19">
+        <v>44383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="19">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="19">
+        <v>44385</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="19">
+        <v>44386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="18">
+        <f>SUM(N2:N36)</f>
+        <v>24068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 5-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17172,8 +17172,8 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18141,13 +18141,13 @@
         <v>91549.81</v>
       </c>
       <c r="C24" s="13">
-        <v>130.84</v>
+        <v>40</v>
       </c>
       <c r="D24" s="13">
         <v>5531.03</v>
       </c>
       <c r="E24" s="5">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F24" s="5">
         <v>90</v>
@@ -18156,19 +18156,19 @@
         <v>0</v>
       </c>
       <c r="H24" s="6">
-        <v>64124.14</v>
+        <v>64124</v>
       </c>
       <c r="I24" s="6">
-        <v>32062.07</v>
+        <v>32062</v>
       </c>
       <c r="J24" s="13">
-        <v>50243.72</v>
+        <v>50243.65</v>
       </c>
       <c r="K24" s="6">
         <v>0</v>
       </c>
       <c r="L24" s="6">
-        <v>41508.54</v>
+        <v>41738</v>
       </c>
       <c r="N24" s="13">
         <v>1188</v>

</xml_diff>

<commit_message>
Update 8-Jul-2021, midday update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="274">
   <si>
     <t>Date</t>
   </si>
@@ -838,6 +838,9 @@
   </si>
   <si>
     <t>1568-42473</t>
+  </si>
+  <si>
+    <t>Market closed</t>
   </si>
 </sst>
 </file>
@@ -17169,11 +17172,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17846,7 +17849,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="19">
         <v>44370</v>
       </c>
@@ -17887,7 +17890,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="19">
         <v>44371</v>
       </c>
@@ -17928,7 +17931,7 @@
         <v>-652</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" s="19">
         <v>44372</v>
       </c>
@@ -17969,7 +17972,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" s="1">
         <v>44375</v>
       </c>
@@ -18010,7 +18013,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="1">
         <v>44376</v>
       </c>
@@ -18051,7 +18054,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="1">
         <v>44377</v>
       </c>
@@ -18092,7 +18095,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" s="1">
         <v>44378</v>
       </c>
@@ -18133,7 +18136,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" s="1">
         <v>44379</v>
       </c>
@@ -18174,27 +18177,102 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="19">
         <v>44382</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="19">
         <v>44383</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="B26" s="6">
+        <v>91549.81</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13">
+        <v>5531.03</v>
+      </c>
+      <c r="E26" s="5">
+        <v>296</v>
+      </c>
+      <c r="F26" s="5">
+        <v>90</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6">
+        <v>64124</v>
+      </c>
+      <c r="I26" s="6">
+        <v>32062</v>
+      </c>
+      <c r="J26" s="13">
+        <v>50243.65</v>
+      </c>
+      <c r="K26" s="6">
+        <v>0</v>
+      </c>
+      <c r="L26" s="6">
+        <v>41738</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="19">
         <v>44384</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="B27" s="6">
+        <v>89838</v>
+      </c>
+      <c r="C27" s="13">
+        <v>-2160.67</v>
+      </c>
+      <c r="D27" s="13">
+        <v>3831.69</v>
+      </c>
+      <c r="E27" s="5">
+        <v>500</v>
+      </c>
+      <c r="F27" s="5">
+        <v>169</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6">
+        <v>59016.88</v>
+      </c>
+      <c r="I27" s="6">
+        <v>29508.44</v>
+      </c>
+      <c r="J27" s="13">
+        <v>50975.87</v>
+      </c>
+      <c r="K27" s="6">
+        <v>0</v>
+      </c>
+      <c r="L27" s="6">
+        <v>41954.8</v>
+      </c>
+      <c r="N27" s="13">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="19">
         <v>44385</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" s="19">
         <v>44386</v>
       </c>
@@ -18215,7 +18293,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="18">
         <f>SUM(N2:N36)</f>
-        <v>24068</v>
+        <v>25339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 10-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17176,7 +17176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18271,6 +18271,42 @@
       <c r="A28" s="19">
         <v>44385</v>
       </c>
+      <c r="B28" s="6">
+        <v>89821.35</v>
+      </c>
+      <c r="C28" s="13">
+        <v>-1828.27</v>
+      </c>
+      <c r="D28" s="13">
+        <v>3814.42</v>
+      </c>
+      <c r="E28" s="5">
+        <v>499</v>
+      </c>
+      <c r="F28" s="5">
+        <v>196</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6">
+        <v>57914.41</v>
+      </c>
+      <c r="I28" s="6">
+        <v>28957.21</v>
+      </c>
+      <c r="J28" s="13">
+        <v>50975.87</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+      <c r="L28" s="6">
+        <v>39175.65</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="19">

</xml_diff>

<commit_message>
Update 13 Jul 2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17176,7 +17176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18353,6 +18353,42 @@
       <c r="A30" s="1">
         <v>44389</v>
       </c>
+      <c r="B30" s="6">
+        <v>93162.44</v>
+      </c>
+      <c r="C30" s="13">
+        <v>135</v>
+      </c>
+      <c r="D30" s="13">
+        <v>7170.61</v>
+      </c>
+      <c r="E30" s="5">
+        <v>270</v>
+      </c>
+      <c r="F30" s="5">
+        <v>196</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>42067.39</v>
+      </c>
+      <c r="I30" s="6">
+        <v>21033.69</v>
+      </c>
+      <c r="J30" s="6">
+        <v>51608.17</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6">
+        <v>30851.39</v>
+      </c>
+      <c r="N30" s="13">
+        <v>1727</v>
+      </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="1">
@@ -18390,7 +18426,7 @@
       <c r="M39" s="17"/>
       <c r="N39" s="18">
         <f>SUM(N2:N38)</f>
-        <v>25509</v>
+        <v>27236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 16-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/Tastyworks Trading.xlsx
+++ b/Tastyworks Trading.xlsx
@@ -17176,7 +17176,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18476,6 +18476,42 @@
       <c r="A33" s="1">
         <v>44392</v>
       </c>
+      <c r="B33" s="6">
+        <v>92153.600000000006</v>
+      </c>
+      <c r="C33" s="13">
+        <v>-219.13</v>
+      </c>
+      <c r="D33" s="13">
+        <v>6191.6</v>
+      </c>
+      <c r="E33" s="5">
+        <v>110</v>
+      </c>
+      <c r="F33" s="5">
+        <v>48</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6">
+        <v>114540.07</v>
+      </c>
+      <c r="I33" s="6">
+        <v>52270.04</v>
+      </c>
+      <c r="J33" s="13">
+        <v>50594.45</v>
+      </c>
+      <c r="K33" s="6">
+        <v>0</v>
+      </c>
+      <c r="L33" s="6">
+        <v>67041.3</v>
+      </c>
+      <c r="N33" s="13">
+        <v>-13058</v>
+      </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="1">
@@ -18498,7 +18534,7 @@
       <c r="M39" s="17"/>
       <c r="N39" s="18">
         <f>SUM(N2:N38)</f>
-        <v>27355</v>
+        <v>14297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>